<commit_message>
add results for Genetic Algo for population 40 and 400
</commit_message>
<xml_diff>
--- a/results_from_all_algos.xlsx
+++ b/results_from_all_algos.xlsx
@@ -5,14 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="WOA_CONV" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="WOA_RESULTS" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="GA" sheetId="3" state="visible" r:id="rId5"/>
-    <sheet name="SA" sheetId="4" state="visible" r:id="rId6"/>
-    <sheet name="CSA" sheetId="5" state="visible" r:id="rId7"/>
+    <sheet name="WOA_CONV" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="WOA_RESULTS" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="GA" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="SA" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="CSA" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="143">
   <si>
     <t xml:space="preserve">ITER#</t>
   </si>
@@ -448,6 +448,12 @@
   <si>
     <t xml:space="preserve">Time</t>
   </si>
+  <si>
+    <t xml:space="preserve">Population 40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Population 400</t>
+  </si>
 </sst>
 </file>
 
@@ -557,128 +563,22 @@
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
-  <a:themeElements>
-    <a:clrScheme name="LibreOffice">
-      <a:dk1>
-        <a:srgbClr val="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:srgbClr val="ffffff"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="000000"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="ffffff"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="18a303"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="0369a3"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="a33e03"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8e03a3"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="c99c00"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="c9211e"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000ee"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="551a8b"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme>
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:CW132"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="Y84" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="Y2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="Y1" activeCellId="0" sqref="Y1"/>
-      <selection pane="bottomLeft" activeCell="A84" activeCellId="0" sqref="A84"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
       <selection pane="bottomRight" activeCell="B102" activeCellId="0" sqref="B102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="6.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.77"/>
   </cols>
@@ -25026,23 +24926,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AC32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="N1" activeCellId="0" sqref="N1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Y3" activeCellId="0" sqref="Y3"/>
+      <selection pane="bottomRight" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="6.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="10.66"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27368,18 +27268,1205 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K12" activeCellId="0" sqref="K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="6.15625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>10.7238724226071</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>0.665894571203777</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>0.0567502524855161</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>2.02966883627781</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>9.52999999999884</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>4.8560721953008</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>0.493153851655819</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>0.0132803310206709</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>2.01846792074959</v>
+      </c>
+      <c r="M3" s="0" t="n">
+        <v>27.7199999999975</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>8.2311927603102</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>0.583075888706101</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>0.0310018093126386</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>2.03729585389696</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>5.41313325442353</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>0.464554466776339</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>0.00665539117373578</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>2.03274443888134</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <v>26.760000000002</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>8.36573141875861</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>0.59051913310922</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>0.0427982170087977</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>2.01630784636292</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>8.27999999999884</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>4.75882657268915</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>0.485544667763393</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>0.010994275659824</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>2.02246143575805</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <v>27.6999999999971</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>9.78204287810597</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>0.655016379372005</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>0.0376393250840426</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>2.03302577307298</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>8.40000000000146</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>6.72519994526819</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>0.585558114584079</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>0.0330848397110364</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <v>2.0187444865651</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <v>26.5800000000017</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>4.80704998386385</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>0.478124883770832</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>0.0106567264144196</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>2.0197863767494</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>7.86000000000058</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>5.58490329535578</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>0.525620198841285</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>0.0226525387311351</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <v>2.01846076818539</v>
+      </c>
+      <c r="M7" s="0" t="n">
+        <v>26.5300000000025</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>4.89230681519811</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>0.468101566411559</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>0.00878234203561977</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>2.02026798273848</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>7.77999999999884</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>4.87347665134813</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>0.481825334382376</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>0.00955719047278449</v>
+      </c>
+      <c r="L8" s="0" t="n">
+        <v>2.02315046610877</v>
+      </c>
+      <c r="M8" s="0" t="n">
+        <v>27.6800000000003</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>6.13068742880313</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>0.481228524426007</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>0.0066976920105858</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>2.02249481439096</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>7.5099999999984</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>5.39477395868778</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>0.504275802875331</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>0.0176461775266433</v>
+      </c>
+      <c r="L9" s="0" t="n">
+        <v>2.01393557923849</v>
+      </c>
+      <c r="M9" s="0" t="n">
+        <v>27.4499999999971</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>8.52891610209896</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>0.542214719977112</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>0.0100502238752593</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>2.02697470376463</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>7.59000000000015</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>5.65706427499715</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>0.509580716686932</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>0.018491432086403</v>
+      </c>
+      <c r="L10" s="0" t="n">
+        <v>2.01132966168371</v>
+      </c>
+      <c r="M10" s="0" t="n">
+        <v>27.1500000000015</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>8.11085953040049</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>0.557195050425578</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>0.0349911402617839</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>2.00799179839306</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>7.72999999999956</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>5.34136807201857</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>0.489899721049996</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <v>0.0152641831056434</v>
+      </c>
+      <c r="L11" s="0" t="n">
+        <v>2.01600743866676</v>
+      </c>
+      <c r="M11" s="0" t="n">
+        <v>27.1899999999987</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>5.56137912700172</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>0.530211572848866</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>0.0203606717688291</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>2.02881291276256</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>7.38999999999942</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>5.20746906269837</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>0.482855875831486</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <v>0.012593990415564</v>
+      </c>
+      <c r="L12" s="0" t="n">
+        <v>2.01402141000882</v>
+      </c>
+      <c r="M12" s="0" t="n">
+        <v>27.4500000000007</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>6.87240674308172</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>0.458079393462556</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>0.00495278249052285</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>2.04170183344062</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>7.90999999999985</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>5.17219153416732</v>
+      </c>
+      <c r="J13" s="0" t="n">
+        <v>0.478774336599671</v>
+      </c>
+      <c r="K13" s="0" t="n">
+        <v>0.00811038752592804</v>
+      </c>
+      <c r="L13" s="0" t="n">
+        <v>2.02871277686384</v>
+      </c>
+      <c r="M13" s="0" t="n">
+        <v>27.8500000000022</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>11.7992521716872</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>0.742606680494958</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>0.0669209361276018</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>2.02163889087571</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>7.38000000000102</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <v>4.74913733488581</v>
+      </c>
+      <c r="J14" s="0" t="n">
+        <v>0.481101494885917</v>
+      </c>
+      <c r="K14" s="0" t="n">
+        <v>0.0109079590873328</v>
+      </c>
+      <c r="L14" s="0" t="n">
+        <v>2.02147199771118</v>
+      </c>
+      <c r="M14" s="0" t="n">
+        <v>27.1899999999987</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>7.32066712827672</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>0.444751019240398</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>0.0059189374150633</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>2.033173592733</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>7.52000000000044</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <v>5.84214788558607</v>
+      </c>
+      <c r="J15" s="0" t="n">
+        <v>0.467430941992704</v>
+      </c>
+      <c r="K15" s="0" t="n">
+        <v>0.00603907560260353</v>
+      </c>
+      <c r="L15" s="0" t="n">
+        <v>2.01889469041318</v>
+      </c>
+      <c r="M15" s="0" t="n">
+        <v>27.2999999999993</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>10.303163183044</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>0.591743079894142</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>0.0484002197267721</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>2.00957728345612</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>7.32999999999811</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="I16" s="0" t="n">
+        <v>5.63001930715198</v>
+      </c>
+      <c r="J16" s="0" t="n">
+        <v>0.481380158786925</v>
+      </c>
+      <c r="K16" s="0" t="n">
+        <v>0.0141504516129032</v>
+      </c>
+      <c r="L16" s="0" t="n">
+        <v>2.01625062584937</v>
+      </c>
+      <c r="M16" s="0" t="n">
+        <v>27.1599999999999</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>5.82043858044748</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>0.554273371003505</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>0.0240800014305128</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>2.02505304818444</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>7.2400000000016</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <v>5.92498850484905</v>
+      </c>
+      <c r="J17" s="0" t="n">
+        <v>0.512333023388885</v>
+      </c>
+      <c r="K17" s="0" t="n">
+        <v>0.0214518237608183</v>
+      </c>
+      <c r="L17" s="0" t="n">
+        <v>2.01946927973679</v>
+      </c>
+      <c r="M17" s="0" t="n">
+        <v>26.4099999999999</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>5.57819031029712</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>0.457154709963522</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>0.00486484629139547</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>2.02957585294328</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>7.93999999999869</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="I18" s="0" t="n">
+        <v>5.91997515362382</v>
+      </c>
+      <c r="J18" s="0" t="n">
+        <v>0.506364351620056</v>
+      </c>
+      <c r="K18" s="0" t="n">
+        <v>0.01716934039053</v>
+      </c>
+      <c r="L18" s="0" t="n">
+        <v>2.03278973845457</v>
+      </c>
+      <c r="M18" s="0" t="n">
+        <v>27.3400000000001</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>11.1292238715918</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>0.699761104355912</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>0.0522674117731207</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>2.01029015568748</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>7.31999999999971</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="I19" s="0" t="n">
+        <v>4.94705089616361</v>
+      </c>
+      <c r="J19" s="0" t="n">
+        <v>0.471418067377155</v>
+      </c>
+      <c r="K19" s="0" t="n">
+        <v>0.00932444059795437</v>
+      </c>
+      <c r="L19" s="0" t="n">
+        <v>2.01801969339342</v>
+      </c>
+      <c r="M19" s="0" t="n">
+        <v>26.8899999999994</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>6.48093602028307</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>0.549965238538016</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>0.0259950670195265</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>2.00992299072551</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>7.20000000000073</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="I20" s="0" t="n">
+        <v>5.55062117506604</v>
+      </c>
+      <c r="J20" s="0" t="n">
+        <v>0.509136113296617</v>
+      </c>
+      <c r="K20" s="0" t="n">
+        <v>0.0121014333738645</v>
+      </c>
+      <c r="L20" s="0" t="n">
+        <v>2.02112152206566</v>
+      </c>
+      <c r="M20" s="0" t="n">
+        <v>27.2700000000004</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>5.43061488776379</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>0.502813246548888</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>0.017604829411344</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>2.01393557923849</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>7.27000000000044</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="I21" s="0" t="n">
+        <v>5.07601479750456</v>
+      </c>
+      <c r="J21" s="0" t="n">
+        <v>0.463810600100136</v>
+      </c>
+      <c r="K21" s="0" t="n">
+        <v>0.00668835533938917</v>
+      </c>
+      <c r="L21" s="0" t="n">
+        <v>2.02729180077725</v>
+      </c>
+      <c r="M21" s="0" t="n">
+        <v>26.7100000000028</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>6.0669214375464</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>0.545446534582648</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>0.0273788950718833</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>2.01765729680757</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <v>7.15999999999985</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I22" s="0" t="n">
+        <v>5.25282752318205</v>
+      </c>
+      <c r="J22" s="0" t="n">
+        <v>0.529186753451112</v>
+      </c>
+      <c r="K22" s="0" t="n">
+        <v>0.0205898013017667</v>
+      </c>
+      <c r="L22" s="0" t="n">
+        <v>2.02237560498772</v>
+      </c>
+      <c r="M22" s="0" t="n">
+        <v>26.8399999999965</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>8.19438921721926</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>0.562394106287104</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>0.0303041313210786</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>2.00201940729085</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>8.45999999999913</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="I23" s="0" t="n">
+        <v>5.13546827101928</v>
+      </c>
+      <c r="J23" s="0" t="n">
+        <v>0.474263643516201</v>
+      </c>
+      <c r="K23" s="0" t="n">
+        <v>0.00828292539875545</v>
+      </c>
+      <c r="L23" s="0" t="n">
+        <v>2.01897336861932</v>
+      </c>
+      <c r="M23" s="0" t="n">
+        <v>28.9600000000028</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>7.19229193143501</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>0.572517559545097</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>0.0322256754166369</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>2.00907660396252</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <v>7.22999999999956</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="I24" s="0" t="n">
+        <v>5.18453281165338</v>
+      </c>
+      <c r="J24" s="0" t="n">
+        <v>0.518758887061011</v>
+      </c>
+      <c r="K24" s="0" t="n">
+        <v>0.0152832375366569</v>
+      </c>
+      <c r="L24" s="0" t="n">
+        <v>2.02434017595308</v>
+      </c>
+      <c r="M24" s="0" t="n">
+        <v>27.1800000000003</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>10.2943713892955</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>0.584805092625707</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>0.0134891675845791</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>2.02583983024581</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <v>7.10000000000218</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="I25" s="0" t="n">
+        <v>5.33450276955544</v>
+      </c>
+      <c r="J25" s="0" t="n">
+        <v>0.497936914383807</v>
+      </c>
+      <c r="K25" s="0" t="n">
+        <v>0.0153470698805522</v>
+      </c>
+      <c r="L25" s="0" t="n">
+        <v>2.01282216341225</v>
+      </c>
+      <c r="M25" s="0" t="n">
+        <v>23.1299999999974</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>8.0847582994177</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>0.63206294256491</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>0.040670313425363</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>2.02027751949074</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <v>7.18999999999869</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="I26" s="0" t="n">
+        <v>5.33190538595603</v>
+      </c>
+      <c r="J26" s="0" t="n">
+        <v>0.514771761676561</v>
+      </c>
+      <c r="K26" s="0" t="n">
+        <v>0.0145525001072885</v>
+      </c>
+      <c r="L26" s="0" t="n">
+        <v>2.01896621605512</v>
+      </c>
+      <c r="M26" s="0" t="n">
+        <v>23.0699999999997</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>7.70890806029643</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>0.579850940562192</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>0.0316555668407124</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>2.03396752735856</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>6.90000000000146</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="I27" s="0" t="n">
+        <v>5.48988153152741</v>
+      </c>
+      <c r="J27" s="0" t="n">
+        <v>0.464500679493599</v>
+      </c>
+      <c r="K27" s="0" t="n">
+        <v>0.00646818138902797</v>
+      </c>
+      <c r="L27" s="0" t="n">
+        <v>2.01804830365019</v>
+      </c>
+      <c r="M27" s="0" t="n">
+        <v>22.5300000000025</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>7.70479994703415</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>0.553680566483084</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>0.0143528096702668</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>2.03468039958992</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <v>6.90999999999985</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="I28" s="0" t="n">
+        <v>5.50037317551044</v>
+      </c>
+      <c r="J28" s="0" t="n">
+        <v>0.515874973177884</v>
+      </c>
+      <c r="K28" s="0" t="n">
+        <v>0.020746714541163</v>
+      </c>
+      <c r="L28" s="0" t="n">
+        <v>2.02114774813437</v>
+      </c>
+      <c r="M28" s="0" t="n">
+        <v>22.3999999999978</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>9.58705445864311</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>0.592194549746084</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>0.0384659063014091</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <v>1.99944209999285</v>
+      </c>
+      <c r="F29" s="0" t="n">
+        <v>6.88999999999942</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I29" s="0" t="n">
+        <v>6.03519906331861</v>
+      </c>
+      <c r="J29" s="0" t="n">
+        <v>0.501632215149131</v>
+      </c>
+      <c r="K29" s="0" t="n">
+        <v>0.0185382107145412</v>
+      </c>
+      <c r="L29" s="0" t="n">
+        <v>2.02676966359106</v>
+      </c>
+      <c r="M29" s="0" t="n">
+        <v>23.5699999999997</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>5.56395603205606</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>0.504508690365496</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>0.017885405908018</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <v>2.01233817323511</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <v>7.06999999999971</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="I30" s="0" t="n">
+        <v>6.14080119964072</v>
+      </c>
+      <c r="J30" s="0" t="n">
+        <v>0.55536227737644</v>
+      </c>
+      <c r="K30" s="0" t="n">
+        <v>0.0287466221300336</v>
+      </c>
+      <c r="L30" s="0" t="n">
+        <v>2.0191235724674</v>
+      </c>
+      <c r="M30" s="0" t="n">
+        <v>23.6500000000015</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>7.62771539518925</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>0.594727701881124</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>0.024662304842286</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <v>2.0287628448132</v>
+      </c>
+      <c r="F31" s="0" t="n">
+        <v>7.06000000000131</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="I31" s="0" t="n">
+        <v>6.39310458902364</v>
+      </c>
+      <c r="J31" s="0" t="n">
+        <v>0.557446820685216</v>
+      </c>
+      <c r="K31" s="0" t="n">
+        <v>0.0193043893855947</v>
+      </c>
+      <c r="L31" s="0" t="n">
+        <v>2.02748015163436</v>
+      </c>
+      <c r="M31" s="0" t="n">
+        <v>23.7200000000012</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>5.55863921208211</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>0.517846792074959</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>0.0144019701022817</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <v>2.01854421476766</v>
+      </c>
+      <c r="F32" s="0" t="n">
+        <v>7.22999999999956</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="I32" s="0" t="n">
+        <v>5.44866067470833</v>
+      </c>
+      <c r="J32" s="0" t="n">
+        <v>0.497357270581504</v>
+      </c>
+      <c r="K32" s="0" t="n">
+        <v>0.0161116289249696</v>
+      </c>
+      <c r="L32" s="0" t="n">
+        <v>2.02766611830341</v>
+      </c>
+      <c r="M32" s="0" t="n">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -27391,526 +28478,683 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:AC32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="n">
-        <v>6.93028632450325</v>
-      </c>
-      <c r="B1" s="2" t="n">
-        <v>0.524859554787541</v>
-      </c>
-      <c r="C1" s="2" t="n">
-        <v>0.0289444141627922</v>
-      </c>
-      <c r="D1" s="2" t="n">
-        <v>2.01543621076715</v>
-      </c>
-      <c r="E1" s="2" t="n">
-        <v>268.29</v>
+    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="n">
-        <v>7.12145951023274</v>
+      <c r="A2" s="1" t="s">
+        <v>101</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.546171004730499</v>
+        <v>6.93028632450325</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>0.0319548169907672</v>
+        <v>0.524859554787541</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>2.01076862756348</v>
+        <v>0.0289444141627922</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>383.48</v>
+        <v>2.01543621076715</v>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>268.29</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="n">
-        <v>8.06585750737078</v>
+      <c r="A3" s="1" t="s">
+        <v>103</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>0.584556993835105</v>
+        <v>7.12145951023274</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>0.0440314894255499</v>
+        <v>0.546171004730499</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>2.01371873141363</v>
+        <v>0.0319548169907672</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>276.33</v>
+        <v>2.01076862756348</v>
+      </c>
+      <c r="F3" s="2" t="n">
+        <v>383.48</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="n">
-        <v>6.13686366876309</v>
+      <c r="A4" s="1" t="s">
+        <v>104</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>0.488253836088191</v>
+        <v>8.06585750737078</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>0.0189523996697701</v>
+        <v>0.584556993835105</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>2.01361917597072</v>
+        <v>0.0440314894255499</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>336.56</v>
+        <v>2.01371873141363</v>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>276.33</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="n">
-        <v>7.01200286082769</v>
+      <c r="A5" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>0.532498716372549</v>
+        <v>6.13686366876309</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>0.0301691284947793</v>
+        <v>0.488253836088191</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>2.01607813154779</v>
+        <v>0.0189523996697701</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>331.54</v>
+        <v>2.01361917597072</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>336.56</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="n">
-        <v>6.13923710658133</v>
+      <c r="A6" s="1" t="s">
+        <v>106</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>0.473252886835473</v>
+        <v>7.01200286082769</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>0.0151266721448187</v>
+        <v>0.532498716372549</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>2.0162567894857</v>
+        <v>0.0301691284947793</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>269.35</v>
+        <v>2.01607813154779</v>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>331.54</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="n">
-        <v>8.36563289055019</v>
+      <c r="A7" s="1" t="s">
+        <v>107</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>0.598373817612299</v>
+        <v>6.13923710658133</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>0.0471818294780156</v>
+        <v>0.473252886835473</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>2.01405121829215</v>
+        <v>0.0151266721448187</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>282.77</v>
+        <v>2.0162567894857</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>269.35</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="n">
-        <v>11.0317934017224</v>
+      <c r="A8" s="1" t="s">
+        <v>108</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>0.5</v>
+        <v>8.36563289055019</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>0.03</v>
+        <v>0.598373817612299</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>2</v>
+        <v>0.0471818294780156</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>232.46</v>
+        <v>2.01405121829215</v>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>282.77</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="n">
-        <v>6.35839907625018</v>
+      <c r="A9" s="1" t="s">
+        <v>109</v>
       </c>
       <c r="B9" s="2" t="n">
-        <v>0.480848385910513</v>
+        <v>11.0317934017224</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>0.0159647606559745</v>
+        <v>0.5</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>2.01772698056421</v>
+        <v>0.03</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>435.619999999999</v>
+        <v>2</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>232.46</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="n">
-        <v>6.64601194394861</v>
+      <c r="A10" s="1" t="s">
+        <v>110</v>
       </c>
       <c r="B10" s="2" t="n">
-        <v>0.518332659762903</v>
+        <v>6.35839907625018</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>0.0268100209948945</v>
+        <v>0.480848385910513</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>2.01419803427063</v>
+        <v>0.0159647606559745</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>528.96</v>
+        <v>2.01772698056421</v>
+      </c>
+      <c r="F10" s="2" t="n">
+        <v>435.619999999999</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="n">
-        <v>10.7570517164249</v>
+      <c r="A11" s="1" t="s">
+        <v>111</v>
       </c>
       <c r="B11" s="2" t="n">
-        <v>0.511745157023533</v>
+        <v>6.64601194394861</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>0.0327405366388244</v>
+        <v>0.518332659762903</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>1.99459539159636</v>
+        <v>0.0268100209948945</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>324.97</v>
+        <v>2.01419803427063</v>
+      </c>
+      <c r="F11" s="2" t="n">
+        <v>528.96</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="n">
-        <v>9.62101798446815</v>
+      <c r="A12" s="1" t="s">
+        <v>112</v>
       </c>
       <c r="B12" s="2" t="n">
-        <v>0.6459200128464</v>
+        <v>10.7570517164249</v>
       </c>
       <c r="C12" s="2" t="n">
-        <v>0.0645946950589519</v>
+        <v>0.511745157023533</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>2.0111643680606</v>
+        <v>0.0327405366388244</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>385.21</v>
+        <v>1.99459539159636</v>
+      </c>
+      <c r="F12" s="2" t="n">
+        <v>324.97</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="n">
-        <v>6.89052685064197</v>
+      <c r="A13" s="1" t="s">
+        <v>113</v>
       </c>
       <c r="B13" s="2" t="n">
-        <v>0.535147844947261</v>
+        <v>9.62101798446815</v>
       </c>
       <c r="C13" s="2" t="n">
-        <v>0.0310224593277019</v>
+        <v>0.6459200128464</v>
       </c>
       <c r="D13" s="2" t="n">
-        <v>2.01455193720292</v>
+        <v>0.0645946950589519</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>584.91</v>
+        <v>2.0111643680606</v>
+      </c>
+      <c r="F13" s="2" t="n">
+        <v>385.21</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="n">
-        <v>7.32125720900175</v>
+      <c r="A14" s="1" t="s">
+        <v>114</v>
       </c>
       <c r="B14" s="2" t="n">
-        <v>0.557150517356331</v>
+        <v>6.89052685064197</v>
       </c>
       <c r="C14" s="2" t="n">
-        <v>0.0385399551307968</v>
+        <v>0.535147844947261</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>2.01113203569632</v>
+        <v>0.0310224593277019</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>431.780000000001</v>
+        <v>2.01455193720292</v>
+      </c>
+      <c r="F14" s="2" t="n">
+        <v>584.91</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="n">
-        <v>6.65373593151003</v>
+      <c r="A15" s="1" t="s">
+        <v>115</v>
       </c>
       <c r="B15" s="2" t="n">
-        <v>0.513321748253538</v>
+        <v>7.32125720900175</v>
       </c>
       <c r="C15" s="2" t="n">
-        <v>0.023985448211857</v>
+        <v>0.557150517356331</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>2.01042075458442</v>
+        <v>0.0385399551307968</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>455.75</v>
+        <v>2.01113203569632</v>
+      </c>
+      <c r="F15" s="2" t="n">
+        <v>431.780000000001</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="n">
-        <v>6.53950163359604</v>
+      <c r="A16" s="1" t="s">
+        <v>116</v>
       </c>
       <c r="B16" s="2" t="n">
-        <v>0.502996513092871</v>
+        <v>6.65373593151003</v>
       </c>
       <c r="C16" s="2" t="n">
-        <v>0.020866748124223</v>
+        <v>0.513321748253538</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>2.01412601171575</v>
+        <v>0.023985448211857</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>386.839999999999</v>
+        <v>2.01042075458442</v>
+      </c>
+      <c r="F16" s="2" t="n">
+        <v>455.75</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2" t="n">
-        <v>7.13126607639065</v>
+      <c r="A17" s="1" t="s">
+        <v>117</v>
       </c>
       <c r="B17" s="2" t="n">
-        <v>0.543014231235991</v>
+        <v>6.53950163359604</v>
       </c>
       <c r="C17" s="2" t="n">
-        <v>0.0328599150760521</v>
+        <v>0.502996513092871</v>
       </c>
       <c r="D17" s="2" t="n">
-        <v>2.01810073919145</v>
+        <v>0.020866748124223</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>470.43</v>
+        <v>2.01412601171575</v>
+      </c>
+      <c r="F17" s="2" t="n">
+        <v>386.839999999999</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2" t="n">
-        <v>8.62388826583393</v>
+      <c r="A18" s="1" t="s">
+        <v>118</v>
       </c>
       <c r="B18" s="2" t="n">
-        <v>0.607429528400724</v>
+        <v>7.13126607639065</v>
       </c>
       <c r="C18" s="2" t="n">
-        <v>0.051176100886292</v>
+        <v>0.543014231235991</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>2.01335433027284</v>
+        <v>0.0328599150760521</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>493.219999999999</v>
+        <v>2.01810073919145</v>
+      </c>
+      <c r="F18" s="2" t="n">
+        <v>470.43</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="n">
-        <v>6.98376251834528</v>
+      <c r="A19" s="1" t="s">
+        <v>119</v>
       </c>
       <c r="B19" s="2" t="n">
-        <v>0.532848003333</v>
+        <v>8.62388826583393</v>
       </c>
       <c r="C19" s="2" t="n">
-        <v>0.029399659128075</v>
+        <v>0.607429528400724</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>2.01383868377864</v>
+        <v>0.051176100886292</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>619.790000000001</v>
+        <v>2.01335433027284</v>
+      </c>
+      <c r="F19" s="2" t="n">
+        <v>493.219999999999</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2" t="n">
-        <v>6.23430366722677</v>
+      <c r="A20" s="1" t="s">
+        <v>120</v>
       </c>
       <c r="B20" s="2" t="n">
-        <v>0.470928237391508</v>
+        <v>6.98376251834528</v>
       </c>
       <c r="C20" s="2" t="n">
-        <v>0.0140110846484889</v>
+        <v>0.532848003333</v>
       </c>
       <c r="D20" s="2" t="n">
-        <v>2.01523370332756</v>
+        <v>0.029399659128075</v>
       </c>
       <c r="E20" s="2" t="n">
-        <v>582.01</v>
+        <v>2.01383868377864</v>
+      </c>
+      <c r="F20" s="2" t="n">
+        <v>619.790000000001</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2" t="n">
-        <v>7.62008021546003</v>
+      <c r="A21" s="1" t="s">
+        <v>121</v>
       </c>
       <c r="B21" s="2" t="n">
-        <v>0.567415222531485</v>
+        <v>6.23430366722677</v>
       </c>
       <c r="C21" s="2" t="n">
-        <v>0.0394120948737954</v>
+        <v>0.470928237391508</v>
       </c>
       <c r="D21" s="2" t="n">
-        <v>2.01589216699744</v>
+        <v>0.0140110846484889</v>
       </c>
       <c r="E21" s="2" t="n">
-        <v>815.4</v>
+        <v>2.01523370332756</v>
+      </c>
+      <c r="F21" s="2" t="n">
+        <v>582.01</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2" t="n">
-        <v>7.84092468974464</v>
+      <c r="A22" s="1" t="s">
+        <v>122</v>
       </c>
       <c r="B22" s="2" t="n">
-        <v>0.572652843368219</v>
+        <v>7.62008021546003</v>
       </c>
       <c r="C22" s="2" t="n">
-        <v>0.0422298293307148</v>
+        <v>0.567415222531485</v>
       </c>
       <c r="D22" s="2" t="n">
-        <v>2.01192219614761</v>
+        <v>0.0394120948737954</v>
       </c>
       <c r="E22" s="2" t="n">
-        <v>603.93</v>
+        <v>2.01589216699744</v>
+      </c>
+      <c r="F22" s="2" t="n">
+        <v>815.4</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="2" t="n">
-        <v>7.82759356560142</v>
+      <c r="A23" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="B23" s="2" t="n">
-        <v>0.573636997213633</v>
+        <v>7.84092468974464</v>
       </c>
       <c r="C23" s="2" t="n">
-        <v>0.0416752157118297</v>
+        <v>0.572652843368219</v>
       </c>
       <c r="D23" s="2" t="n">
-        <v>2.00659590334396</v>
+        <v>0.0422298293307148</v>
       </c>
       <c r="E23" s="2" t="n">
-        <v>623.049999999999</v>
+        <v>2.01192219614761</v>
+      </c>
+      <c r="F23" s="2" t="n">
+        <v>603.93</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="2" t="n">
-        <v>7.69105606485592</v>
+      <c r="A24" s="1" t="s">
+        <v>124</v>
       </c>
       <c r="B24" s="2" t="n">
-        <v>0.567267151862527</v>
+        <v>7.82759356560142</v>
       </c>
       <c r="C24" s="2" t="n">
-        <v>0.0395108618495128</v>
+        <v>0.573636997213633</v>
       </c>
       <c r="D24" s="2" t="n">
-        <v>2.01412792590296</v>
+        <v>0.0416752157118297</v>
       </c>
       <c r="E24" s="2" t="n">
-        <v>762.23</v>
+        <v>2.00659590334396</v>
+      </c>
+      <c r="F24" s="2" t="n">
+        <v>623.049999999999</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="2" t="n">
-        <v>7.99207528977856</v>
+      <c r="A25" s="1" t="s">
+        <v>125</v>
       </c>
       <c r="B25" s="2" t="n">
-        <v>0.580119287898651</v>
+        <v>7.69105606485592</v>
       </c>
       <c r="C25" s="2" t="n">
-        <v>0.0434199507308901</v>
+        <v>0.567267151862527</v>
       </c>
       <c r="D25" s="2" t="n">
-        <v>2.01344266134737</v>
+        <v>0.0395108618495128</v>
       </c>
       <c r="E25" s="2" t="n">
-        <v>780.01</v>
+        <v>2.01412792590296</v>
+      </c>
+      <c r="F25" s="2" t="n">
+        <v>762.23</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="2" t="n">
-        <v>7.50286278469249</v>
+      <c r="A26" s="1" t="s">
+        <v>126</v>
       </c>
       <c r="B26" s="2" t="n">
-        <v>0.559657009834094</v>
+        <v>7.99207528977856</v>
       </c>
       <c r="C26" s="2" t="n">
-        <v>0.0376280562921721</v>
+        <v>0.580119287898651</v>
       </c>
       <c r="D26" s="2" t="n">
-        <v>2.01420578737007</v>
+        <v>0.0434199507308901</v>
       </c>
       <c r="E26" s="2" t="n">
-        <v>562.110000000001</v>
+        <v>2.01344266134737</v>
+      </c>
+      <c r="F26" s="2" t="n">
+        <v>780.01</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="2" t="n">
-        <v>6.84853066747513</v>
+      <c r="A27" s="1" t="s">
+        <v>127</v>
       </c>
       <c r="B27" s="2" t="n">
-        <v>0.519320810726022</v>
+        <v>7.50286278469249</v>
       </c>
       <c r="C27" s="2" t="n">
-        <v>0.0274388617373422</v>
+        <v>0.559657009834094</v>
       </c>
       <c r="D27" s="2" t="n">
-        <v>2.01550649489432</v>
+        <v>0.0376280562921721</v>
       </c>
       <c r="E27" s="2" t="n">
-        <v>526.57</v>
+        <v>2.01420578737007</v>
+      </c>
+      <c r="F27" s="2" t="n">
+        <v>562.110000000001</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="2" t="n">
-        <v>9.14333172665165</v>
+      <c r="A28" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="B28" s="2" t="n">
-        <v>0.642485475713828</v>
+        <v>6.84853066747513</v>
       </c>
       <c r="C28" s="2" t="n">
-        <v>0.0601153343313675</v>
+        <v>0.519320810726022</v>
       </c>
       <c r="D28" s="2" t="n">
-        <v>2.01555432283395</v>
+        <v>0.0274388617373422</v>
       </c>
       <c r="E28" s="2" t="n">
-        <v>982.790000000001</v>
+        <v>2.01550649489432</v>
+      </c>
+      <c r="F28" s="2" t="n">
+        <v>526.57</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="2" t="n">
-        <v>8.21177640874369</v>
+      <c r="A29" s="1" t="s">
+        <v>129</v>
       </c>
       <c r="B29" s="2" t="n">
-        <v>0.591839877046792</v>
+        <v>9.14333172665165</v>
       </c>
       <c r="C29" s="2" t="n">
-        <v>0.0461762202080638</v>
+        <v>0.642485475713828</v>
       </c>
       <c r="D29" s="2" t="n">
-        <v>2.01104547043623</v>
+        <v>0.0601153343313675</v>
       </c>
       <c r="E29" s="2" t="n">
-        <v>536.66</v>
+        <v>2.01555432283395</v>
+      </c>
+      <c r="F29" s="2" t="n">
+        <v>982.790000000001</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="2" t="n">
+      <c r="A30" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B30" s="2" t="n">
+        <v>8.21177640874369</v>
+      </c>
+      <c r="C30" s="2" t="n">
+        <v>0.591839877046792</v>
+      </c>
+      <c r="D30" s="2" t="n">
+        <v>0.0461762202080638</v>
+      </c>
+      <c r="E30" s="2" t="n">
+        <v>2.01104547043623</v>
+      </c>
+      <c r="F30" s="2" t="n">
+        <v>536.66</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B31" s="2" t="n">
         <v>6.20424969723244</v>
       </c>
-      <c r="B30" s="2" t="n">
+      <c r="C31" s="2" t="n">
         <v>0.500510559563247</v>
       </c>
-      <c r="C30" s="2" t="n">
+      <c r="D31" s="2" t="n">
         <v>0.0220650119427435</v>
       </c>
-      <c r="D30" s="2" t="n">
+      <c r="E31" s="2" t="n">
         <v>2.01030516181707</v>
       </c>
-      <c r="E30" s="2" t="n">
+      <c r="F31" s="2" t="n">
         <v>549.419999999998</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -27925,7 +29169,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -27935,7 +29179,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
box plots etc analysis with our 4 algos
</commit_message>
<xml_diff>
--- a/results_from_all_algos.xlsx
+++ b/results_from_all_algos.xlsx
@@ -8,11 +8,11 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="WOA_CONV" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="WOA_RESULTS" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="GA" sheetId="3" state="visible" r:id="rId5"/>
-    <sheet name="SA" sheetId="4" state="visible" r:id="rId6"/>
-    <sheet name="CSA" sheetId="5" state="visible" r:id="rId7"/>
+    <sheet name="WOA_CONV" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="WOA_RESULTS" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="GA" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="SA" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="CSA" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="147">
   <si>
     <t xml:space="preserve">ITER#</t>
   </si>
@@ -434,6 +434,9 @@
     <t xml:space="preserve">Convergence agents 300 iters 30</t>
   </si>
   <si>
+    <t xml:space="preserve">Obj</t>
+  </si>
+  <si>
     <t xml:space="preserve">Par1</t>
   </si>
   <si>
@@ -443,10 +446,19 @@
     <t xml:space="preserve">Par3 </t>
   </si>
   <si>
-    <t xml:space="preserve">Obj</t>
+    <t xml:space="preserve">Time</t>
   </si>
   <si>
-    <t xml:space="preserve">Time</t>
+    <t xml:space="preserve">Agents 1000 iters 30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agents 500 iters 100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agents 50 iters 100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agents 300 iters 30</t>
   </si>
   <si>
     <t xml:space="preserve">Population 40</t>
@@ -559,114 +571,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
-  <a:themeElements>
-    <a:clrScheme name="LibreOffice">
-      <a:dk1>
-        <a:srgbClr val="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:srgbClr val="ffffff"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="000000"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="ffffff"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="18a303"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="0369a3"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="a33e03"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8e03a3"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="c99c00"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="c9211e"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000ee"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="551a8b"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme>
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -677,10 +583,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="Y1" activeCellId="0" sqref="Y1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B102" activeCellId="1" sqref="B2:F31 B102"/>
+      <selection pane="bottomRight" activeCell="B102" activeCellId="0" sqref="B102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="6.796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.77"/>
   </cols>
@@ -25028,7 +24934,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -25039,12 +24945,12 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" activeCellId="1" sqref="B2:F31 A2"/>
+      <selection pane="bottomRight" activeCell="R3" activeCellId="0" sqref="R3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="6.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="10.65"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25113,28 +25019,28 @@
       <c r="A2" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>102</v>
+      <c r="C2" s="1" t="s">
+        <v>141</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>133</v>
+      <c r="K2" s="1" t="s">
+        <v>142</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="R2" s="1" t="s">
-        <v>134</v>
+      <c r="S2" s="1" t="s">
+        <v>143</v>
       </c>
       <c r="X2" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="Y2" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="Z2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1" t="s">
+        <v>144</v>
+      </c>
       <c r="AA2" s="1"/>
       <c r="AB2" s="1"/>
     </row>
@@ -25143,16 +25049,16 @@
         <v>103</v>
       </c>
       <c r="B3" s="2" t="n">
+        <v>4.73282705256699</v>
+      </c>
+      <c r="C3" s="2" t="n">
         <v>0.483995014449269</v>
       </c>
-      <c r="C3" s="2" t="n">
+      <c r="D3" s="2" t="n">
         <v>0.0112592656129446</v>
       </c>
-      <c r="D3" s="2" t="n">
+      <c r="E3" s="2" t="n">
         <v>2.02294816843838</v>
-      </c>
-      <c r="E3" s="2" t="n">
-        <v>4.73282705256699</v>
       </c>
       <c r="F3" s="2" t="n">
         <v>113.549999999999</v>
@@ -25161,16 +25067,16 @@
         <v>103</v>
       </c>
       <c r="J3" s="2" t="n">
+        <v>4.73384437044199</v>
+      </c>
+      <c r="K3" s="2" t="n">
         <v>0.486686723823064</v>
       </c>
-      <c r="K3" s="2" t="n">
+      <c r="L3" s="2" t="n">
         <v>0.0117550885940693</v>
       </c>
-      <c r="L3" s="2" t="n">
+      <c r="M3" s="2" t="n">
         <v>2.0227828178733</v>
-      </c>
-      <c r="M3" s="2" t="n">
-        <v>4.73384437044199</v>
       </c>
       <c r="N3" s="2" t="n">
         <v>200.299999999999</v>
@@ -25179,16 +25085,16 @@
         <v>103</v>
       </c>
       <c r="R3" s="2" t="n">
+        <v>10.7344618261651</v>
+      </c>
+      <c r="S3" s="2" t="n">
         <v>0.70250555215571</v>
       </c>
-      <c r="S3" s="2" t="n">
+      <c r="T3" s="2" t="n">
         <v>0.0639060190144499</v>
       </c>
-      <c r="T3" s="2" t="n">
+      <c r="U3" s="2" t="n">
         <v>2.01687084448769</v>
-      </c>
-      <c r="U3" s="2" t="n">
-        <v>10.7344618261651</v>
       </c>
       <c r="V3" s="2" t="n">
         <v>49.380000000001</v>
@@ -25197,16 +25103,16 @@
         <v>103</v>
       </c>
       <c r="Y3" s="2" t="n">
+        <v>6.69584862019204</v>
+      </c>
+      <c r="Z3" s="2" t="n">
         <v>0.573781261508616</v>
       </c>
-      <c r="Z3" s="2" t="n">
+      <c r="AA3" s="2" t="n">
         <v>0.0333309402681</v>
       </c>
-      <c r="AA3" s="2" t="n">
+      <c r="AB3" s="2" t="n">
         <v>2.01851960457967</v>
-      </c>
-      <c r="AB3" s="2" t="n">
-        <v>6.69584862019204</v>
       </c>
       <c r="AC3" s="2" t="n">
         <v>22.7600000000002</v>
@@ -25217,16 +25123,16 @@
         <v>104</v>
       </c>
       <c r="B4" s="2" t="n">
+        <v>4.73251624066684</v>
+      </c>
+      <c r="C4" s="2" t="n">
         <v>0.48453890996233</v>
       </c>
-      <c r="C4" s="2" t="n">
+      <c r="D4" s="2" t="n">
         <v>0.0113588997505762</v>
       </c>
-      <c r="D4" s="2" t="n">
+      <c r="E4" s="2" t="n">
         <v>2.02289857296998</v>
-      </c>
-      <c r="E4" s="2" t="n">
-        <v>4.73251624066684</v>
       </c>
       <c r="F4" s="2" t="n">
         <v>211.469999999999</v>
@@ -25235,16 +25141,16 @@
         <v>104</v>
       </c>
       <c r="J4" s="2" t="n">
+        <v>4.84794027256065</v>
+      </c>
+      <c r="K4" s="2" t="n">
         <v>0.501964506312286</v>
       </c>
-      <c r="K4" s="2" t="n">
+      <c r="L4" s="2" t="n">
         <v>0.0152840476580599</v>
       </c>
-      <c r="L4" s="2" t="n">
+      <c r="M4" s="2" t="n">
         <v>2.02184590448036</v>
-      </c>
-      <c r="M4" s="2" t="n">
-        <v>4.84794027256065</v>
       </c>
       <c r="N4" s="2" t="n">
         <v>391.849999999999</v>
@@ -25253,16 +25159,16 @@
         <v>104</v>
       </c>
       <c r="R4" s="2" t="n">
+        <v>14.5297619190541</v>
+      </c>
+      <c r="S4" s="2" t="n">
         <v>0.762478631397603</v>
       </c>
-      <c r="S4" s="2" t="n">
+      <c r="T4" s="2" t="n">
         <v>0.0953098289247004</v>
       </c>
-      <c r="T4" s="2" t="n">
+      <c r="U4" s="2" t="n">
         <v>2.01261747116299</v>
-      </c>
-      <c r="U4" s="2" t="n">
-        <v>14.5297619190541</v>
       </c>
       <c r="V4" s="2" t="n">
         <v>103.880000000001</v>
@@ -25271,16 +25177,16 @@
         <v>104</v>
       </c>
       <c r="Y4" s="2" t="n">
+        <v>4.93002892499933</v>
+      </c>
+      <c r="Z4" s="2" t="n">
         <v>0.510256231968616</v>
       </c>
-      <c r="Z4" s="2" t="n">
+      <c r="AA4" s="2" t="n">
         <v>0.0167051762212759</v>
       </c>
-      <c r="AA4" s="2" t="n">
+      <c r="AB4" s="2" t="n">
         <v>2.02173487369732</v>
-      </c>
-      <c r="AB4" s="2" t="n">
-        <v>4.93002892499933</v>
       </c>
       <c r="AC4" s="2" t="n">
         <v>43.3400000000001</v>
@@ -25291,16 +25197,16 @@
         <v>105</v>
       </c>
       <c r="B5" s="2" t="n">
+        <v>4.73750625719472</v>
+      </c>
+      <c r="C5" s="2" t="n">
         <v>0.488255319227011</v>
       </c>
-      <c r="C5" s="2" t="n">
+      <c r="D5" s="2" t="n">
         <v>0.0121396899075259</v>
       </c>
-      <c r="D5" s="2" t="n">
+      <c r="E5" s="2" t="n">
         <v>2.02269208900668</v>
-      </c>
-      <c r="E5" s="2" t="n">
-        <v>4.73750625719472</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>305</v>
@@ -25309,16 +25215,16 @@
         <v>105</v>
       </c>
       <c r="J5" s="2" t="n">
+        <v>4.73605216732573</v>
+      </c>
+      <c r="K5" s="2" t="n">
         <v>0.481902460643336</v>
       </c>
-      <c r="K5" s="2" t="n">
+      <c r="L5" s="2" t="n">
         <v>0.0107935163956716</v>
       </c>
-      <c r="L5" s="2" t="n">
+      <c r="M5" s="2" t="n">
         <v>2.02304612788988</v>
-      </c>
-      <c r="M5" s="2" t="n">
-        <v>4.73605216732573</v>
       </c>
       <c r="N5" s="2" t="n">
         <v>580.74</v>
@@ -25327,16 +25233,16 @@
         <v>105</v>
       </c>
       <c r="R5" s="2" t="n">
+        <v>4.84804171549978</v>
+      </c>
+      <c r="S5" s="2" t="n">
         <v>0.504907264556651</v>
       </c>
-      <c r="S5" s="2" t="n">
+      <c r="T5" s="2" t="n">
         <v>0.0151636060931207</v>
       </c>
-      <c r="T5" s="2" t="n">
+      <c r="U5" s="2" t="n">
         <v>2.0222645194372</v>
-      </c>
-      <c r="U5" s="2" t="n">
-        <v>4.84804171549978</v>
       </c>
       <c r="V5" s="2" t="n">
         <v>145.140000000003</v>
@@ -25345,16 +25251,16 @@
         <v>105</v>
       </c>
       <c r="Y5" s="2" t="n">
+        <v>4.73609256977679</v>
+      </c>
+      <c r="Z5" s="2" t="n">
         <v>0.487641598070697</v>
       </c>
-      <c r="Z5" s="2" t="n">
+      <c r="AA5" s="2" t="n">
         <v>0.0120176090070576</v>
       </c>
-      <c r="AA5" s="2" t="n">
+      <c r="AB5" s="2" t="n">
         <v>2.02271261361793</v>
-      </c>
-      <c r="AB5" s="2" t="n">
-        <v>4.73609256977679</v>
       </c>
       <c r="AC5" s="2" t="n">
         <v>62.2899999999991</v>
@@ -25365,16 +25271,16 @@
         <v>106</v>
       </c>
       <c r="B6" s="2" t="n">
+        <v>4.73482989807527</v>
+      </c>
+      <c r="C6" s="2" t="n">
         <v>0.486920727836057</v>
       </c>
-      <c r="C6" s="2" t="n">
+      <c r="D6" s="2" t="n">
         <v>0.0118805081393316</v>
       </c>
-      <c r="D6" s="2" t="n">
+      <c r="E6" s="2" t="n">
         <v>2.02273985286532</v>
-      </c>
-      <c r="E6" s="2" t="n">
-        <v>4.73482989807527</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>397.769999999999</v>
@@ -25383,16 +25289,16 @@
         <v>106</v>
       </c>
       <c r="J6" s="2" t="n">
+        <v>4.74029720513826</v>
+      </c>
+      <c r="K6" s="2" t="n">
         <v>0.488586469425249</v>
       </c>
-      <c r="K6" s="2" t="n">
+      <c r="L6" s="2" t="n">
         <v>0.0122937737971205</v>
       </c>
-      <c r="L6" s="2" t="n">
+      <c r="M6" s="2" t="n">
         <v>2.02259988299427</v>
-      </c>
-      <c r="M6" s="2" t="n">
-        <v>4.74029720513826</v>
       </c>
       <c r="N6" s="2" t="n">
         <v>765.299999999999</v>
@@ -25401,16 +25307,16 @@
         <v>106</v>
       </c>
       <c r="R6" s="2" t="n">
+        <v>7.76741733991397</v>
+      </c>
+      <c r="S6" s="2" t="n">
         <v>0.596774641811278</v>
       </c>
-      <c r="S6" s="2" t="n">
+      <c r="T6" s="2" t="n">
         <v>0.0410998544992935</v>
       </c>
-      <c r="T6" s="2" t="n">
+      <c r="U6" s="2" t="n">
         <v>2.01726506829025</v>
-      </c>
-      <c r="U6" s="2" t="n">
-        <v>7.76741733991397</v>
       </c>
       <c r="V6" s="2" t="n">
         <v>193.170000000002</v>
@@ -25419,16 +25325,16 @@
         <v>106</v>
       </c>
       <c r="Y6" s="2" t="n">
+        <v>4.86063198429821</v>
+      </c>
+      <c r="Z6" s="2" t="n">
         <v>0.505927587799093</v>
       </c>
-      <c r="Z6" s="2" t="n">
+      <c r="AA6" s="2" t="n">
         <v>0.0154304267644149</v>
       </c>
-      <c r="AA6" s="2" t="n">
+      <c r="AB6" s="2" t="n">
         <v>2.02210058835512</v>
-      </c>
-      <c r="AB6" s="2" t="n">
-        <v>4.86063198429821</v>
       </c>
       <c r="AC6" s="2" t="n">
         <v>81.3600000000006</v>
@@ -25439,16 +25345,16 @@
         <v>107</v>
       </c>
       <c r="B7" s="2" t="n">
+        <v>4.73256901104308</v>
+      </c>
+      <c r="C7" s="2" t="n">
         <v>0.484369816622317</v>
       </c>
-      <c r="C7" s="2" t="n">
+      <c r="D7" s="2" t="n">
         <v>0.0113165593622519</v>
       </c>
-      <c r="D7" s="2" t="n">
+      <c r="E7" s="2" t="n">
         <v>2.0228363511855</v>
-      </c>
-      <c r="E7" s="2" t="n">
-        <v>4.73256901104308</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>490.279999999999</v>
@@ -25457,16 +25363,16 @@
         <v>107</v>
       </c>
       <c r="J7" s="2" t="n">
+        <v>4.73272127602358</v>
+      </c>
+      <c r="K7" s="2" t="n">
         <v>0.483923166804581</v>
       </c>
-      <c r="K7" s="2" t="n">
+      <c r="L7" s="2" t="n">
         <v>0.0112759683315727</v>
       </c>
-      <c r="L7" s="2" t="n">
+      <c r="M7" s="2" t="n">
         <v>2.02291384221503</v>
-      </c>
-      <c r="M7" s="2" t="n">
-        <v>4.73272127602358</v>
       </c>
       <c r="N7" s="2" t="n">
         <v>954.009999999998</v>
@@ -25475,16 +25381,16 @@
         <v>107</v>
       </c>
       <c r="R7" s="2" t="n">
+        <v>4.77334183599085</v>
+      </c>
+      <c r="S7" s="2" t="n">
         <v>0.474399476808662</v>
       </c>
-      <c r="S7" s="2" t="n">
+      <c r="T7" s="2" t="n">
         <v>0.0094660091812013</v>
       </c>
-      <c r="T7" s="2" t="n">
+      <c r="U7" s="2" t="n">
         <v>2.02332243348813</v>
-      </c>
-      <c r="U7" s="2" t="n">
-        <v>4.77334183599085</v>
       </c>
       <c r="V7" s="2" t="n">
         <v>237.940000000002</v>
@@ -25493,16 +25399,16 @@
         <v>107</v>
       </c>
       <c r="Y7" s="2" t="n">
+        <v>6.60147190401879</v>
+      </c>
+      <c r="Z7" s="2" t="n">
         <v>0.581859590187604</v>
       </c>
-      <c r="Z7" s="2" t="n">
+      <c r="AA7" s="2" t="n">
         <v>0.0322061123393598</v>
       </c>
-      <c r="AA7" s="2" t="n">
+      <c r="AB7" s="2" t="n">
         <v>2.01971131920745</v>
-      </c>
-      <c r="AB7" s="2" t="n">
-        <v>6.60147190401879</v>
       </c>
       <c r="AC7" s="2" t="n">
         <v>100.67</v>
@@ -25513,16 +25419,16 @@
         <v>108</v>
       </c>
       <c r="B8" s="2" t="n">
+        <v>4.73561216373413</v>
+      </c>
+      <c r="C8" s="2" t="n">
         <v>0.482080680682704</v>
       </c>
-      <c r="C8" s="2" t="n">
+      <c r="D8" s="2" t="n">
         <v>0.0108364418800382</v>
       </c>
-      <c r="D8" s="2" t="n">
+      <c r="E8" s="2" t="n">
         <v>2.02303898337413</v>
-      </c>
-      <c r="E8" s="2" t="n">
-        <v>4.73561216373413</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>585.82</v>
@@ -25531,16 +25437,16 @@
         <v>108</v>
       </c>
       <c r="J8" s="2" t="n">
+        <v>4.7333403236908</v>
+      </c>
+      <c r="K8" s="2" t="n">
         <v>0.48349900778137</v>
       </c>
-      <c r="K8" s="2" t="n">
+      <c r="L8" s="2" t="n">
         <v>0.0111101068358233</v>
       </c>
-      <c r="L8" s="2" t="n">
+      <c r="M8" s="2" t="n">
         <v>2.02297873418055</v>
-      </c>
-      <c r="M8" s="2" t="n">
-        <v>4.7333403236908</v>
       </c>
       <c r="N8" s="2" t="n">
         <v>1143.98</v>
@@ -25549,16 +25455,16 @@
         <v>108</v>
       </c>
       <c r="R8" s="2" t="n">
+        <v>5.9514484943827</v>
+      </c>
+      <c r="S8" s="2" t="n">
         <v>0.537463043234561</v>
       </c>
-      <c r="S8" s="2" t="n">
+      <c r="T8" s="2" t="n">
         <v>0.0258729206168746</v>
       </c>
-      <c r="T8" s="2" t="n">
+      <c r="U8" s="2" t="n">
         <v>2.01905457190039</v>
-      </c>
-      <c r="U8" s="2" t="n">
-        <v>5.9514484943827</v>
       </c>
       <c r="V8" s="2" t="n">
         <v>290.600000000002</v>
@@ -25567,16 +25473,16 @@
         <v>108</v>
       </c>
       <c r="Y8" s="2" t="n">
+        <v>5.32508805696527</v>
+      </c>
+      <c r="Z8" s="2" t="n">
         <v>0.52391739504947</v>
       </c>
-      <c r="Z8" s="2" t="n">
+      <c r="AA8" s="2" t="n">
         <v>0.0211143002626029</v>
       </c>
-      <c r="AA8" s="2" t="n">
+      <c r="AB8" s="2" t="n">
         <v>2.02032324216094</v>
-      </c>
-      <c r="AB8" s="2" t="n">
-        <v>5.32508805696527</v>
       </c>
       <c r="AC8" s="2" t="n">
         <v>119.77</v>
@@ -25587,16 +25493,16 @@
         <v>109</v>
       </c>
       <c r="B9" s="2" t="n">
+        <v>4.73264877533292</v>
+      </c>
+      <c r="C9" s="2" t="n">
         <v>0.484869753426814</v>
       </c>
-      <c r="C9" s="2" t="n">
+      <c r="D9" s="2" t="n">
         <v>0.0114109372160713</v>
       </c>
-      <c r="D9" s="2" t="n">
+      <c r="E9" s="2" t="n">
         <v>2.0228852689319</v>
-      </c>
-      <c r="E9" s="2" t="n">
-        <v>4.73264877533292</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>685.15</v>
@@ -25605,16 +25511,16 @@
         <v>109</v>
       </c>
       <c r="J9" s="2" t="n">
+        <v>4.79325080296581</v>
+      </c>
+      <c r="K9" s="2" t="n">
         <v>0.498072195395889</v>
       </c>
-      <c r="K9" s="2" t="n">
+      <c r="L9" s="2" t="n">
         <v>0.0141764024557666</v>
       </c>
-      <c r="L9" s="2" t="n">
+      <c r="M9" s="2" t="n">
         <v>2.02222982573153</v>
-      </c>
-      <c r="M9" s="2" t="n">
-        <v>4.79325080296581</v>
       </c>
       <c r="N9" s="2" t="n">
         <v>1333.63</v>
@@ -25623,16 +25529,16 @@
         <v>109</v>
       </c>
       <c r="R9" s="2" t="n">
+        <v>5.34689717187448</v>
+      </c>
+      <c r="S9" s="2" t="n">
         <v>0.535495712555746</v>
       </c>
-      <c r="S9" s="2" t="n">
+      <c r="T9" s="2" t="n">
         <v>0.0212835570985228</v>
       </c>
-      <c r="T9" s="2" t="n">
+      <c r="U9" s="2" t="n">
         <v>2.02138301988147</v>
-      </c>
-      <c r="U9" s="2" t="n">
-        <v>5.34689717187448</v>
       </c>
       <c r="V9" s="2" t="n">
         <v>337.170000000002</v>
@@ -25641,16 +25547,16 @@
         <v>109</v>
       </c>
       <c r="Y9" s="2" t="n">
+        <v>5.00113948180471</v>
+      </c>
+      <c r="Z9" s="2" t="n">
         <v>0.509737160282644</v>
       </c>
-      <c r="Z9" s="2" t="n">
+      <c r="AA9" s="2" t="n">
         <v>0.0174673638832025</v>
       </c>
-      <c r="AA9" s="2" t="n">
+      <c r="AB9" s="2" t="n">
         <v>2.02103148452504</v>
-      </c>
-      <c r="AB9" s="2" t="n">
-        <v>5.00113948180471</v>
       </c>
       <c r="AC9" s="2" t="n">
         <v>138.969999999999</v>
@@ -25661,16 +25567,16 @@
         <v>110</v>
       </c>
       <c r="B10" s="2" t="n">
+        <v>4.74131495839404</v>
+      </c>
+      <c r="C10" s="2" t="n">
         <v>0.489956988361554</v>
       </c>
-      <c r="C10" s="2" t="n">
+      <c r="D10" s="2" t="n">
         <v>0.012368679977516</v>
       </c>
-      <c r="D10" s="2" t="n">
+      <c r="E10" s="2" t="n">
         <v>2.02266395137885</v>
-      </c>
-      <c r="E10" s="2" t="n">
-        <v>4.74131495839404</v>
       </c>
       <c r="F10" s="2" t="n">
         <v>784.5</v>
@@ -25679,16 +25585,16 @@
         <v>110</v>
       </c>
       <c r="J10" s="2" t="n">
+        <v>4.73735478004939</v>
+      </c>
+      <c r="K10" s="2" t="n">
         <v>0.488077030100962</v>
       </c>
-      <c r="K10" s="2" t="n">
+      <c r="L10" s="2" t="n">
         <v>0.012121624921767</v>
       </c>
-      <c r="L10" s="2" t="n">
+      <c r="M10" s="2" t="n">
         <v>2.02267908532667</v>
-      </c>
-      <c r="M10" s="2" t="n">
-        <v>4.73735478004939</v>
       </c>
       <c r="N10" s="2" t="n">
         <v>1529.04</v>
@@ -25697,16 +25603,16 @@
         <v>110</v>
       </c>
       <c r="R10" s="2" t="n">
+        <v>6.30863179469164</v>
+      </c>
+      <c r="S10" s="2" t="n">
         <v>0.566669859201638</v>
       </c>
-      <c r="S10" s="2" t="n">
+      <c r="T10" s="2" t="n">
         <v>0.030344388859594</v>
       </c>
-      <c r="T10" s="2" t="n">
+      <c r="U10" s="2" t="n">
         <v>2.01940093529176</v>
-      </c>
-      <c r="U10" s="2" t="n">
-        <v>6.30863179469164</v>
       </c>
       <c r="V10" s="2" t="n">
         <v>388.950000000001</v>
@@ -25715,16 +25621,16 @@
         <v>110</v>
       </c>
       <c r="Y10" s="2" t="n">
+        <v>4.77622194267296</v>
+      </c>
+      <c r="Z10" s="2" t="n">
         <v>0.494577810189531</v>
       </c>
-      <c r="Z10" s="2" t="n">
+      <c r="AA10" s="2" t="n">
         <v>0.013660038381724</v>
       </c>
-      <c r="AA10" s="2" t="n">
+      <c r="AB10" s="2" t="n">
         <v>2.02214118791182</v>
-      </c>
-      <c r="AB10" s="2" t="n">
-        <v>4.77622194267296</v>
       </c>
       <c r="AC10" s="2" t="n">
         <v>157.9</v>
@@ -25735,16 +25641,16 @@
         <v>111</v>
       </c>
       <c r="B11" s="2" t="n">
+        <v>4.74341171169469</v>
+      </c>
+      <c r="C11" s="2" t="n">
         <v>0.490042199680028</v>
       </c>
-      <c r="C11" s="2" t="n">
+      <c r="D11" s="2" t="n">
         <v>0.0125160431424966</v>
       </c>
-      <c r="D11" s="2" t="n">
+      <c r="E11" s="2" t="n">
         <v>2.02259340337452</v>
-      </c>
-      <c r="E11" s="2" t="n">
-        <v>4.74341171169469</v>
       </c>
       <c r="F11" s="2" t="n">
         <v>885.129999999999</v>
@@ -25753,16 +25659,16 @@
         <v>111</v>
       </c>
       <c r="J11" s="2" t="n">
+        <v>4.73656998313829</v>
+      </c>
+      <c r="K11" s="2" t="n">
         <v>0.487590201683967</v>
       </c>
-      <c r="K11" s="2" t="n">
+      <c r="L11" s="2" t="n">
         <v>0.0120429467435466</v>
       </c>
-      <c r="L11" s="2" t="n">
+      <c r="M11" s="2" t="n">
         <v>2.02268585798644</v>
-      </c>
-      <c r="M11" s="2" t="n">
-        <v>4.73656998313829</v>
       </c>
       <c r="N11" s="2" t="n">
         <v>1727.35</v>
@@ -25771,16 +25677,16 @@
         <v>111</v>
       </c>
       <c r="R11" s="2" t="n">
+        <v>11.5474903969739</v>
+      </c>
+      <c r="S11" s="2" t="n">
         <v>0.705731959158286</v>
       </c>
-      <c r="S11" s="2" t="n">
+      <c r="T11" s="2" t="n">
         <v>0.0713197949829187</v>
       </c>
-      <c r="T11" s="2" t="n">
+      <c r="U11" s="2" t="n">
         <v>2.01507962508213</v>
-      </c>
-      <c r="U11" s="2" t="n">
-        <v>11.5474903969739</v>
       </c>
       <c r="V11" s="2" t="n">
         <v>440.360000000001</v>
@@ -25789,16 +25695,16 @@
         <v>111</v>
       </c>
       <c r="Y11" s="2" t="n">
+        <v>4.7616530580448</v>
+      </c>
+      <c r="Z11" s="2" t="n">
         <v>0.484889808225817</v>
       </c>
-      <c r="Z11" s="2" t="n">
+      <c r="AA11" s="2" t="n">
         <v>0.0120590748985078</v>
       </c>
-      <c r="AA11" s="2" t="n">
+      <c r="AB11" s="2" t="n">
         <v>2.0224987497498</v>
-      </c>
-      <c r="AB11" s="2" t="n">
-        <v>4.7616530580448</v>
       </c>
       <c r="AC11" s="2" t="n">
         <v>177.17</v>
@@ -25809,16 +25715,16 @@
         <v>112</v>
       </c>
       <c r="B12" s="2" t="n">
+        <v>4.73648664066337</v>
+      </c>
+      <c r="C12" s="2" t="n">
         <v>0.487487705243317</v>
       </c>
-      <c r="C12" s="2" t="n">
+      <c r="D12" s="2" t="n">
         <v>0.0120295958192213</v>
       </c>
-      <c r="D12" s="2" t="n">
+      <c r="E12" s="2" t="n">
         <v>2.02268541474894</v>
-      </c>
-      <c r="E12" s="2" t="n">
-        <v>4.73648664066337</v>
       </c>
       <c r="F12" s="2" t="n">
         <v>984.279999999999</v>
@@ -25827,16 +25733,16 @@
         <v>112</v>
       </c>
       <c r="J12" s="2" t="n">
+        <v>4.73301559715109</v>
+      </c>
+      <c r="K12" s="2" t="n">
         <v>0.485915675625117</v>
       </c>
-      <c r="K12" s="2" t="n">
+      <c r="L12" s="2" t="n">
         <v>0.0116649147933046</v>
       </c>
-      <c r="L12" s="2" t="n">
+      <c r="M12" s="2" t="n">
         <v>2.02278694356013</v>
-      </c>
-      <c r="M12" s="2" t="n">
-        <v>4.73301559715109</v>
       </c>
       <c r="N12" s="2" t="n">
         <v>1929.11</v>
@@ -25845,16 +25751,16 @@
         <v>112</v>
       </c>
       <c r="R12" s="2" t="n">
+        <v>5.28169354702721</v>
+      </c>
+      <c r="S12" s="2" t="n">
         <v>0.526519624734034</v>
       </c>
-      <c r="S12" s="2" t="n">
+      <c r="T12" s="2" t="n">
         <v>0.0209980096030192</v>
       </c>
-      <c r="T12" s="2" t="n">
+      <c r="U12" s="2" t="n">
         <v>2.02069182087361</v>
-      </c>
-      <c r="U12" s="2" t="n">
-        <v>5.28169354702721</v>
       </c>
       <c r="V12" s="2" t="n">
         <v>493.16</v>
@@ -25863,16 +25769,16 @@
         <v>112</v>
       </c>
       <c r="Y12" s="2" t="n">
+        <v>5.68621616072169</v>
+      </c>
+      <c r="Z12" s="2" t="n">
         <v>0.550729116328858</v>
       </c>
-      <c r="Z12" s="2" t="n">
+      <c r="AA12" s="2" t="n">
         <v>0.0241401540325002</v>
       </c>
-      <c r="AA12" s="2" t="n">
+      <c r="AB12" s="2" t="n">
         <v>2.02111164912474</v>
-      </c>
-      <c r="AB12" s="2" t="n">
-        <v>5.68621616072169</v>
       </c>
       <c r="AC12" s="2" t="n">
         <v>195.99</v>
@@ -25883,16 +25789,16 @@
         <v>113</v>
       </c>
       <c r="B13" s="2" t="n">
+        <v>4.73692276540307</v>
+      </c>
+      <c r="C13" s="2" t="n">
         <v>0.481925785181409</v>
       </c>
-      <c r="C13" s="2" t="n">
+      <c r="D13" s="2" t="n">
         <v>0.0107468659146244</v>
       </c>
-      <c r="D13" s="2" t="n">
+      <c r="E13" s="2" t="n">
         <v>2.02309831256724</v>
-      </c>
-      <c r="E13" s="2" t="n">
-        <v>4.73692276540307</v>
       </c>
       <c r="F13" s="2" t="n">
         <v>1083.19</v>
@@ -25901,16 +25807,16 @@
         <v>113</v>
       </c>
       <c r="J13" s="2" t="n">
+        <v>4.80216798492102</v>
+      </c>
+      <c r="K13" s="2" t="n">
         <v>0.498435743334862</v>
       </c>
-      <c r="K13" s="2" t="n">
+      <c r="L13" s="2" t="n">
         <v>0.014375442657964</v>
       </c>
-      <c r="L13" s="2" t="n">
+      <c r="M13" s="2" t="n">
         <v>2.02212274654092</v>
-      </c>
-      <c r="M13" s="2" t="n">
-        <v>4.80216798492102</v>
       </c>
       <c r="N13" s="2" t="n">
         <v>2130.21</v>
@@ -25919,16 +25825,16 @@
         <v>113</v>
       </c>
       <c r="R13" s="2" t="n">
+        <v>5.88178503180781</v>
+      </c>
+      <c r="S13" s="2" t="n">
         <v>0.541847904581337</v>
       </c>
-      <c r="S13" s="2" t="n">
+      <c r="T13" s="2" t="n">
         <v>0.026088534008324</v>
       </c>
-      <c r="T13" s="2" t="n">
+      <c r="U13" s="2" t="n">
         <v>2.01933686811595</v>
-      </c>
-      <c r="U13" s="2" t="n">
-        <v>5.88178503180781</v>
       </c>
       <c r="V13" s="2" t="n">
         <v>555.920000000002</v>
@@ -25937,16 +25843,16 @@
         <v>113</v>
       </c>
       <c r="Y13" s="2" t="n">
+        <v>4.73758688292009</v>
+      </c>
+      <c r="Z13" s="2" t="n">
         <v>0.488527002970693</v>
       </c>
-      <c r="Z13" s="2" t="n">
+      <c r="AA13" s="2" t="n">
         <v>0.0121472607154107</v>
       </c>
-      <c r="AA13" s="2" t="n">
+      <c r="AB13" s="2" t="n">
         <v>2.02271148184962</v>
-      </c>
-      <c r="AB13" s="2" t="n">
-        <v>4.73758688292009</v>
       </c>
       <c r="AC13" s="2" t="n">
         <v>215.120000000001</v>
@@ -25957,16 +25863,16 @@
         <v>114</v>
       </c>
       <c r="B14" s="2" t="n">
+        <v>4.73314513055998</v>
+      </c>
+      <c r="C14" s="2" t="n">
         <v>0.483570944580916</v>
       </c>
-      <c r="C14" s="2" t="n">
+      <c r="D14" s="2" t="n">
         <v>0.0111843226277482</v>
       </c>
-      <c r="D14" s="2" t="n">
+      <c r="E14" s="2" t="n">
         <v>2.02292081791604</v>
-      </c>
-      <c r="E14" s="2" t="n">
-        <v>4.73314513055998</v>
       </c>
       <c r="F14" s="2" t="n">
         <v>1183.74</v>
@@ -25975,16 +25881,16 @@
         <v>114</v>
       </c>
       <c r="J14" s="2" t="n">
+        <v>4.73751039481966</v>
+      </c>
+      <c r="K14" s="2" t="n">
         <v>0.481313787145444</v>
       </c>
-      <c r="K14" s="2" t="n">
+      <c r="L14" s="2" t="n">
         <v>0.0106823516658476</v>
       </c>
-      <c r="L14" s="2" t="n">
+      <c r="M14" s="2" t="n">
         <v>2.02307948539383</v>
-      </c>
-      <c r="M14" s="2" t="n">
-        <v>4.73751039481966</v>
       </c>
       <c r="N14" s="2" t="n">
         <v>2329.38</v>
@@ -25993,16 +25899,16 @@
         <v>114</v>
       </c>
       <c r="R14" s="2" t="n">
+        <v>14.5582643173828</v>
+      </c>
+      <c r="S14" s="2" t="n">
         <v>0.774988228655992</v>
       </c>
-      <c r="S14" s="2" t="n">
+      <c r="T14" s="2" t="n">
         <v>0.096873528581999</v>
       </c>
-      <c r="T14" s="2" t="n">
+      <c r="U14" s="2" t="n">
         <v>2.0129974060995</v>
-      </c>
-      <c r="U14" s="2" t="n">
-        <v>14.5582643173828</v>
       </c>
       <c r="V14" s="2" t="n">
         <v>610.59</v>
@@ -26011,16 +25917,16 @@
         <v>114</v>
       </c>
       <c r="Y14" s="2" t="n">
+        <v>4.81435007595051</v>
+      </c>
+      <c r="Z14" s="2" t="n">
         <v>0.500509530146158</v>
       </c>
-      <c r="Z14" s="2" t="n">
+      <c r="AA14" s="2" t="n">
         <v>0.0146612144728454</v>
       </c>
-      <c r="AA14" s="2" t="n">
+      <c r="AB14" s="2" t="n">
         <v>2.02218110450913</v>
-      </c>
-      <c r="AB14" s="2" t="n">
-        <v>4.81435007595051</v>
       </c>
       <c r="AC14" s="2" t="n">
         <v>234.93</v>
@@ -26031,16 +25937,16 @@
         <v>115</v>
       </c>
       <c r="B15" s="2" t="n">
+        <v>4.73375992424785</v>
+      </c>
+      <c r="C15" s="2" t="n">
         <v>0.486452638339125</v>
       </c>
-      <c r="C15" s="2" t="n">
+      <c r="D15" s="2" t="n">
         <v>0.0117491433047291</v>
       </c>
-      <c r="D15" s="2" t="n">
+      <c r="E15" s="2" t="n">
         <v>2.02279010691657</v>
-      </c>
-      <c r="E15" s="2" t="n">
-        <v>4.73375992424785</v>
       </c>
       <c r="F15" s="2" t="n">
         <v>1282.09</v>
@@ -26049,16 +25955,16 @@
         <v>115</v>
       </c>
       <c r="J15" s="2" t="n">
+        <v>4.73560747462796</v>
+      </c>
+      <c r="K15" s="2" t="n">
         <v>0.487195090834307</v>
       </c>
-      <c r="K15" s="2" t="n">
+      <c r="L15" s="2" t="n">
         <v>0.0119547932618644</v>
       </c>
-      <c r="L15" s="2" t="n">
+      <c r="M15" s="2" t="n">
         <v>2.02271116492208</v>
-      </c>
-      <c r="M15" s="2" t="n">
-        <v>4.73560747462796</v>
       </c>
       <c r="N15" s="2" t="n">
         <v>2536.14</v>
@@ -26067,16 +25973,16 @@
         <v>115</v>
       </c>
       <c r="R15" s="2" t="n">
+        <v>11.8556919869248</v>
+      </c>
+      <c r="S15" s="2" t="n">
         <v>0.715741418893173</v>
       </c>
-      <c r="S15" s="2" t="n">
+      <c r="T15" s="2" t="n">
         <v>0.0739514877525552</v>
       </c>
-      <c r="T15" s="2" t="n">
+      <c r="U15" s="2" t="n">
         <v>2.01497036629778</v>
-      </c>
-      <c r="U15" s="2" t="n">
-        <v>11.8556919869248</v>
       </c>
       <c r="V15" s="2" t="n">
         <v>652.950000000001</v>
@@ -26085,16 +25991,16 @@
         <v>115</v>
       </c>
       <c r="Y15" s="2" t="n">
+        <v>5.16877539087627</v>
+      </c>
+      <c r="Z15" s="2" t="n">
         <v>0.526115886200987</v>
       </c>
-      <c r="Z15" s="2" t="n">
+      <c r="AA15" s="2" t="n">
         <v>0.0195758104148813</v>
       </c>
-      <c r="AA15" s="2" t="n">
+      <c r="AB15" s="2" t="n">
         <v>2.0214757228493</v>
-      </c>
-      <c r="AB15" s="2" t="n">
-        <v>5.16877539087627</v>
       </c>
       <c r="AC15" s="2" t="n">
         <v>253.65</v>
@@ -26105,16 +26011,16 @@
         <v>116</v>
       </c>
       <c r="B16" s="2" t="n">
+        <v>4.73255095728732</v>
+      </c>
+      <c r="C16" s="2" t="n">
         <v>0.485266574729285</v>
       </c>
-      <c r="C16" s="2" t="n">
+      <c r="D16" s="2" t="n">
         <v>0.0114431495749795</v>
       </c>
-      <c r="D16" s="2" t="n">
+      <c r="E16" s="2" t="n">
         <v>2.02299536134802</v>
-      </c>
-      <c r="E16" s="2" t="n">
-        <v>4.73255095728732</v>
       </c>
       <c r="F16" s="2" t="n">
         <v>1381.48</v>
@@ -26123,16 +26029,16 @@
         <v>116</v>
       </c>
       <c r="J16" s="2" t="n">
+        <v>4.73358870609277</v>
+      </c>
+      <c r="K16" s="2" t="n">
         <v>0.486334908535697</v>
       </c>
-      <c r="K16" s="2" t="n">
+      <c r="L16" s="2" t="n">
         <v>0.0117210764837736</v>
       </c>
-      <c r="L16" s="2" t="n">
+      <c r="M16" s="2" t="n">
         <v>2.02279777580486</v>
-      </c>
-      <c r="M16" s="2" t="n">
-        <v>4.73358870609277</v>
       </c>
       <c r="N16" s="2" t="n">
         <v>2731.38</v>
@@ -26141,16 +26047,16 @@
         <v>116</v>
       </c>
       <c r="R16" s="2" t="n">
+        <v>4.73468742483637</v>
+      </c>
+      <c r="S16" s="2" t="n">
         <v>0.487292801271241</v>
       </c>
-      <c r="S16" s="2" t="n">
+      <c r="T16" s="2" t="n">
         <v>0.0118434914597135</v>
       </c>
-      <c r="T16" s="2" t="n">
+      <c r="U16" s="2" t="n">
         <v>2.0228137742823</v>
-      </c>
-      <c r="U16" s="2" t="n">
-        <v>4.73468742483637</v>
       </c>
       <c r="V16" s="2" t="n">
         <v>691.280000000003</v>
@@ -26159,16 +26065,16 @@
         <v>116</v>
       </c>
       <c r="Y16" s="2" t="n">
+        <v>4.76757257254872</v>
+      </c>
+      <c r="Z16" s="2" t="n">
         <v>0.494714017032156</v>
       </c>
-      <c r="Z16" s="2" t="n">
+      <c r="AA16" s="2" t="n">
         <v>0.0134696460555681</v>
       </c>
-      <c r="AA16" s="2" t="n">
+      <c r="AB16" s="2" t="n">
         <v>2.02238460546414</v>
-      </c>
-      <c r="AB16" s="2" t="n">
-        <v>4.76757257254872</v>
       </c>
       <c r="AC16" s="2" t="n">
         <v>274.950000000001</v>
@@ -26179,16 +26085,16 @@
         <v>117</v>
       </c>
       <c r="B17" s="2" t="n">
+        <v>4.73264797386738</v>
+      </c>
+      <c r="C17" s="2" t="n">
         <v>0.484852986525434</v>
       </c>
-      <c r="C17" s="2" t="n">
+      <c r="D17" s="2" t="n">
         <v>0.011409496541767</v>
       </c>
-      <c r="D17" s="2" t="n">
+      <c r="E17" s="2" t="n">
         <v>2.02288566607849</v>
-      </c>
-      <c r="E17" s="2" t="n">
-        <v>4.73264797386738</v>
       </c>
       <c r="F17" s="2" t="n">
         <v>1480.85</v>
@@ -26197,16 +26103,16 @@
         <v>117</v>
       </c>
       <c r="J17" s="2" t="n">
+        <v>4.73241918756398</v>
+      </c>
+      <c r="K17" s="2" t="n">
         <v>0.484993264429524</v>
       </c>
-      <c r="K17" s="2" t="n">
+      <c r="L17" s="2" t="n">
         <v>0.0114695858242343</v>
       </c>
-      <c r="L17" s="2" t="n">
+      <c r="M17" s="2" t="n">
         <v>2.02284937300368</v>
-      </c>
-      <c r="M17" s="2" t="n">
-        <v>4.73241918756398</v>
       </c>
       <c r="N17" s="2" t="n">
         <v>2921.38</v>
@@ -26215,16 +26121,16 @@
         <v>117</v>
       </c>
       <c r="R17" s="2" t="n">
+        <v>6.18732062337219</v>
+      </c>
+      <c r="S17" s="2" t="n">
         <v>0.554872470932307</v>
       </c>
-      <c r="S17" s="2" t="n">
+      <c r="T17" s="2" t="n">
         <v>0.0289854704792675</v>
       </c>
-      <c r="T17" s="2" t="n">
+      <c r="U17" s="2" t="n">
         <v>2.01904941973475</v>
-      </c>
-      <c r="U17" s="2" t="n">
-        <v>6.18732062337219</v>
       </c>
       <c r="V17" s="2" t="n">
         <v>734.82</v>
@@ -26233,16 +26139,16 @@
         <v>117</v>
       </c>
       <c r="Y17" s="2" t="n">
+        <v>5.22476421829463</v>
+      </c>
+      <c r="Z17" s="2" t="n">
         <v>0.529731302076161</v>
       </c>
-      <c r="Z17" s="2" t="n">
+      <c r="AA17" s="2" t="n">
         <v>0.0199028781415373</v>
       </c>
-      <c r="AA17" s="2" t="n">
+      <c r="AB17" s="2" t="n">
         <v>2.02173496437402</v>
-      </c>
-      <c r="AB17" s="2" t="n">
-        <v>5.22476421829463</v>
       </c>
       <c r="AC17" s="2" t="n">
         <v>296.9</v>
@@ -26253,16 +26159,16 @@
         <v>118</v>
       </c>
       <c r="B18" s="2" t="n">
+        <v>4.73248753274178</v>
+      </c>
+      <c r="C18" s="2" t="n">
         <v>0.48485401527131</v>
       </c>
-      <c r="C18" s="2" t="n">
+      <c r="D18" s="2" t="n">
         <v>0.0114020830898292</v>
       </c>
-      <c r="D18" s="2" t="n">
+      <c r="E18" s="2" t="n">
         <v>2.022881086327</v>
-      </c>
-      <c r="E18" s="2" t="n">
-        <v>4.73248753274178</v>
       </c>
       <c r="F18" s="2" t="n">
         <v>1580.12</v>
@@ -26271,16 +26177,16 @@
         <v>118</v>
       </c>
       <c r="J18" s="2" t="n">
+        <v>4.77669216311506</v>
+      </c>
+      <c r="K18" s="2" t="n">
         <v>0.495414479181898</v>
       </c>
-      <c r="K18" s="2" t="n">
+      <c r="L18" s="2" t="n">
         <v>0.0137246373502613</v>
       </c>
-      <c r="L18" s="2" t="n">
+      <c r="M18" s="2" t="n">
         <v>2.0222695728743</v>
-      </c>
-      <c r="M18" s="2" t="n">
-        <v>4.77669216311506</v>
       </c>
       <c r="N18" s="2" t="n">
         <v>3105.83</v>
@@ -26289,16 +26195,16 @@
         <v>118</v>
       </c>
       <c r="R18" s="2" t="n">
+        <v>5.28134539080513</v>
+      </c>
+      <c r="S18" s="2" t="n">
         <v>0.531357198793434</v>
       </c>
-      <c r="S18" s="2" t="n">
+      <c r="T18" s="2" t="n">
         <v>0.0208859953286733</v>
       </c>
-      <c r="T18" s="2" t="n">
+      <c r="U18" s="2" t="n">
         <v>2.0212254148495</v>
-      </c>
-      <c r="U18" s="2" t="n">
-        <v>5.28134539080513</v>
       </c>
       <c r="V18" s="2" t="n">
         <v>786.540000000001</v>
@@ -26307,16 +26213,16 @@
         <v>118</v>
       </c>
       <c r="Y18" s="2" t="n">
+        <v>5.81314261535196</v>
+      </c>
+      <c r="Z18" s="2" t="n">
         <v>0.552438666640035</v>
       </c>
-      <c r="Z18" s="2" t="n">
+      <c r="AA18" s="2" t="n">
         <v>0.0260364439741952</v>
       </c>
-      <c r="AA18" s="2" t="n">
+      <c r="AB18" s="2" t="n">
         <v>2.02006521694369</v>
-      </c>
-      <c r="AB18" s="2" t="n">
-        <v>5.81314261535196</v>
       </c>
       <c r="AC18" s="2" t="n">
         <v>314.98</v>
@@ -26327,16 +26233,16 @@
         <v>119</v>
       </c>
       <c r="B19" s="2" t="n">
+        <v>4.7330864373861</v>
+      </c>
+      <c r="C19" s="2" t="n">
         <v>0.485753589303298</v>
       </c>
-      <c r="C19" s="2" t="n">
+      <c r="D19" s="2" t="n">
         <v>0.0116133013856941</v>
       </c>
-      <c r="D19" s="2" t="n">
+      <c r="E19" s="2" t="n">
         <v>2.02282259261874</v>
-      </c>
-      <c r="E19" s="2" t="n">
-        <v>4.7330864373861</v>
       </c>
       <c r="F19" s="2" t="n">
         <v>1682.39</v>
@@ -26345,16 +26251,16 @@
         <v>119</v>
       </c>
       <c r="J19" s="2" t="n">
+        <v>4.73834933861092</v>
+      </c>
+      <c r="K19" s="2" t="n">
         <v>0.481105786305422</v>
       </c>
-      <c r="K19" s="2" t="n">
+      <c r="L19" s="2" t="n">
         <v>0.0106260503903813</v>
       </c>
-      <c r="L19" s="2" t="n">
+      <c r="M19" s="2" t="n">
         <v>2.02310321175238</v>
-      </c>
-      <c r="M19" s="2" t="n">
-        <v>4.73834933861092</v>
       </c>
       <c r="N19" s="2" t="n">
         <v>3293.46</v>
@@ -26363,16 +26269,16 @@
         <v>119</v>
       </c>
       <c r="R19" s="2" t="n">
+        <v>5.9803077113851</v>
+      </c>
+      <c r="S19" s="2" t="n">
         <v>0.556150212218715</v>
       </c>
-      <c r="S19" s="2" t="n">
+      <c r="T19" s="2" t="n">
         <v>0.0275960798838708</v>
       </c>
-      <c r="T19" s="2" t="n">
+      <c r="U19" s="2" t="n">
         <v>2.01983412262115</v>
-      </c>
-      <c r="U19" s="2" t="n">
-        <v>5.9803077113851</v>
       </c>
       <c r="V19" s="2" t="n">
         <v>828.75</v>
@@ -26381,16 +26287,16 @@
         <v>119</v>
       </c>
       <c r="Y19" s="2" t="n">
+        <v>5.11984047261926</v>
+      </c>
+      <c r="Z19" s="2" t="n">
         <v>0.5237416884558</v>
       </c>
-      <c r="Z19" s="2" t="n">
+      <c r="AA19" s="2" t="n">
         <v>0.0179299563022002</v>
       </c>
-      <c r="AA19" s="2" t="n">
+      <c r="AB19" s="2" t="n">
         <v>2.0223093658777</v>
-      </c>
-      <c r="AB19" s="2" t="n">
-        <v>5.11984047261926</v>
       </c>
       <c r="AC19" s="2" t="n">
         <v>333.76</v>
@@ -26401,16 +26307,16 @@
         <v>120</v>
       </c>
       <c r="B20" s="2" t="n">
+        <v>4.73579054858861</v>
+      </c>
+      <c r="C20" s="2" t="n">
         <v>0.487839966860063</v>
       </c>
-      <c r="C20" s="2" t="n">
+      <c r="D20" s="2" t="n">
         <v>0.011984052181976</v>
       </c>
-      <c r="D20" s="2" t="n">
+      <c r="E20" s="2" t="n">
         <v>2.02274278922304</v>
-      </c>
-      <c r="E20" s="2" t="n">
-        <v>4.73579054858861</v>
       </c>
       <c r="F20" s="2" t="n">
         <v>1775.63</v>
@@ -26419,16 +26325,16 @@
         <v>120</v>
       </c>
       <c r="J20" s="2" t="n">
+        <v>4.73849025987369</v>
+      </c>
+      <c r="K20" s="2" t="n">
         <v>0.481280083277685</v>
       </c>
-      <c r="K20" s="2" t="n">
+      <c r="L20" s="2" t="n">
         <v>0.0106273021604792</v>
       </c>
-      <c r="L20" s="2" t="n">
+      <c r="M20" s="2" t="n">
         <v>2.02312322928082</v>
-      </c>
-      <c r="M20" s="2" t="n">
-        <v>4.73849025987369</v>
       </c>
       <c r="N20" s="2" t="n">
         <v>3496.81</v>
@@ -26437,16 +26343,16 @@
         <v>120</v>
       </c>
       <c r="R20" s="2" t="n">
+        <v>4.75755084223834</v>
+      </c>
+      <c r="S20" s="2" t="n">
         <v>0.4937422846595</v>
       </c>
-      <c r="S20" s="2" t="n">
+      <c r="T20" s="2" t="n">
         <v>0.0130622540715576</v>
       </c>
-      <c r="T20" s="2" t="n">
+      <c r="U20" s="2" t="n">
         <v>2.02259009753887</v>
-      </c>
-      <c r="U20" s="2" t="n">
-        <v>4.75755084223834</v>
       </c>
       <c r="V20" s="2" t="n">
         <v>868.75</v>
@@ -26455,16 +26361,16 @@
         <v>120</v>
       </c>
       <c r="Y20" s="2" t="n">
+        <v>5.53061476143937</v>
+      </c>
+      <c r="Z20" s="2" t="n">
         <v>0.544067303981715</v>
       </c>
-      <c r="Z20" s="2" t="n">
+      <c r="AA20" s="2" t="n">
         <v>0.0228259975865514</v>
       </c>
-      <c r="AA20" s="2" t="n">
+      <c r="AB20" s="2" t="n">
         <v>2.02110545965087</v>
-      </c>
-      <c r="AB20" s="2" t="n">
-        <v>5.53061476143937</v>
       </c>
       <c r="AC20" s="2" t="n">
         <v>354.780000000001</v>
@@ -26475,16 +26381,16 @@
         <v>121</v>
       </c>
       <c r="B21" s="2" t="n">
+        <v>4.73319867607468</v>
+      </c>
+      <c r="C21" s="2" t="n">
         <v>0.483607385815407</v>
       </c>
-      <c r="C21" s="2" t="n">
+      <c r="D21" s="2" t="n">
         <v>0.0111483072722219</v>
       </c>
-      <c r="D21" s="2" t="n">
+      <c r="E21" s="2" t="n">
         <v>2.02292645232688</v>
-      </c>
-      <c r="E21" s="2" t="n">
-        <v>4.73319867607468</v>
       </c>
       <c r="F21" s="2" t="n">
         <v>1871.51</v>
@@ -26493,16 +26399,16 @@
         <v>121</v>
       </c>
       <c r="J21" s="2" t="n">
+        <v>4.73354898677983</v>
+      </c>
+      <c r="K21" s="2" t="n">
         <v>0.483253573307956</v>
       </c>
-      <c r="K21" s="2" t="n">
+      <c r="L21" s="2" t="n">
         <v>0.0110852178796879</v>
       </c>
-      <c r="L21" s="2" t="n">
+      <c r="M21" s="2" t="n">
         <v>2.02296716033847</v>
-      </c>
-      <c r="M21" s="2" t="n">
-        <v>4.73354898677983</v>
       </c>
       <c r="N21" s="2" t="n">
         <v>3694.92</v>
@@ -26511,16 +26417,16 @@
         <v>121</v>
       </c>
       <c r="R21" s="2" t="n">
+        <v>4.7331248630718</v>
+      </c>
+      <c r="S21" s="2" t="n">
         <v>0.485272347057502</v>
       </c>
-      <c r="S21" s="2" t="n">
+      <c r="T21" s="2" t="n">
         <v>0.011406013099693</v>
       </c>
-      <c r="T21" s="2" t="n">
+      <c r="U21" s="2" t="n">
         <v>2.02293723685077</v>
-      </c>
-      <c r="U21" s="2" t="n">
-        <v>4.7331248630718</v>
       </c>
       <c r="V21" s="2" t="n">
         <v>910.050000000003</v>
@@ -26529,16 +26435,16 @@
         <v>121</v>
       </c>
       <c r="Y21" s="2" t="n">
+        <v>5.2828873580718</v>
+      </c>
+      <c r="Z21" s="2" t="n">
         <v>0.530037021685518</v>
       </c>
-      <c r="Z21" s="2" t="n">
+      <c r="AA21" s="2" t="n">
         <v>0.021010595448446</v>
       </c>
-      <c r="AA21" s="2" t="n">
+      <c r="AB21" s="2" t="n">
         <v>2.0205822677958</v>
-      </c>
-      <c r="AB21" s="2" t="n">
-        <v>5.2828873580718</v>
       </c>
       <c r="AC21" s="2" t="n">
         <v>374.030000000001</v>
@@ -26549,16 +26455,16 @@
         <v>122</v>
       </c>
       <c r="B22" s="2" t="n">
+        <v>4.79348280829329</v>
+      </c>
+      <c r="C22" s="2" t="n">
         <v>0.498066450857373</v>
       </c>
-      <c r="C22" s="2" t="n">
+      <c r="D22" s="2" t="n">
         <v>0.0141821487240554</v>
       </c>
-      <c r="D22" s="2" t="n">
+      <c r="E22" s="2" t="n">
         <v>2.02223163265957</v>
-      </c>
-      <c r="E22" s="2" t="n">
-        <v>4.79348280829329</v>
       </c>
       <c r="F22" s="2" t="n">
         <v>1970.68</v>
@@ -26567,16 +26473,16 @@
         <v>122</v>
       </c>
       <c r="J22" s="2" t="n">
+        <v>4.73334886183427</v>
+      </c>
+      <c r="K22" s="2" t="n">
         <v>0.486182458278899</v>
       </c>
-      <c r="K22" s="2" t="n">
+      <c r="L22" s="2" t="n">
         <v>0.0116140901791884</v>
       </c>
-      <c r="L22" s="2" t="n">
+      <c r="M22" s="2" t="n">
         <v>2.02287216569605</v>
-      </c>
-      <c r="M22" s="2" t="n">
-        <v>4.73334886183427</v>
       </c>
       <c r="N22" s="2" t="n">
         <v>3894.3</v>
@@ -26585,16 +26491,16 @@
         <v>122</v>
       </c>
       <c r="R22" s="2" t="n">
+        <v>11.7694177170813</v>
+      </c>
+      <c r="S22" s="2" t="n">
         <v>0.705382587214474</v>
       </c>
-      <c r="S22" s="2" t="n">
+      <c r="T22" s="2" t="n">
         <v>0.0728133047891965</v>
       </c>
-      <c r="T22" s="2" t="n">
+      <c r="U22" s="2" t="n">
         <v>2.01466901234254</v>
-      </c>
-      <c r="U22" s="2" t="n">
-        <v>11.7694177170813</v>
       </c>
       <c r="V22" s="2" t="n">
         <v>960.57</v>
@@ -26603,16 +26509,16 @@
         <v>122</v>
       </c>
       <c r="Y22" s="2" t="n">
+        <v>4.86966307436344</v>
+      </c>
+      <c r="Z22" s="2" t="n">
         <v>0.502964956823651</v>
       </c>
-      <c r="Z22" s="2" t="n">
+      <c r="AA22" s="2" t="n">
         <v>0.0156250656601103</v>
       </c>
-      <c r="AA22" s="2" t="n">
+      <c r="AB22" s="2" t="n">
         <v>2.02172328591852</v>
-      </c>
-      <c r="AB22" s="2" t="n">
-        <v>4.86966307436344</v>
       </c>
       <c r="AC22" s="2" t="n">
         <v>393.49</v>
@@ -26623,16 +26529,16 @@
         <v>123</v>
       </c>
       <c r="B23" s="2" t="n">
+        <v>4.74378462377099</v>
+      </c>
+      <c r="C23" s="2" t="n">
         <v>0.490241466189082</v>
       </c>
-      <c r="C23" s="2" t="n">
+      <c r="D23" s="2" t="n">
         <v>0.0125382278713031</v>
       </c>
-      <c r="D23" s="2" t="n">
+      <c r="E23" s="2" t="n">
         <v>2.02258031008103</v>
-      </c>
-      <c r="E23" s="2" t="n">
-        <v>4.74378462377099</v>
       </c>
       <c r="F23" s="2" t="n">
         <v>2066</v>
@@ -26641,16 +26547,16 @@
         <v>123</v>
       </c>
       <c r="J23" s="2" t="n">
+        <v>4.73292971435406</v>
+      </c>
+      <c r="K23" s="2" t="n">
         <v>0.485850592996181</v>
       </c>
-      <c r="K23" s="2" t="n">
+      <c r="L23" s="2" t="n">
         <v>0.011634890946519</v>
       </c>
-      <c r="L23" s="2" t="n">
+      <c r="M23" s="2" t="n">
         <v>2.02282266987091</v>
-      </c>
-      <c r="M23" s="2" t="n">
-        <v>4.73292971435406</v>
       </c>
       <c r="N23" s="2" t="n">
         <v>4093.77</v>
@@ -26659,16 +26565,16 @@
         <v>123</v>
       </c>
       <c r="R23" s="2" t="n">
+        <v>6.59016356265067</v>
+      </c>
+      <c r="S23" s="2" t="n">
         <v>0.572825057677677</v>
       </c>
-      <c r="S23" s="2" t="n">
+      <c r="T23" s="2" t="n">
         <v>0.032583147575317</v>
       </c>
-      <c r="T23" s="2" t="n">
+      <c r="U23" s="2" t="n">
         <v>2.01888770499756</v>
-      </c>
-      <c r="U23" s="2" t="n">
-        <v>6.59016356265067</v>
       </c>
       <c r="V23" s="2" t="n">
         <v>1000.8</v>
@@ -26677,16 +26583,16 @@
         <v>123</v>
       </c>
       <c r="Y23" s="2" t="n">
+        <v>5.6917015780514</v>
+      </c>
+      <c r="Z23" s="2" t="n">
         <v>0.551282825258859</v>
       </c>
-      <c r="Z23" s="2" t="n">
+      <c r="AA23" s="2" t="n">
         <v>0.0238474547305066</v>
       </c>
-      <c r="AA23" s="2" t="n">
+      <c r="AB23" s="2" t="n">
         <v>2.02155054029698</v>
-      </c>
-      <c r="AB23" s="2" t="n">
-        <v>5.6917015780514</v>
       </c>
       <c r="AC23" s="2" t="n">
         <v>412.27</v>
@@ -26697,16 +26603,16 @@
         <v>124</v>
       </c>
       <c r="B24" s="2" t="n">
+        <v>4.73989285970444</v>
+      </c>
+      <c r="C24" s="2" t="n">
         <v>0.488713970621203</v>
       </c>
-      <c r="C24" s="2" t="n">
+      <c r="D24" s="2" t="n">
         <v>0.0122874029570318</v>
       </c>
-      <c r="D24" s="2" t="n">
+      <c r="E24" s="2" t="n">
         <v>2.02251799986116</v>
-      </c>
-      <c r="E24" s="2" t="n">
-        <v>4.73989285970444</v>
       </c>
       <c r="F24" s="2" t="n">
         <v>2166.31</v>
@@ -26715,16 +26621,16 @@
         <v>124</v>
       </c>
       <c r="J24" s="2" t="n">
+        <v>4.83921510655197</v>
+      </c>
+      <c r="K24" s="2" t="n">
         <v>0.469664186585207</v>
       </c>
-      <c r="K24" s="2" t="n">
+      <c r="L24" s="2" t="n">
         <v>0.0083181625092688</v>
       </c>
-      <c r="L24" s="2" t="n">
+      <c r="M24" s="2" t="n">
         <v>2.02383834605996</v>
-      </c>
-      <c r="M24" s="2" t="n">
-        <v>4.83921510655197</v>
       </c>
       <c r="N24" s="2" t="n">
         <v>4291.26</v>
@@ -26733,16 +26639,16 @@
         <v>124</v>
       </c>
       <c r="R24" s="2" t="n">
+        <v>5.79392894754167</v>
+      </c>
+      <c r="S24" s="2" t="n">
         <v>0.555308152273156</v>
       </c>
-      <c r="S24" s="2" t="n">
+      <c r="T24" s="2" t="n">
         <v>0.0239942955300447</v>
       </c>
-      <c r="T24" s="2" t="n">
+      <c r="U24" s="2" t="n">
         <v>2.02162093489613</v>
-      </c>
-      <c r="U24" s="2" t="n">
-        <v>5.79392894754167</v>
       </c>
       <c r="V24" s="2" t="n">
         <v>1049.83</v>
@@ -26751,16 +26657,16 @@
         <v>124</v>
       </c>
       <c r="Y24" s="2" t="n">
+        <v>4.75295112455731</v>
+      </c>
+      <c r="Z24" s="2" t="n">
         <v>0.491596896089408</v>
       </c>
-      <c r="Z24" s="2" t="n">
+      <c r="AA24" s="2" t="n">
         <v>0.0129265590049605</v>
       </c>
-      <c r="AA24" s="2" t="n">
+      <c r="AB24" s="2" t="n">
         <v>2.02249915173666</v>
-      </c>
-      <c r="AB24" s="2" t="n">
-        <v>4.75295112455731</v>
       </c>
       <c r="AC24" s="2" t="n">
         <v>430.85</v>
@@ -26771,16 +26677,16 @@
         <v>125</v>
       </c>
       <c r="B25" s="2" t="n">
+        <v>4.74077023018602</v>
+      </c>
+      <c r="C25" s="2" t="n">
         <v>0.489806441724872</v>
       </c>
-      <c r="C25" s="2" t="n">
+      <c r="D25" s="2" t="n">
         <v>0.0123675024655646</v>
       </c>
-      <c r="D25" s="2" t="n">
+      <c r="E25" s="2" t="n">
         <v>2.0226003735816</v>
-      </c>
-      <c r="E25" s="2" t="n">
-        <v>4.74077023018602</v>
       </c>
       <c r="F25" s="2" t="n">
         <v>2265.93</v>
@@ -26789,16 +26695,16 @@
         <v>125</v>
       </c>
       <c r="J25" s="2" t="n">
+        <v>4.73258144253468</v>
+      </c>
+      <c r="K25" s="2" t="n">
         <v>0.485378310158194</v>
       </c>
-      <c r="K25" s="2" t="n">
+      <c r="L25" s="2" t="n">
         <v>0.0114412614119393</v>
       </c>
-      <c r="L25" s="2" t="n">
+      <c r="M25" s="2" t="n">
         <v>2.02289234955163</v>
-      </c>
-      <c r="M25" s="2" t="n">
-        <v>4.73258144253468</v>
       </c>
       <c r="N25" s="2" t="n">
         <v>4482.82</v>
@@ -26807,16 +26713,16 @@
         <v>125</v>
       </c>
       <c r="R25" s="2" t="n">
+        <v>14.5864054153343</v>
+      </c>
+      <c r="S25" s="2" t="n">
         <v>0.766995285607553</v>
       </c>
-      <c r="S25" s="2" t="n">
+      <c r="T25" s="2" t="n">
         <v>0.0961933523526666</v>
       </c>
-      <c r="T25" s="2" t="n">
+      <c r="U25" s="2" t="n">
         <v>2.01266208930023</v>
-      </c>
-      <c r="U25" s="2" t="n">
-        <v>14.5864054153343</v>
       </c>
       <c r="V25" s="2" t="n">
         <v>1099.35</v>
@@ -26825,16 +26731,16 @@
         <v>125</v>
       </c>
       <c r="Y25" s="2" t="n">
+        <v>5.79493054981968</v>
+      </c>
+      <c r="Z25" s="2" t="n">
         <v>0.552679315673452</v>
       </c>
-      <c r="Z25" s="2" t="n">
+      <c r="AA25" s="2" t="n">
         <v>0.0257898341104866</v>
       </c>
-      <c r="AA25" s="2" t="n">
+      <c r="AB25" s="2" t="n">
         <v>2.02039586868464</v>
-      </c>
-      <c r="AB25" s="2" t="n">
-        <v>5.79493054981968</v>
       </c>
       <c r="AC25" s="2" t="n">
         <v>449.73</v>
@@ -26845,16 +26751,16 @@
         <v>126</v>
       </c>
       <c r="B26" s="2" t="n">
+        <v>4.73324406483686</v>
+      </c>
+      <c r="C26" s="2" t="n">
         <v>0.485726345949523</v>
       </c>
-      <c r="C26" s="2" t="n">
+      <c r="D26" s="2" t="n">
         <v>0.0116259150426616</v>
       </c>
-      <c r="D26" s="2" t="n">
+      <c r="E26" s="2" t="n">
         <v>2.02270430880762</v>
-      </c>
-      <c r="E26" s="2" t="n">
-        <v>4.73324406483686</v>
       </c>
       <c r="F26" s="2" t="n">
         <v>2365.77</v>
@@ -26863,16 +26769,16 @@
         <v>126</v>
       </c>
       <c r="J26" s="2" t="n">
+        <v>4.73297046133708</v>
+      </c>
+      <c r="K26" s="2" t="n">
         <v>0.48568067262847</v>
       </c>
-      <c r="K26" s="2" t="n">
+      <c r="L26" s="2" t="n">
         <v>0.0115256045417603</v>
       </c>
-      <c r="L26" s="2" t="n">
+      <c r="M26" s="2" t="n">
         <v>2.02288651364477</v>
-      </c>
-      <c r="M26" s="2" t="n">
-        <v>4.73297046133708</v>
       </c>
       <c r="N26" s="2" t="n">
         <v>4668.56</v>
@@ -26881,16 +26787,16 @@
         <v>126</v>
       </c>
       <c r="R26" s="2" t="n">
+        <v>5.02478243838729</v>
+      </c>
+      <c r="S26" s="2" t="n">
         <v>0.463375459734602</v>
       </c>
-      <c r="S26" s="2" t="n">
+      <c r="T26" s="2" t="n">
         <v>0.00674916970178051</v>
       </c>
-      <c r="T26" s="2" t="n">
+      <c r="U26" s="2" t="n">
         <v>2.02465660221152</v>
-      </c>
-      <c r="U26" s="2" t="n">
-        <v>5.02478243838729</v>
       </c>
       <c r="V26" s="2" t="n">
         <v>1151.84</v>
@@ -26899,16 +26805,16 @@
         <v>126</v>
       </c>
       <c r="Y26" s="2" t="n">
+        <v>5.00942022103225</v>
+      </c>
+      <c r="Z26" s="2" t="n">
         <v>0.517117055651651</v>
       </c>
-      <c r="Z26" s="2" t="n">
+      <c r="AA26" s="2" t="n">
         <v>0.0175787935517858</v>
       </c>
-      <c r="AA26" s="2" t="n">
+      <c r="AB26" s="2" t="n">
         <v>2.02182923249266</v>
-      </c>
-      <c r="AB26" s="2" t="n">
-        <v>5.00942022103225</v>
       </c>
       <c r="AC26" s="2" t="n">
         <v>469.289999999999</v>
@@ -26919,16 +26825,16 @@
         <v>127</v>
       </c>
       <c r="B27" s="2" t="n">
+        <v>4.73264681850242</v>
+      </c>
+      <c r="C27" s="2" t="n">
         <v>0.484773766799881</v>
       </c>
-      <c r="C27" s="2" t="n">
+      <c r="D27" s="2" t="n">
         <v>0.011396574020999</v>
       </c>
-      <c r="D27" s="2" t="n">
+      <c r="E27" s="2" t="n">
         <v>2.02288556575111</v>
-      </c>
-      <c r="E27" s="2" t="n">
-        <v>4.73264681850242</v>
       </c>
       <c r="F27" s="2" t="n">
         <v>2460.03</v>
@@ -26937,16 +26843,16 @@
         <v>127</v>
       </c>
       <c r="J27" s="2" t="n">
+        <v>4.73333615333202</v>
+      </c>
+      <c r="K27" s="2" t="n">
         <v>0.486125326235334</v>
       </c>
-      <c r="K27" s="2" t="n">
+      <c r="L27" s="2" t="n">
         <v>0.0116741122706659</v>
       </c>
-      <c r="L27" s="2" t="n">
+      <c r="M27" s="2" t="n">
         <v>2.02281552024105</v>
-      </c>
-      <c r="M27" s="2" t="n">
-        <v>4.73333615333202</v>
       </c>
       <c r="N27" s="2" t="n">
         <v>4867.8</v>
@@ -26955,16 +26861,16 @@
         <v>127</v>
       </c>
       <c r="R27" s="2" t="n">
+        <v>13.98904397094</v>
+      </c>
+      <c r="S27" s="2" t="n">
         <v>0.763619639914303</v>
       </c>
-      <c r="S27" s="2" t="n">
+      <c r="T27" s="2" t="n">
         <v>0.0920100943790351</v>
       </c>
-      <c r="T27" s="2" t="n">
+      <c r="U27" s="2" t="n">
         <v>2.01332784278771</v>
-      </c>
-      <c r="U27" s="2" t="n">
-        <v>13.98904397094</v>
       </c>
       <c r="V27" s="2" t="n">
         <v>1201.69</v>
@@ -26973,16 +26879,16 @@
         <v>127</v>
       </c>
       <c r="Y27" s="2" t="n">
+        <v>4.73365937265043</v>
+      </c>
+      <c r="Z27" s="2" t="n">
         <v>0.483673565939086</v>
       </c>
-      <c r="Z27" s="2" t="n">
+      <c r="AA27" s="2" t="n">
         <v>0.0111067789602397</v>
       </c>
-      <c r="AA27" s="2" t="n">
+      <c r="AB27" s="2" t="n">
         <v>2.02299936744483</v>
-      </c>
-      <c r="AB27" s="2" t="n">
-        <v>4.73365937265043</v>
       </c>
       <c r="AC27" s="2" t="n">
         <v>489.35</v>
@@ -26993,16 +26899,16 @@
         <v>128</v>
       </c>
       <c r="B28" s="2" t="n">
+        <v>4.74092073533195</v>
+      </c>
+      <c r="C28" s="2" t="n">
         <v>0.480295855115685</v>
       </c>
-      <c r="C28" s="2" t="n">
+      <c r="D28" s="2" t="n">
         <v>0.0104586142218422</v>
       </c>
-      <c r="D28" s="2" t="n">
+      <c r="E28" s="2" t="n">
         <v>2.02313091663461</v>
-      </c>
-      <c r="E28" s="2" t="n">
-        <v>4.74092073533195</v>
       </c>
       <c r="F28" s="2" t="n">
         <v>2553.17</v>
@@ -27011,16 +26917,16 @@
         <v>128</v>
       </c>
       <c r="J28" s="2" t="n">
+        <v>4.73617492678719</v>
+      </c>
+      <c r="K28" s="2" t="n">
         <v>0.487942072183846</v>
       </c>
-      <c r="K28" s="2" t="n">
+      <c r="L28" s="2" t="n">
         <v>0.0120623962489738</v>
       </c>
-      <c r="L28" s="2" t="n">
+      <c r="M28" s="2" t="n">
         <v>2.02267222431049</v>
-      </c>
-      <c r="M28" s="2" t="n">
-        <v>4.73617492678719</v>
       </c>
       <c r="N28" s="2" t="n">
         <v>5061.42</v>
@@ -27029,16 +26935,16 @@
         <v>128</v>
       </c>
       <c r="R28" s="2" t="n">
+        <v>5.80647672017915</v>
+      </c>
+      <c r="S28" s="2" t="n">
         <v>0.535307628931789</v>
       </c>
-      <c r="S28" s="2" t="n">
+      <c r="T28" s="2" t="n">
         <v>0.0249516928823957</v>
       </c>
-      <c r="T28" s="2" t="n">
+      <c r="U28" s="2" t="n">
         <v>2.01933193331388</v>
-      </c>
-      <c r="U28" s="2" t="n">
-        <v>5.80647672017915</v>
       </c>
       <c r="V28" s="2" t="n">
         <v>1248.62</v>
@@ -27047,16 +26953,16 @@
         <v>128</v>
       </c>
       <c r="Y28" s="2" t="n">
+        <v>4.99188121808989</v>
+      </c>
+      <c r="Z28" s="2" t="n">
         <v>0.51621370105816</v>
       </c>
-      <c r="Z28" s="2" t="n">
+      <c r="AA28" s="2" t="n">
         <v>0.0171909710769401</v>
       </c>
-      <c r="AA28" s="2" t="n">
+      <c r="AB28" s="2" t="n">
         <v>2.02205879088233</v>
-      </c>
-      <c r="AB28" s="2" t="n">
-        <v>4.99188121808989</v>
       </c>
       <c r="AC28" s="2" t="n">
         <v>509.4</v>
@@ -27067,16 +26973,16 @@
         <v>129</v>
       </c>
       <c r="B29" s="2" t="n">
+        <v>4.73449635107517</v>
+      </c>
+      <c r="C29" s="2" t="n">
         <v>0.486680336522834</v>
       </c>
-      <c r="C29" s="2" t="n">
+      <c r="D29" s="2" t="n">
         <v>0.0118370228419102</v>
       </c>
-      <c r="D29" s="2" t="n">
+      <c r="E29" s="2" t="n">
         <v>2.02269567770149</v>
-      </c>
-      <c r="E29" s="2" t="n">
-        <v>4.73449635107517</v>
       </c>
       <c r="F29" s="2" t="n">
         <v>2645.86</v>
@@ -27085,16 +26991,16 @@
         <v>129</v>
       </c>
       <c r="J29" s="2" t="n">
+        <v>4.7412878728931</v>
+      </c>
+      <c r="K29" s="2" t="n">
         <v>0.489500503965415</v>
       </c>
-      <c r="K29" s="2" t="n">
+      <c r="L29" s="2" t="n">
         <v>0.0123967756173097</v>
       </c>
-      <c r="L29" s="2" t="n">
+      <c r="M29" s="2" t="n">
         <v>2.0226239150409</v>
-      </c>
-      <c r="M29" s="2" t="n">
-        <v>4.7412878728931</v>
       </c>
       <c r="N29" s="2" t="n">
         <v>5254.36</v>
@@ -27103,16 +27009,16 @@
         <v>129</v>
       </c>
       <c r="R29" s="2" t="n">
+        <v>5.19172872965442</v>
+      </c>
+      <c r="S29" s="2" t="n">
         <v>0.519151033991847</v>
       </c>
-      <c r="S29" s="2" t="n">
+      <c r="T29" s="2" t="n">
         <v>0.0197758268825193</v>
       </c>
-      <c r="T29" s="2" t="n">
+      <c r="U29" s="2" t="n">
         <v>2.02069997880961</v>
-      </c>
-      <c r="U29" s="2" t="n">
-        <v>5.19172872965442</v>
       </c>
       <c r="V29" s="2" t="n">
         <v>1291.8</v>
@@ -27121,16 +27027,16 @@
         <v>129</v>
       </c>
       <c r="Y29" s="2" t="n">
+        <v>4.73910454348866</v>
+      </c>
+      <c r="Z29" s="2" t="n">
         <v>0.488627287987745</v>
       </c>
-      <c r="Z29" s="2" t="n">
+      <c r="AA29" s="2" t="n">
         <v>0.012247400967034</v>
       </c>
-      <c r="AA29" s="2" t="n">
+      <c r="AB29" s="2" t="n">
         <v>2.02262960575295</v>
-      </c>
-      <c r="AB29" s="2" t="n">
-        <v>4.73910454348866</v>
       </c>
       <c r="AC29" s="2" t="n">
         <v>529.93</v>
@@ -27141,16 +27047,16 @@
         <v>130</v>
       </c>
       <c r="B30" s="2" t="n">
+        <v>4.73379934517056</v>
+      </c>
+      <c r="C30" s="2" t="n">
         <v>0.482953623448318</v>
       </c>
-      <c r="C30" s="2" t="n">
+      <c r="D30" s="2" t="n">
         <v>0.0110631897345459</v>
       </c>
-      <c r="D30" s="2" t="n">
+      <c r="E30" s="2" t="n">
         <v>2.02297437402652</v>
-      </c>
-      <c r="E30" s="2" t="n">
-        <v>4.73379934517056</v>
       </c>
       <c r="F30" s="2" t="n">
         <v>2738.61</v>
@@ -27159,16 +27065,16 @@
         <v>130</v>
       </c>
       <c r="J30" s="2" t="n">
+        <v>4.73271698603789</v>
+      </c>
+      <c r="K30" s="2" t="n">
         <v>0.485055177965332</v>
       </c>
-      <c r="K30" s="2" t="n">
+      <c r="L30" s="2" t="n">
         <v>0.0114707863057356</v>
       </c>
-      <c r="L30" s="2" t="n">
+      <c r="M30" s="2" t="n">
         <v>2.02285745534938</v>
-      </c>
-      <c r="M30" s="2" t="n">
-        <v>4.73271698603789</v>
       </c>
       <c r="N30" s="2" t="n">
         <v>5446.92</v>
@@ -27177,16 +27083,16 @@
         <v>130</v>
       </c>
       <c r="R30" s="2" t="n">
+        <v>10.4142054699306</v>
+      </c>
+      <c r="S30" s="2" t="n">
         <v>0.521703161691092</v>
       </c>
-      <c r="S30" s="2" t="n">
+      <c r="T30" s="2" t="n">
         <v>0.00451780384737546</v>
       </c>
-      <c r="T30" s="2" t="n">
+      <c r="U30" s="2" t="n">
         <v>2.03293730079954</v>
-      </c>
-      <c r="U30" s="2" t="n">
-        <v>10.4142054699306</v>
       </c>
       <c r="V30" s="2" t="n">
         <v>1341.08</v>
@@ -27195,16 +27101,16 @@
         <v>130</v>
       </c>
       <c r="Y30" s="2" t="n">
+        <v>5.54636459222882</v>
+      </c>
+      <c r="Z30" s="2" t="n">
         <v>0.450301525598511</v>
       </c>
-      <c r="Z30" s="2" t="n">
+      <c r="AA30" s="2" t="n">
         <v>0.00439832399308458</v>
       </c>
-      <c r="AA30" s="2" t="n">
+      <c r="AB30" s="2" t="n">
         <v>2.02623292995681</v>
-      </c>
-      <c r="AB30" s="2" t="n">
-        <v>5.54636459222882</v>
       </c>
       <c r="AC30" s="2" t="n">
         <v>548.75</v>
@@ -27215,16 +27121,16 @@
         <v>131</v>
       </c>
       <c r="B31" s="2" t="n">
+        <v>4.73297207839648</v>
+      </c>
+      <c r="C31" s="2" t="n">
         <v>0.485639831322016</v>
       </c>
-      <c r="C31" s="2" t="n">
+      <c r="D31" s="2" t="n">
         <v>0.0115843482428836</v>
       </c>
-      <c r="D31" s="2" t="n">
+      <c r="E31" s="2" t="n">
         <v>2.02283240445411</v>
-      </c>
-      <c r="E31" s="2" t="n">
-        <v>4.73297207839648</v>
       </c>
       <c r="F31" s="2" t="n">
         <v>2833.84</v>
@@ -27233,16 +27139,16 @@
         <v>131</v>
       </c>
       <c r="J31" s="2" t="n">
+        <v>4.76321502114731</v>
+      </c>
+      <c r="K31" s="2" t="n">
         <v>0.476441730908921</v>
       </c>
-      <c r="K31" s="2" t="n">
+      <c r="L31" s="2" t="n">
         <v>0.00966693539404089</v>
       </c>
-      <c r="L31" s="2" t="n">
+      <c r="M31" s="2" t="n">
         <v>2.02338793186904</v>
-      </c>
-      <c r="M31" s="2" t="n">
-        <v>4.76321502114731</v>
       </c>
       <c r="N31" s="2" t="n">
         <v>5633.46</v>
@@ -27251,16 +27157,16 @@
         <v>131</v>
       </c>
       <c r="R31" s="2" t="n">
+        <v>7.23738434138332</v>
+      </c>
+      <c r="S31" s="2" t="n">
         <v>0.563485655514734</v>
       </c>
-      <c r="S31" s="2" t="n">
+      <c r="T31" s="2" t="n">
         <v>0.0345598346150393</v>
       </c>
-      <c r="T31" s="2" t="n">
+      <c r="U31" s="2" t="n">
         <v>2.01727669965836</v>
-      </c>
-      <c r="U31" s="2" t="n">
-        <v>7.23738434138332</v>
       </c>
       <c r="V31" s="2" t="n">
         <v>1391.8</v>
@@ -27269,16 +27175,16 @@
         <v>131</v>
       </c>
       <c r="Y31" s="2" t="n">
+        <v>8.71009886078587</v>
+      </c>
+      <c r="Z31" s="2" t="n">
         <v>0.628011529441782</v>
       </c>
-      <c r="Z31" s="2" t="n">
+      <c r="AA31" s="2" t="n">
         <v>0.0485381822999904</v>
       </c>
-      <c r="AA31" s="2" t="n">
+      <c r="AB31" s="2" t="n">
         <v>2.01471658138896</v>
-      </c>
-      <c r="AB31" s="2" t="n">
-        <v>8.71009886078587</v>
       </c>
       <c r="AC31" s="2" t="n">
         <v>567.440000000001</v>
@@ -27289,16 +27195,16 @@
         <v>132</v>
       </c>
       <c r="B32" s="2" t="n">
+        <v>4.73772845282572</v>
+      </c>
+      <c r="C32" s="2" t="n">
         <v>0.48847252756799</v>
       </c>
-      <c r="C32" s="2" t="n">
+      <c r="D32" s="2" t="n">
         <v>0.0121601160878525</v>
       </c>
-      <c r="D32" s="2" t="n">
+      <c r="E32" s="2" t="n">
         <v>2.02269325556195</v>
-      </c>
-      <c r="E32" s="2" t="n">
-        <v>4.73772845282572</v>
       </c>
       <c r="F32" s="2" t="n">
         <v>2942.52</v>
@@ -27307,16 +27213,16 @@
         <v>132</v>
       </c>
       <c r="J32" s="2" t="n">
+        <v>4.75586731408389</v>
+      </c>
+      <c r="K32" s="2" t="n">
         <v>0.492406089094184</v>
       </c>
-      <c r="K32" s="2" t="n">
+      <c r="L32" s="2" t="n">
         <v>0.0130653479416265</v>
       </c>
-      <c r="L32" s="2" t="n">
+      <c r="M32" s="2" t="n">
         <v>2.02241876561011</v>
-      </c>
-      <c r="M32" s="2" t="n">
-        <v>4.75586731408389</v>
       </c>
       <c r="N32" s="2" t="n">
         <v>5819.25</v>
@@ -27325,16 +27231,16 @@
         <v>132</v>
       </c>
       <c r="R32" s="2" t="n">
+        <v>6.79126082662106</v>
+      </c>
+      <c r="S32" s="2" t="n">
         <v>0.587057909370176</v>
       </c>
-      <c r="S32" s="2" t="n">
+      <c r="T32" s="2" t="n">
         <v>0.0338481485476043</v>
       </c>
-      <c r="T32" s="2" t="n">
+      <c r="U32" s="2" t="n">
         <v>2.01945480387697</v>
-      </c>
-      <c r="U32" s="2" t="n">
-        <v>6.79126082662106</v>
       </c>
       <c r="V32" s="2" t="n">
         <v>1438.69</v>
@@ -27343,16 +27249,16 @@
         <v>132</v>
       </c>
       <c r="Y32" s="2" t="n">
+        <v>5.29161793897107</v>
+      </c>
+      <c r="Z32" s="2" t="n">
         <v>0.532915414088237</v>
       </c>
-      <c r="Z32" s="2" t="n">
+      <c r="AA32" s="2" t="n">
         <v>0.0200434216808821</v>
       </c>
-      <c r="AA32" s="2" t="n">
+      <c r="AB32" s="2" t="n">
         <v>2.02112866865988</v>
-      </c>
-      <c r="AB32" s="2" t="n">
-        <v>5.29161793897107</v>
       </c>
       <c r="AC32" s="2" t="n">
         <v>586.110000000001</v>
@@ -27370,33 +27276,33 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K12" activeCellId="1" sqref="B2:F31 K12"/>
+      <selection pane="topLeft" activeCell="M15" activeCellId="0" sqref="M15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.15625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="6.1640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>101</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>140</v>
@@ -27405,16 +27311,16 @@
         <v>101</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>140</v>
@@ -27422,10 +27328,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="2" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28580,75 +28486,78 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AC32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B2:F31 A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.71"/>
+  </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>140</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>139</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>140</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>139</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>140</v>
       </c>
       <c r="Y1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>139</v>
       </c>
       <c r="AC1" s="1" t="s">
         <v>140</v>
@@ -28658,40 +28567,25 @@
       <c r="A2" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B2" s="2" t="n">
-        <v>6.93028632450325</v>
-      </c>
-      <c r="C2" s="2" t="n">
-        <v>0.524859554787541</v>
-      </c>
-      <c r="D2" s="2" t="n">
-        <v>0.0289444141627922</v>
-      </c>
-      <c r="E2" s="2" t="n">
-        <v>2.01543621076715</v>
-      </c>
-      <c r="F2" s="2" t="n">
-        <v>268.29</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>103</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>7.12145951023274</v>
+        <v>6.93028632450325</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>0.546171004730499</v>
+        <v>0.524859554787541</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>0.0319548169907672</v>
+        <v>0.0289444141627922</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>2.01076862756348</v>
+        <v>2.01543621076715</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>383.48</v>
+        <v>268.29</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28699,19 +28593,19 @@
         <v>104</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>8.06585750737078</v>
+        <v>7.12145951023274</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>0.584556993835105</v>
+        <v>0.546171004730499</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>0.0440314894255499</v>
+        <v>0.0319548169907672</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>2.01371873141363</v>
+        <v>2.01076862756348</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>276.33</v>
+        <v>383.48</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28719,19 +28613,19 @@
         <v>105</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>6.13686366876309</v>
+        <v>8.06585750737078</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>0.488253836088191</v>
+        <v>0.584556993835105</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>0.0189523996697701</v>
+        <v>0.0440314894255499</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>2.01361917597072</v>
+        <v>2.01371873141363</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>336.56</v>
+        <v>276.33</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28739,19 +28633,19 @@
         <v>106</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>7.01200286082769</v>
+        <v>6.13686366876309</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>0.532498716372549</v>
+        <v>0.488253836088191</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>0.0301691284947793</v>
+        <v>0.0189523996697701</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>2.01607813154779</v>
+        <v>2.01361917597072</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>331.54</v>
+        <v>336.56</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28759,19 +28653,19 @@
         <v>107</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>6.13923710658133</v>
+        <v>7.01200286082769</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>0.473252886835473</v>
+        <v>0.532498716372549</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>0.0151266721448187</v>
+        <v>0.0301691284947793</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>2.0162567894857</v>
+        <v>2.01607813154779</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>269.35</v>
+        <v>331.54</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28779,19 +28673,19 @@
         <v>108</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>8.36563289055019</v>
+        <v>6.13923710658133</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>0.598373817612299</v>
+        <v>0.473252886835473</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>0.0471818294780156</v>
+        <v>0.0151266721448187</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>2.01405121829215</v>
+        <v>2.0162567894857</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>282.77</v>
+        <v>269.35</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28799,19 +28693,19 @@
         <v>109</v>
       </c>
       <c r="B9" s="2" t="n">
-        <v>11.0317934017224</v>
+        <v>8.36563289055019</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>0.5</v>
+        <v>0.598373817612299</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>0.03</v>
+        <v>0.0471818294780156</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>2</v>
+        <v>2.01405121829215</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>232.46</v>
+        <v>282.77</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28819,19 +28713,19 @@
         <v>110</v>
       </c>
       <c r="B10" s="2" t="n">
-        <v>6.35839907625018</v>
+        <v>11.0317934017224</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>0.480848385910513</v>
+        <v>0.5</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>0.0159647606559745</v>
+        <v>0.03</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>2.01772698056421</v>
+        <v>2</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>435.619999999999</v>
+        <v>232.46</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28839,19 +28733,19 @@
         <v>111</v>
       </c>
       <c r="B11" s="2" t="n">
-        <v>6.64601194394861</v>
+        <v>6.35839907625018</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>0.518332659762903</v>
+        <v>0.480848385910513</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>0.0268100209948945</v>
+        <v>0.0159647606559745</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>2.01419803427063</v>
+        <v>2.01772698056421</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>528.96</v>
+        <v>435.619999999999</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28859,19 +28753,19 @@
         <v>112</v>
       </c>
       <c r="B12" s="2" t="n">
-        <v>10.7570517164249</v>
+        <v>6.64601194394861</v>
       </c>
       <c r="C12" s="2" t="n">
-        <v>0.511745157023533</v>
+        <v>0.518332659762903</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>0.0327405366388244</v>
+        <v>0.0268100209948945</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>1.99459539159636</v>
+        <v>2.01419803427063</v>
       </c>
       <c r="F12" s="2" t="n">
-        <v>324.97</v>
+        <v>528.96</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28879,19 +28773,19 @@
         <v>113</v>
       </c>
       <c r="B13" s="2" t="n">
-        <v>9.62101798446815</v>
+        <v>10.7570517164249</v>
       </c>
       <c r="C13" s="2" t="n">
-        <v>0.6459200128464</v>
+        <v>0.511745157023533</v>
       </c>
       <c r="D13" s="2" t="n">
-        <v>0.0645946950589519</v>
+        <v>0.0327405366388244</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>2.0111643680606</v>
+        <v>1.99459539159636</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>385.21</v>
+        <v>324.97</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28899,19 +28793,19 @@
         <v>114</v>
       </c>
       <c r="B14" s="2" t="n">
-        <v>6.89052685064197</v>
+        <v>9.62101798446815</v>
       </c>
       <c r="C14" s="2" t="n">
-        <v>0.535147844947261</v>
+        <v>0.6459200128464</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>0.0310224593277019</v>
+        <v>0.0645946950589519</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>2.01455193720292</v>
+        <v>2.0111643680606</v>
       </c>
       <c r="F14" s="2" t="n">
-        <v>584.91</v>
+        <v>385.21</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28919,19 +28813,19 @@
         <v>115</v>
       </c>
       <c r="B15" s="2" t="n">
-        <v>7.32125720900175</v>
+        <v>6.89052685064197</v>
       </c>
       <c r="C15" s="2" t="n">
-        <v>0.557150517356331</v>
+        <v>0.535147844947261</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>0.0385399551307968</v>
+        <v>0.0310224593277019</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>2.01113203569632</v>
+        <v>2.01455193720292</v>
       </c>
       <c r="F15" s="2" t="n">
-        <v>431.780000000001</v>
+        <v>584.91</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28939,19 +28833,19 @@
         <v>116</v>
       </c>
       <c r="B16" s="2" t="n">
-        <v>6.65373593151003</v>
+        <v>7.32125720900175</v>
       </c>
       <c r="C16" s="2" t="n">
-        <v>0.513321748253538</v>
+        <v>0.557150517356331</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>0.023985448211857</v>
+        <v>0.0385399551307968</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>2.01042075458442</v>
+        <v>2.01113203569632</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>455.75</v>
+        <v>431.780000000001</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28959,19 +28853,19 @@
         <v>117</v>
       </c>
       <c r="B17" s="2" t="n">
-        <v>6.53950163359604</v>
+        <v>6.65373593151003</v>
       </c>
       <c r="C17" s="2" t="n">
-        <v>0.502996513092871</v>
+        <v>0.513321748253538</v>
       </c>
       <c r="D17" s="2" t="n">
-        <v>0.020866748124223</v>
+        <v>0.023985448211857</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>2.01412601171575</v>
+        <v>2.01042075458442</v>
       </c>
       <c r="F17" s="2" t="n">
-        <v>386.839999999999</v>
+        <v>455.75</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28979,19 +28873,19 @@
         <v>118</v>
       </c>
       <c r="B18" s="2" t="n">
-        <v>7.13126607639065</v>
+        <v>6.53950163359604</v>
       </c>
       <c r="C18" s="2" t="n">
-        <v>0.543014231235991</v>
+        <v>0.502996513092871</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>0.0328599150760521</v>
+        <v>0.020866748124223</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>2.01810073919145</v>
+        <v>2.01412601171575</v>
       </c>
       <c r="F18" s="2" t="n">
-        <v>470.43</v>
+        <v>386.839999999999</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28999,19 +28893,19 @@
         <v>119</v>
       </c>
       <c r="B19" s="2" t="n">
-        <v>8.62388826583393</v>
+        <v>7.13126607639065</v>
       </c>
       <c r="C19" s="2" t="n">
-        <v>0.607429528400724</v>
+        <v>0.543014231235991</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>0.051176100886292</v>
+        <v>0.0328599150760521</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>2.01335433027284</v>
+        <v>2.01810073919145</v>
       </c>
       <c r="F19" s="2" t="n">
-        <v>493.219999999999</v>
+        <v>470.43</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29019,19 +28913,19 @@
         <v>120</v>
       </c>
       <c r="B20" s="2" t="n">
-        <v>6.98376251834528</v>
+        <v>8.62388826583393</v>
       </c>
       <c r="C20" s="2" t="n">
-        <v>0.532848003333</v>
+        <v>0.607429528400724</v>
       </c>
       <c r="D20" s="2" t="n">
-        <v>0.029399659128075</v>
+        <v>0.051176100886292</v>
       </c>
       <c r="E20" s="2" t="n">
-        <v>2.01383868377864</v>
+        <v>2.01335433027284</v>
       </c>
       <c r="F20" s="2" t="n">
-        <v>619.790000000001</v>
+        <v>493.219999999999</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29039,19 +28933,19 @@
         <v>121</v>
       </c>
       <c r="B21" s="2" t="n">
-        <v>6.23430366722677</v>
+        <v>6.98376251834528</v>
       </c>
       <c r="C21" s="2" t="n">
-        <v>0.470928237391508</v>
+        <v>0.532848003333</v>
       </c>
       <c r="D21" s="2" t="n">
-        <v>0.0140110846484889</v>
+        <v>0.029399659128075</v>
       </c>
       <c r="E21" s="2" t="n">
-        <v>2.01523370332756</v>
+        <v>2.01383868377864</v>
       </c>
       <c r="F21" s="2" t="n">
-        <v>582.01</v>
+        <v>619.790000000001</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29059,19 +28953,19 @@
         <v>122</v>
       </c>
       <c r="B22" s="2" t="n">
-        <v>7.62008021546003</v>
+        <v>6.23430366722677</v>
       </c>
       <c r="C22" s="2" t="n">
-        <v>0.567415222531485</v>
+        <v>0.470928237391508</v>
       </c>
       <c r="D22" s="2" t="n">
-        <v>0.0394120948737954</v>
+        <v>0.0140110846484889</v>
       </c>
       <c r="E22" s="2" t="n">
-        <v>2.01589216699744</v>
+        <v>2.01523370332756</v>
       </c>
       <c r="F22" s="2" t="n">
-        <v>815.4</v>
+        <v>582.01</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29079,19 +28973,19 @@
         <v>123</v>
       </c>
       <c r="B23" s="2" t="n">
-        <v>7.84092468974464</v>
+        <v>7.62008021546003</v>
       </c>
       <c r="C23" s="2" t="n">
-        <v>0.572652843368219</v>
+        <v>0.567415222531485</v>
       </c>
       <c r="D23" s="2" t="n">
-        <v>0.0422298293307148</v>
+        <v>0.0394120948737954</v>
       </c>
       <c r="E23" s="2" t="n">
-        <v>2.01192219614761</v>
+        <v>2.01589216699744</v>
       </c>
       <c r="F23" s="2" t="n">
-        <v>603.93</v>
+        <v>815.4</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29099,19 +28993,19 @@
         <v>124</v>
       </c>
       <c r="B24" s="2" t="n">
-        <v>7.82759356560142</v>
+        <v>7.84092468974464</v>
       </c>
       <c r="C24" s="2" t="n">
-        <v>0.573636997213633</v>
+        <v>0.572652843368219</v>
       </c>
       <c r="D24" s="2" t="n">
-        <v>0.0416752157118297</v>
+        <v>0.0422298293307148</v>
       </c>
       <c r="E24" s="2" t="n">
-        <v>2.00659590334396</v>
+        <v>2.01192219614761</v>
       </c>
       <c r="F24" s="2" t="n">
-        <v>623.049999999999</v>
+        <v>603.93</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29119,19 +29013,19 @@
         <v>125</v>
       </c>
       <c r="B25" s="2" t="n">
-        <v>7.69105606485592</v>
+        <v>7.82759356560142</v>
       </c>
       <c r="C25" s="2" t="n">
-        <v>0.567267151862527</v>
+        <v>0.573636997213633</v>
       </c>
       <c r="D25" s="2" t="n">
-        <v>0.0395108618495128</v>
+        <v>0.0416752157118297</v>
       </c>
       <c r="E25" s="2" t="n">
-        <v>2.01412792590296</v>
+        <v>2.00659590334396</v>
       </c>
       <c r="F25" s="2" t="n">
-        <v>762.23</v>
+        <v>623.049999999999</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29139,19 +29033,19 @@
         <v>126</v>
       </c>
       <c r="B26" s="2" t="n">
-        <v>7.99207528977856</v>
+        <v>7.69105606485592</v>
       </c>
       <c r="C26" s="2" t="n">
-        <v>0.580119287898651</v>
+        <v>0.567267151862527</v>
       </c>
       <c r="D26" s="2" t="n">
-        <v>0.0434199507308901</v>
+        <v>0.0395108618495128</v>
       </c>
       <c r="E26" s="2" t="n">
-        <v>2.01344266134737</v>
+        <v>2.01412792590296</v>
       </c>
       <c r="F26" s="2" t="n">
-        <v>780.01</v>
+        <v>762.23</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29159,19 +29053,19 @@
         <v>127</v>
       </c>
       <c r="B27" s="2" t="n">
-        <v>7.50286278469249</v>
+        <v>7.99207528977856</v>
       </c>
       <c r="C27" s="2" t="n">
-        <v>0.559657009834094</v>
+        <v>0.580119287898651</v>
       </c>
       <c r="D27" s="2" t="n">
-        <v>0.0376280562921721</v>
+        <v>0.0434199507308901</v>
       </c>
       <c r="E27" s="2" t="n">
-        <v>2.01420578737007</v>
+        <v>2.01344266134737</v>
       </c>
       <c r="F27" s="2" t="n">
-        <v>562.110000000001</v>
+        <v>780.01</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29179,19 +29073,19 @@
         <v>128</v>
       </c>
       <c r="B28" s="2" t="n">
-        <v>6.84853066747513</v>
+        <v>7.50286278469249</v>
       </c>
       <c r="C28" s="2" t="n">
-        <v>0.519320810726022</v>
+        <v>0.559657009834094</v>
       </c>
       <c r="D28" s="2" t="n">
-        <v>0.0274388617373422</v>
+        <v>0.0376280562921721</v>
       </c>
       <c r="E28" s="2" t="n">
-        <v>2.01550649489432</v>
+        <v>2.01420578737007</v>
       </c>
       <c r="F28" s="2" t="n">
-        <v>526.57</v>
+        <v>562.110000000001</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29199,19 +29093,19 @@
         <v>129</v>
       </c>
       <c r="B29" s="2" t="n">
-        <v>9.14333172665165</v>
+        <v>6.84853066747513</v>
       </c>
       <c r="C29" s="2" t="n">
-        <v>0.642485475713828</v>
+        <v>0.519320810726022</v>
       </c>
       <c r="D29" s="2" t="n">
-        <v>0.0601153343313675</v>
+        <v>0.0274388617373422</v>
       </c>
       <c r="E29" s="2" t="n">
-        <v>2.01555432283395</v>
+        <v>2.01550649489432</v>
       </c>
       <c r="F29" s="2" t="n">
-        <v>982.790000000001</v>
+        <v>526.57</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29219,19 +29113,19 @@
         <v>130</v>
       </c>
       <c r="B30" s="2" t="n">
-        <v>8.21177640874369</v>
+        <v>9.14333172665165</v>
       </c>
       <c r="C30" s="2" t="n">
-        <v>0.591839877046792</v>
+        <v>0.642485475713828</v>
       </c>
       <c r="D30" s="2" t="n">
-        <v>0.0461762202080638</v>
+        <v>0.0601153343313675</v>
       </c>
       <c r="E30" s="2" t="n">
-        <v>2.01104547043623</v>
+        <v>2.01555432283395</v>
       </c>
       <c r="F30" s="2" t="n">
-        <v>536.66</v>
+        <v>982.790000000001</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29239,24 +29133,39 @@
         <v>131</v>
       </c>
       <c r="B31" s="2" t="n">
-        <v>6.20424969723244</v>
+        <v>8.21177640874369</v>
       </c>
       <c r="C31" s="2" t="n">
-        <v>0.500510559563247</v>
+        <v>0.591839877046792</v>
       </c>
       <c r="D31" s="2" t="n">
-        <v>0.0220650119427435</v>
+        <v>0.0461762202080638</v>
       </c>
       <c r="E31" s="2" t="n">
-        <v>2.01030516181707</v>
+        <v>2.01104547043623</v>
       </c>
       <c r="F31" s="2" t="n">
-        <v>549.419999999998</v>
+        <v>536.66</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
         <v>132</v>
+      </c>
+      <c r="B32" s="2" t="n">
+        <v>6.20424969723244</v>
+      </c>
+      <c r="C32" s="2" t="n">
+        <v>0.500510559563247</v>
+      </c>
+      <c r="D32" s="2" t="n">
+        <v>0.0220650119427435</v>
+      </c>
+      <c r="E32" s="2" t="n">
+        <v>2.01030516181707</v>
+      </c>
+      <c r="F32" s="2" t="n">
+        <v>549.419999999998</v>
       </c>
     </row>
   </sheetData>
@@ -29271,31 +29180,34 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2:F31"/>
+      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.98"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>140</v>
@@ -29305,40 +29217,25 @@
       <c r="A2" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B2" s="2" t="n">
-        <v>0.483924250986352</v>
-      </c>
-      <c r="C2" s="2" t="n">
-        <v>0.0112092953899811</v>
-      </c>
-      <c r="D2" s="2" t="n">
-        <v>2.02473055389905</v>
-      </c>
-      <c r="E2" s="2" t="n">
-        <v>4.63995155076485</v>
-      </c>
-      <c r="F2" s="2" t="n">
-        <v>25.5099999999984</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>103</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>0.48392464904185</v>
+        <v>4.63995155076485</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>0.0112093013825847</v>
+        <v>0.483924250986352</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>2.02473088808347</v>
+        <v>0.0112092953899811</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>4.63995154982018</v>
+        <v>2.02473055389905</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>45.1699999999983</v>
+        <v>25.5099999999984</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29346,19 +29243,19 @@
         <v>104</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>0.483924236225294</v>
+        <v>4.63995154982018</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>0.0112091703014437</v>
+        <v>0.48392464904185</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>2.02473119032642</v>
+        <v>0.0112093013825847</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>4.63995155035068</v>
+        <v>2.02473088808347</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>65.3499999999985</v>
+        <v>45.1699999999983</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29366,19 +29263,19 @@
         <v>105</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>0.483924836863508</v>
+        <v>4.63995155035068</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>0.0112092962789677</v>
+        <v>0.483924236225294</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>2.02473085194201</v>
+        <v>0.0112091703014437</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>4.63995154981718</v>
+        <v>2.02473119032642</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>85.3199999999997</v>
+        <v>65.3499999999985</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29386,19 +29283,19 @@
         <v>106</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>0.483924319262051</v>
+        <v>4.63995154981718</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>0.0112091366885253</v>
+        <v>0.483924836863508</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>2.02473095281403</v>
+        <v>0.0112092962789677</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>4.6399515503805</v>
+        <v>2.02473085194201</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>104.93</v>
+        <v>85.3199999999997</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29406,19 +29303,19 @@
         <v>107</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>0.48392471488054</v>
+        <v>4.6399515503805</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>0.011209258327629</v>
+        <v>0.483924319262051</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>2.02473092003438</v>
+        <v>0.0112091366885253</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>4.63995154985558</v>
+        <v>2.02473095281403</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>126.610000000001</v>
+        <v>104.93</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29426,19 +29323,19 @@
         <v>108</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>0.483924869241066</v>
+        <v>4.63995154985558</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>0.0112093153697203</v>
+        <v>0.48392471488054</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>2.02473084096144</v>
+        <v>0.011209258327629</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>4.63995154979456</v>
+        <v>2.02473092003438</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>146.080000000002</v>
+        <v>126.610000000001</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29446,19 +29343,19 @@
         <v>109</v>
       </c>
       <c r="B9" s="2" t="n">
-        <v>0.483925437147606</v>
+        <v>4.63995154979456</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>0.0112094516453662</v>
+        <v>0.483924869241066</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>2.02473090620628</v>
+        <v>0.0112093153697203</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>4.63995154999274</v>
+        <v>2.02473084096144</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>165.5</v>
+        <v>146.080000000002</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29466,19 +29363,19 @@
         <v>110</v>
       </c>
       <c r="B10" s="2" t="n">
-        <v>0.483924870055353</v>
+        <v>4.63995154999274</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>0.0112093175347955</v>
+        <v>0.483925437147606</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>2.02473088608028</v>
+        <v>0.0112094516453662</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>4.63995154977424</v>
+        <v>2.02473090620628</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>184.919999999998</v>
+        <v>165.5</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29486,19 +29383,19 @@
         <v>111</v>
       </c>
       <c r="B11" s="2" t="n">
-        <v>0.483924848808133</v>
+        <v>4.63995154977424</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>0.0112093156744636</v>
+        <v>0.483924870055353</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>2.02473089959601</v>
+        <v>0.0112093175347955</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>4.63995154977365</v>
+        <v>2.02473088608028</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>204.52</v>
+        <v>184.919999999998</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29506,19 +29403,19 @@
         <v>112</v>
       </c>
       <c r="B12" s="2" t="n">
-        <v>0.483924825449184</v>
+        <v>4.63995154977365</v>
       </c>
       <c r="C12" s="2" t="n">
-        <v>0.0112093096640374</v>
+        <v>0.483924848808133</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>2.02473088750788</v>
+        <v>0.0112093156744636</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>4.63995154977403</v>
+        <v>2.02473089959601</v>
       </c>
       <c r="F12" s="2" t="n">
-        <v>227.5</v>
+        <v>204.52</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29526,19 +29423,19 @@
         <v>113</v>
       </c>
       <c r="B13" s="2" t="n">
-        <v>0.48392477445533</v>
+        <v>4.63995154977403</v>
       </c>
       <c r="C13" s="2" t="n">
-        <v>0.0112092668400815</v>
+        <v>0.483924825449184</v>
       </c>
       <c r="D13" s="2" t="n">
-        <v>2.02473092401406</v>
+        <v>0.0112093096640374</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>4.63995154986036</v>
+        <v>2.02473088750788</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>247.02</v>
+        <v>227.5</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29546,19 +29443,19 @@
         <v>114</v>
       </c>
       <c r="B14" s="2" t="n">
-        <v>0.483924811494028</v>
+        <v>4.63995154986036</v>
       </c>
       <c r="C14" s="2" t="n">
-        <v>0.0112092785230735</v>
+        <v>0.48392477445533</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>2.02473076718855</v>
+        <v>0.0112092668400815</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>4.63995155000539</v>
+        <v>2.02473092401406</v>
       </c>
       <c r="F14" s="2" t="n">
-        <v>266.59</v>
+        <v>247.02</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29566,19 +29463,19 @@
         <v>115</v>
       </c>
       <c r="B15" s="2" t="n">
-        <v>0.483924595304024</v>
+        <v>4.63995155000539</v>
       </c>
       <c r="C15" s="2" t="n">
-        <v>0.0112092572609299</v>
+        <v>0.483924811494028</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>2.02473088068023</v>
+        <v>0.0112092785230735</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>4.63995154981258</v>
+        <v>2.02473076718855</v>
       </c>
       <c r="F15" s="2" t="n">
-        <v>287.43</v>
+        <v>266.59</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29586,19 +29483,19 @@
         <v>116</v>
       </c>
       <c r="B16" s="2" t="n">
-        <v>0.483924849454178</v>
+        <v>4.63995154981258</v>
       </c>
       <c r="C16" s="2" t="n">
-        <v>0.0112093143966782</v>
+        <v>0.483924595304024</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>2.02473094901455</v>
+        <v>0.0112092572609299</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>4.63995154979167</v>
+        <v>2.02473088068023</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>309.810000000001</v>
+        <v>287.43</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29606,19 +29503,19 @@
         <v>117</v>
       </c>
       <c r="B17" s="2" t="n">
-        <v>0.483924618067386</v>
+        <v>4.63995154979167</v>
       </c>
       <c r="C17" s="2" t="n">
-        <v>0.0112092881701825</v>
+        <v>0.483924849454178</v>
       </c>
       <c r="D17" s="2" t="n">
-        <v>2.02473086683429</v>
+        <v>0.0112093143966782</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>4.63995154980479</v>
+        <v>2.02473094901455</v>
       </c>
       <c r="F17" s="2" t="n">
-        <v>332.220000000001</v>
+        <v>309.810000000001</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29626,19 +29523,19 @@
         <v>118</v>
       </c>
       <c r="B18" s="2" t="n">
-        <v>0.483924924991629</v>
+        <v>4.63995154980479</v>
       </c>
       <c r="C18" s="2" t="n">
-        <v>0.0112093103086182</v>
+        <v>0.483924618067386</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>2.02473092176472</v>
+        <v>0.0112092881701825</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>4.63995154979824</v>
+        <v>2.02473086683429</v>
       </c>
       <c r="F18" s="2" t="n">
-        <v>354.709999999999</v>
+        <v>332.220000000001</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29646,19 +29543,19 @@
         <v>119</v>
       </c>
       <c r="B19" s="2" t="n">
-        <v>0.483924868835047</v>
+        <v>4.63995154979824</v>
       </c>
       <c r="C19" s="2" t="n">
-        <v>0.0112093378928642</v>
+        <v>0.483924924991629</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>2.02473095560423</v>
+        <v>0.0112093103086182</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>4.63995154984606</v>
+        <v>2.02473092176472</v>
       </c>
       <c r="F19" s="2" t="n">
-        <v>377.34</v>
+        <v>354.709999999999</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29666,19 +29563,19 @@
         <v>120</v>
       </c>
       <c r="B20" s="2" t="n">
-        <v>0.483924992489554</v>
+        <v>4.63995154984606</v>
       </c>
       <c r="C20" s="2" t="n">
-        <v>0.0112093398572649</v>
+        <v>0.483924868835047</v>
       </c>
       <c r="D20" s="2" t="n">
-        <v>2.02473090785022</v>
+        <v>0.0112093378928642</v>
       </c>
       <c r="E20" s="2" t="n">
-        <v>4.63995154978257</v>
+        <v>2.02473095560423</v>
       </c>
       <c r="F20" s="2" t="n">
-        <v>399.77</v>
+        <v>377.34</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29686,19 +29583,19 @@
         <v>121</v>
       </c>
       <c r="B21" s="2" t="n">
-        <v>0.483924848086439</v>
+        <v>4.63995154978257</v>
       </c>
       <c r="C21" s="2" t="n">
-        <v>0.011209301042027</v>
+        <v>0.483924992489554</v>
       </c>
       <c r="D21" s="2" t="n">
-        <v>2.02473065253577</v>
+        <v>0.0112093398572649</v>
       </c>
       <c r="E21" s="2" t="n">
-        <v>4.63995155020629</v>
+        <v>2.02473090785022</v>
       </c>
       <c r="F21" s="2" t="n">
-        <v>422.360000000001</v>
+        <v>399.77</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29706,19 +29603,19 @@
         <v>122</v>
       </c>
       <c r="B22" s="2" t="n">
-        <v>0.483924807949757</v>
+        <v>4.63995155020629</v>
       </c>
       <c r="C22" s="2" t="n">
-        <v>0.0112092995852832</v>
+        <v>0.483924848086439</v>
       </c>
       <c r="D22" s="2" t="n">
-        <v>2.02473093925122</v>
+        <v>0.011209301042027</v>
       </c>
       <c r="E22" s="2" t="n">
-        <v>4.63995154978561</v>
+        <v>2.02473065253577</v>
       </c>
       <c r="F22" s="2" t="n">
-        <v>445.59</v>
+        <v>422.360000000001</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29726,19 +29623,19 @@
         <v>123</v>
       </c>
       <c r="B23" s="2" t="n">
-        <v>0.483924837374494</v>
+        <v>4.63995154978561</v>
       </c>
       <c r="C23" s="2" t="n">
-        <v>0.0112093180106047</v>
+        <v>0.483924807949757</v>
       </c>
       <c r="D23" s="2" t="n">
-        <v>2.02473090429279</v>
+        <v>0.0112092995852832</v>
       </c>
       <c r="E23" s="2" t="n">
-        <v>4.63995154977678</v>
+        <v>2.02473093925122</v>
       </c>
       <c r="F23" s="2" t="n">
-        <v>469.119999999999</v>
+        <v>445.59</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29746,19 +29643,19 @@
         <v>124</v>
       </c>
       <c r="B24" s="2" t="n">
-        <v>0.483924641469431</v>
+        <v>4.63995154977678</v>
       </c>
       <c r="C24" s="2" t="n">
-        <v>0.0112092917337785</v>
+        <v>0.483924837374494</v>
       </c>
       <c r="D24" s="2" t="n">
-        <v>2.02473097346272</v>
+        <v>0.0112093180106047</v>
       </c>
       <c r="E24" s="2" t="n">
-        <v>4.639951549853</v>
+        <v>2.02473090429279</v>
       </c>
       <c r="F24" s="2" t="n">
-        <v>491.849999999999</v>
+        <v>469.119999999999</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29766,19 +29663,19 @@
         <v>125</v>
       </c>
       <c r="B25" s="2" t="n">
-        <v>0.483924832034735</v>
+        <v>4.639951549853</v>
       </c>
       <c r="C25" s="2" t="n">
-        <v>0.0112093032656768</v>
+        <v>0.483924641469431</v>
       </c>
       <c r="D25" s="2" t="n">
-        <v>2.02473086386474</v>
+        <v>0.0112092917337785</v>
       </c>
       <c r="E25" s="2" t="n">
-        <v>4.63995154978944</v>
+        <v>2.02473097346272</v>
       </c>
       <c r="F25" s="2" t="n">
-        <v>514.439999999999</v>
+        <v>491.849999999999</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29786,19 +29683,19 @@
         <v>126</v>
       </c>
       <c r="B26" s="2" t="n">
-        <v>0.483924569731916</v>
+        <v>4.63995154978944</v>
       </c>
       <c r="C26" s="2" t="n">
-        <v>0.011209263919931</v>
+        <v>0.483924832034735</v>
       </c>
       <c r="D26" s="2" t="n">
-        <v>2.0247307955171</v>
+        <v>0.0112093032656768</v>
       </c>
       <c r="E26" s="2" t="n">
-        <v>4.63995154986814</v>
+        <v>2.02473086386474</v>
       </c>
       <c r="F26" s="2" t="n">
-        <v>538</v>
+        <v>514.439999999999</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29806,19 +29703,19 @@
         <v>127</v>
       </c>
       <c r="B27" s="2" t="n">
-        <v>0.483924980723191</v>
+        <v>4.63995154986814</v>
       </c>
       <c r="C27" s="2" t="n">
-        <v>0.0112093262167448</v>
+        <v>0.483924569731916</v>
       </c>
       <c r="D27" s="2" t="n">
-        <v>2.0247307320054</v>
+        <v>0.011209263919931</v>
       </c>
       <c r="E27" s="2" t="n">
-        <v>4.63995154998153</v>
+        <v>2.0247307955171</v>
       </c>
       <c r="F27" s="2" t="n">
-        <v>561.549999999999</v>
+        <v>538</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29826,19 +29723,19 @@
         <v>128</v>
       </c>
       <c r="B28" s="2" t="n">
-        <v>0.483924743595052</v>
+        <v>4.63995154998153</v>
       </c>
       <c r="C28" s="2" t="n">
-        <v>0.0112093218932475</v>
+        <v>0.483924980723191</v>
       </c>
       <c r="D28" s="2" t="n">
-        <v>2.02473089315742</v>
+        <v>0.0112093262167448</v>
       </c>
       <c r="E28" s="2" t="n">
-        <v>4.63995154982682</v>
+        <v>2.0247307320054</v>
       </c>
       <c r="F28" s="2" t="n">
-        <v>584.470000000001</v>
+        <v>561.549999999999</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29846,19 +29743,19 @@
         <v>129</v>
       </c>
       <c r="B29" s="2" t="n">
-        <v>0.483924581192209</v>
+        <v>4.63995154982682</v>
       </c>
       <c r="C29" s="2" t="n">
-        <v>0.0112093061083779</v>
+        <v>0.483924743595052</v>
       </c>
       <c r="D29" s="2" t="n">
-        <v>2.02473086847916</v>
+        <v>0.0112093218932475</v>
       </c>
       <c r="E29" s="2" t="n">
-        <v>4.63995154989939</v>
+        <v>2.02473089315742</v>
       </c>
       <c r="F29" s="2" t="n">
-        <v>608.349999999999</v>
+        <v>584.470000000001</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29866,19 +29763,19 @@
         <v>130</v>
       </c>
       <c r="B30" s="2" t="n">
-        <v>0.483925117118884</v>
+        <v>4.63995154989939</v>
       </c>
       <c r="C30" s="2" t="n">
-        <v>0.0112093780188704</v>
+        <v>0.483924581192209</v>
       </c>
       <c r="D30" s="2" t="n">
-        <v>2.02473077186234</v>
+        <v>0.0112093061083779</v>
       </c>
       <c r="E30" s="2" t="n">
-        <v>4.63995154987622</v>
+        <v>2.02473086847916</v>
       </c>
       <c r="F30" s="2" t="n">
-        <v>631.049999999999</v>
+        <v>608.349999999999</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29886,18 +29783,38 @@
         <v>131</v>
       </c>
       <c r="B31" s="2" t="n">
+        <v>4.63995154987622</v>
+      </c>
+      <c r="C31" s="2" t="n">
+        <v>0.483925117118884</v>
+      </c>
+      <c r="D31" s="2" t="n">
+        <v>0.0112093780188704</v>
+      </c>
+      <c r="E31" s="2" t="n">
+        <v>2.02473077186234</v>
+      </c>
+      <c r="F31" s="2" t="n">
+        <v>631.049999999999</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B32" s="2" t="n">
+        <v>4.63995154981533</v>
+      </c>
+      <c r="C32" s="2" t="n">
         <v>0.483924577524277</v>
       </c>
-      <c r="C31" s="2" t="n">
+      <c r="D32" s="2" t="n">
         <v>0.0112092728931079</v>
       </c>
-      <c r="D31" s="2" t="n">
+      <c r="E32" s="2" t="n">
         <v>2.02473084059962</v>
       </c>
-      <c r="E31" s="2" t="n">
-        <v>4.63995154981533</v>
-      </c>
-      <c r="F31" s="2" t="n">
+      <c r="F32" s="2" t="n">
         <v>653.669999999998</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add column for time of each run
</commit_message>
<xml_diff>
--- a/results_from_all_algos.xlsx
+++ b/results_from_all_algos.xlsx
@@ -5,14 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="WOA_CONV" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="WOA_RESULTS" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="GA" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="SA" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="CSA" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="WOA_CONV" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="WOA_RESULTS" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="GA" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="SA" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="CSA" sheetId="5" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="157">
   <si>
     <t xml:space="preserve">ITER#</t>
   </si>
@@ -449,6 +449,9 @@
     <t xml:space="preserve">Time</t>
   </si>
   <si>
+    <t xml:space="preserve">time d</t>
+  </si>
+  <si>
     <t xml:space="preserve">Agents 1000 iters 30</t>
   </si>
   <si>
@@ -459,6 +462,33 @@
   </si>
   <si>
     <t xml:space="preserve">Agents 300 iters 30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r09</t>
   </si>
   <si>
     <t xml:space="preserve">Population 40</t>
@@ -568,17 +598,132 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:CW132"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="Y2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="Y1" activeCellId="0" sqref="Y1"/>
@@ -24934,18 +25079,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AC32"/>
+  <dimension ref="A1:AE32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R3" activeCellId="0" sqref="R3"/>
+      <selection pane="bottomRight" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -24969,6 +25114,9 @@
       <c r="F1" s="1" t="s">
         <v>140</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="J1" s="1" t="s">
         <v>136</v>
       </c>
@@ -24984,6 +25132,9 @@
       <c r="N1" s="1" t="s">
         <v>140</v>
       </c>
+      <c r="O1" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="R1" s="1" t="s">
         <v>136</v>
       </c>
@@ -24999,20 +25150,26 @@
       <c r="V1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="W1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>140</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25020,33 +25177,33 @@
         <v>101</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>101</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>101</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="X2" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="Y2" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="AA2" s="1"/>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="1" t="s">
+        <v>145</v>
+      </c>
       <c r="AB2" s="1"/>
+      <c r="AC2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>103</v>
+        <v>146</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>4.73282705256699</v>
@@ -25063,8 +25220,12 @@
       <c r="F3" s="2" t="n">
         <v>113.549999999999</v>
       </c>
+      <c r="G3" s="0" t="n">
+        <f aca="false">F3-F2</f>
+        <v>113.549999999999</v>
+      </c>
       <c r="I3" s="1" t="s">
-        <v>103</v>
+        <v>146</v>
       </c>
       <c r="J3" s="2" t="n">
         <v>4.73384437044199</v>
@@ -25081,8 +25242,12 @@
       <c r="N3" s="2" t="n">
         <v>200.299999999999</v>
       </c>
+      <c r="O3" s="0" t="n">
+        <f aca="false">N3-N2</f>
+        <v>200.299999999999</v>
+      </c>
       <c r="Q3" s="1" t="s">
-        <v>103</v>
+        <v>146</v>
       </c>
       <c r="R3" s="2" t="n">
         <v>10.7344618261651</v>
@@ -25099,28 +25264,36 @@
       <c r="V3" s="2" t="n">
         <v>49.380000000001</v>
       </c>
-      <c r="X3" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="Y3" s="2" t="n">
+      <c r="W3" s="0" t="n">
+        <f aca="false">V3-V2</f>
+        <v>49.380000000001</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="Z3" s="2" t="n">
         <v>6.69584862019204</v>
       </c>
-      <c r="Z3" s="2" t="n">
+      <c r="AA3" s="2" t="n">
         <v>0.573781261508616</v>
       </c>
-      <c r="AA3" s="2" t="n">
+      <c r="AB3" s="2" t="n">
         <v>0.0333309402681</v>
       </c>
-      <c r="AB3" s="2" t="n">
+      <c r="AC3" s="2" t="n">
         <v>2.01851960457967</v>
       </c>
-      <c r="AC3" s="2" t="n">
+      <c r="AD3" s="2" t="n">
+        <v>22.7600000000002</v>
+      </c>
+      <c r="AE3" s="0" t="n">
+        <f aca="false">AD3-AD2</f>
         <v>22.7600000000002</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>104</v>
+        <v>147</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>4.73251624066684</v>
@@ -25137,8 +25310,12 @@
       <c r="F4" s="2" t="n">
         <v>211.469999999999</v>
       </c>
+      <c r="G4" s="0" t="n">
+        <f aca="false">F4-F3</f>
+        <v>97.92</v>
+      </c>
       <c r="I4" s="1" t="s">
-        <v>104</v>
+        <v>147</v>
       </c>
       <c r="J4" s="2" t="n">
         <v>4.84794027256065</v>
@@ -25155,8 +25332,12 @@
       <c r="N4" s="2" t="n">
         <v>391.849999999999</v>
       </c>
+      <c r="O4" s="0" t="n">
+        <f aca="false">N4-N3</f>
+        <v>191.55</v>
+      </c>
       <c r="Q4" s="1" t="s">
-        <v>104</v>
+        <v>147</v>
       </c>
       <c r="R4" s="2" t="n">
         <v>14.5297619190541</v>
@@ -25173,28 +25354,36 @@
       <c r="V4" s="2" t="n">
         <v>103.880000000001</v>
       </c>
-      <c r="X4" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="Y4" s="2" t="n">
+      <c r="W4" s="0" t="n">
+        <f aca="false">V4-V3</f>
+        <v>54.5</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="Z4" s="2" t="n">
         <v>4.93002892499933</v>
       </c>
-      <c r="Z4" s="2" t="n">
+      <c r="AA4" s="2" t="n">
         <v>0.510256231968616</v>
       </c>
-      <c r="AA4" s="2" t="n">
+      <c r="AB4" s="2" t="n">
         <v>0.0167051762212759</v>
       </c>
-      <c r="AB4" s="2" t="n">
+      <c r="AC4" s="2" t="n">
         <v>2.02173487369732</v>
       </c>
-      <c r="AC4" s="2" t="n">
+      <c r="AD4" s="2" t="n">
         <v>43.3400000000001</v>
+      </c>
+      <c r="AE4" s="0" t="n">
+        <f aca="false">AD4-AD3</f>
+        <v>20.5799999999999</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>105</v>
+        <v>148</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>4.73750625719472</v>
@@ -25211,8 +25400,12 @@
       <c r="F5" s="2" t="n">
         <v>305</v>
       </c>
+      <c r="G5" s="0" t="n">
+        <f aca="false">F5-F4</f>
+        <v>93.530000000001</v>
+      </c>
       <c r="I5" s="1" t="s">
-        <v>105</v>
+        <v>148</v>
       </c>
       <c r="J5" s="2" t="n">
         <v>4.73605216732573</v>
@@ -25229,8 +25422,12 @@
       <c r="N5" s="2" t="n">
         <v>580.74</v>
       </c>
+      <c r="O5" s="0" t="n">
+        <f aca="false">N5-N4</f>
+        <v>188.890000000001</v>
+      </c>
       <c r="Q5" s="1" t="s">
-        <v>105</v>
+        <v>148</v>
       </c>
       <c r="R5" s="2" t="n">
         <v>4.84804171549978</v>
@@ -25247,28 +25444,36 @@
       <c r="V5" s="2" t="n">
         <v>145.140000000003</v>
       </c>
-      <c r="X5" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="Y5" s="2" t="n">
+      <c r="W5" s="0" t="n">
+        <f aca="false">V5-V4</f>
+        <v>41.260000000002</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="Z5" s="2" t="n">
         <v>4.73609256977679</v>
       </c>
-      <c r="Z5" s="2" t="n">
+      <c r="AA5" s="2" t="n">
         <v>0.487641598070697</v>
       </c>
-      <c r="AA5" s="2" t="n">
+      <c r="AB5" s="2" t="n">
         <v>0.0120176090070576</v>
       </c>
-      <c r="AB5" s="2" t="n">
+      <c r="AC5" s="2" t="n">
         <v>2.02271261361793</v>
       </c>
-      <c r="AC5" s="2" t="n">
+      <c r="AD5" s="2" t="n">
         <v>62.2899999999991</v>
+      </c>
+      <c r="AE5" s="0" t="n">
+        <f aca="false">AD5-AD4</f>
+        <v>18.949999999999</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>106</v>
+        <v>149</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>4.73482989807527</v>
@@ -25285,8 +25490,12 @@
       <c r="F6" s="2" t="n">
         <v>397.769999999999</v>
       </c>
+      <c r="G6" s="0" t="n">
+        <f aca="false">F6-F5</f>
+        <v>92.769999999999</v>
+      </c>
       <c r="I6" s="1" t="s">
-        <v>106</v>
+        <v>149</v>
       </c>
       <c r="J6" s="2" t="n">
         <v>4.74029720513826</v>
@@ -25303,8 +25512,12 @@
       <c r="N6" s="2" t="n">
         <v>765.299999999999</v>
       </c>
+      <c r="O6" s="0" t="n">
+        <f aca="false">N6-N5</f>
+        <v>184.559999999999</v>
+      </c>
       <c r="Q6" s="1" t="s">
-        <v>106</v>
+        <v>149</v>
       </c>
       <c r="R6" s="2" t="n">
         <v>7.76741733991397</v>
@@ -25321,28 +25534,36 @@
       <c r="V6" s="2" t="n">
         <v>193.170000000002</v>
       </c>
-      <c r="X6" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="Y6" s="2" t="n">
+      <c r="W6" s="0" t="n">
+        <f aca="false">V6-V5</f>
+        <v>48.029999999999</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="Z6" s="2" t="n">
         <v>4.86063198429821</v>
       </c>
-      <c r="Z6" s="2" t="n">
+      <c r="AA6" s="2" t="n">
         <v>0.505927587799093</v>
       </c>
-      <c r="AA6" s="2" t="n">
+      <c r="AB6" s="2" t="n">
         <v>0.0154304267644149</v>
       </c>
-      <c r="AB6" s="2" t="n">
+      <c r="AC6" s="2" t="n">
         <v>2.02210058835512</v>
       </c>
-      <c r="AC6" s="2" t="n">
+      <c r="AD6" s="2" t="n">
         <v>81.3600000000006</v>
+      </c>
+      <c r="AE6" s="0" t="n">
+        <f aca="false">AD6-AD5</f>
+        <v>19.0700000000015</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>107</v>
+        <v>150</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>4.73256901104308</v>
@@ -25359,8 +25580,12 @@
       <c r="F7" s="2" t="n">
         <v>490.279999999999</v>
       </c>
+      <c r="G7" s="0" t="n">
+        <f aca="false">F7-F6</f>
+        <v>92.51</v>
+      </c>
       <c r="I7" s="1" t="s">
-        <v>107</v>
+        <v>150</v>
       </c>
       <c r="J7" s="2" t="n">
         <v>4.73272127602358</v>
@@ -25377,8 +25602,12 @@
       <c r="N7" s="2" t="n">
         <v>954.009999999998</v>
       </c>
+      <c r="O7" s="0" t="n">
+        <f aca="false">N7-N6</f>
+        <v>188.709999999999</v>
+      </c>
       <c r="Q7" s="1" t="s">
-        <v>107</v>
+        <v>150</v>
       </c>
       <c r="R7" s="2" t="n">
         <v>4.77334183599085</v>
@@ -25395,28 +25624,36 @@
       <c r="V7" s="2" t="n">
         <v>237.940000000002</v>
       </c>
-      <c r="X7" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="Y7" s="2" t="n">
+      <c r="W7" s="0" t="n">
+        <f aca="false">V7-V6</f>
+        <v>44.77</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="Z7" s="2" t="n">
         <v>6.60147190401879</v>
       </c>
-      <c r="Z7" s="2" t="n">
+      <c r="AA7" s="2" t="n">
         <v>0.581859590187604</v>
       </c>
-      <c r="AA7" s="2" t="n">
+      <c r="AB7" s="2" t="n">
         <v>0.0322061123393598</v>
       </c>
-      <c r="AB7" s="2" t="n">
+      <c r="AC7" s="2" t="n">
         <v>2.01971131920745</v>
       </c>
-      <c r="AC7" s="2" t="n">
+      <c r="AD7" s="2" t="n">
         <v>100.67</v>
+      </c>
+      <c r="AE7" s="0" t="n">
+        <f aca="false">AD7-AD6</f>
+        <v>19.3099999999994</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>108</v>
+        <v>151</v>
       </c>
       <c r="B8" s="2" t="n">
         <v>4.73561216373413</v>
@@ -25433,8 +25670,12 @@
       <c r="F8" s="2" t="n">
         <v>585.82</v>
       </c>
+      <c r="G8" s="0" t="n">
+        <f aca="false">F8-F7</f>
+        <v>95.540000000001</v>
+      </c>
       <c r="I8" s="1" t="s">
-        <v>108</v>
+        <v>151</v>
       </c>
       <c r="J8" s="2" t="n">
         <v>4.7333403236908</v>
@@ -25451,8 +25692,12 @@
       <c r="N8" s="2" t="n">
         <v>1143.98</v>
       </c>
+      <c r="O8" s="0" t="n">
+        <f aca="false">N8-N7</f>
+        <v>189.970000000002</v>
+      </c>
       <c r="Q8" s="1" t="s">
-        <v>108</v>
+        <v>151</v>
       </c>
       <c r="R8" s="2" t="n">
         <v>5.9514484943827</v>
@@ -25469,28 +25714,36 @@
       <c r="V8" s="2" t="n">
         <v>290.600000000002</v>
       </c>
-      <c r="X8" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="Y8" s="2" t="n">
+      <c r="W8" s="0" t="n">
+        <f aca="false">V8-V7</f>
+        <v>52.66</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="Z8" s="2" t="n">
         <v>5.32508805696527</v>
       </c>
-      <c r="Z8" s="2" t="n">
+      <c r="AA8" s="2" t="n">
         <v>0.52391739504947</v>
       </c>
-      <c r="AA8" s="2" t="n">
+      <c r="AB8" s="2" t="n">
         <v>0.0211143002626029</v>
       </c>
-      <c r="AB8" s="2" t="n">
+      <c r="AC8" s="2" t="n">
         <v>2.02032324216094</v>
       </c>
-      <c r="AC8" s="2" t="n">
+      <c r="AD8" s="2" t="n">
         <v>119.77</v>
+      </c>
+      <c r="AE8" s="0" t="n">
+        <f aca="false">AD8-AD7</f>
+        <v>19.1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>109</v>
+        <v>152</v>
       </c>
       <c r="B9" s="2" t="n">
         <v>4.73264877533292</v>
@@ -25507,8 +25760,12 @@
       <c r="F9" s="2" t="n">
         <v>685.15</v>
       </c>
+      <c r="G9" s="0" t="n">
+        <f aca="false">F9-F8</f>
+        <v>99.3299999999999</v>
+      </c>
       <c r="I9" s="1" t="s">
-        <v>109</v>
+        <v>152</v>
       </c>
       <c r="J9" s="2" t="n">
         <v>4.79325080296581</v>
@@ -25525,8 +25782,12 @@
       <c r="N9" s="2" t="n">
         <v>1333.63</v>
       </c>
+      <c r="O9" s="0" t="n">
+        <f aca="false">N9-N8</f>
+        <v>189.65</v>
+      </c>
       <c r="Q9" s="1" t="s">
-        <v>109</v>
+        <v>152</v>
       </c>
       <c r="R9" s="2" t="n">
         <v>5.34689717187448</v>
@@ -25543,28 +25804,36 @@
       <c r="V9" s="2" t="n">
         <v>337.170000000002</v>
       </c>
-      <c r="X9" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="Y9" s="2" t="n">
+      <c r="W9" s="0" t="n">
+        <f aca="false">V9-V8</f>
+        <v>46.57</v>
+      </c>
+      <c r="Y9" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="Z9" s="2" t="n">
         <v>5.00113948180471</v>
       </c>
-      <c r="Z9" s="2" t="n">
+      <c r="AA9" s="2" t="n">
         <v>0.509737160282644</v>
       </c>
-      <c r="AA9" s="2" t="n">
+      <c r="AB9" s="2" t="n">
         <v>0.0174673638832025</v>
       </c>
-      <c r="AB9" s="2" t="n">
+      <c r="AC9" s="2" t="n">
         <v>2.02103148452504</v>
       </c>
-      <c r="AC9" s="2" t="n">
+      <c r="AD9" s="2" t="n">
         <v>138.969999999999</v>
+      </c>
+      <c r="AE9" s="0" t="n">
+        <f aca="false">AD9-AD8</f>
+        <v>19.199999999999</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>110</v>
+        <v>153</v>
       </c>
       <c r="B10" s="2" t="n">
         <v>4.74131495839404</v>
@@ -25581,8 +25850,12 @@
       <c r="F10" s="2" t="n">
         <v>784.5</v>
       </c>
+      <c r="G10" s="0" t="n">
+        <f aca="false">F10-F9</f>
+        <v>99.35</v>
+      </c>
       <c r="I10" s="1" t="s">
-        <v>110</v>
+        <v>153</v>
       </c>
       <c r="J10" s="2" t="n">
         <v>4.73735478004939</v>
@@ -25599,8 +25872,12 @@
       <c r="N10" s="2" t="n">
         <v>1529.04</v>
       </c>
+      <c r="O10" s="0" t="n">
+        <f aca="false">N10-N9</f>
+        <v>195.41</v>
+      </c>
       <c r="Q10" s="1" t="s">
-        <v>110</v>
+        <v>153</v>
       </c>
       <c r="R10" s="2" t="n">
         <v>6.30863179469164</v>
@@ -25617,28 +25894,36 @@
       <c r="V10" s="2" t="n">
         <v>388.950000000001</v>
       </c>
-      <c r="X10" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="Y10" s="2" t="n">
+      <c r="W10" s="0" t="n">
+        <f aca="false">V10-V9</f>
+        <v>51.779999999999</v>
+      </c>
+      <c r="Y10" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="Z10" s="2" t="n">
         <v>4.77622194267296</v>
       </c>
-      <c r="Z10" s="2" t="n">
+      <c r="AA10" s="2" t="n">
         <v>0.494577810189531</v>
       </c>
-      <c r="AA10" s="2" t="n">
+      <c r="AB10" s="2" t="n">
         <v>0.013660038381724</v>
       </c>
-      <c r="AB10" s="2" t="n">
+      <c r="AC10" s="2" t="n">
         <v>2.02214118791182</v>
       </c>
-      <c r="AC10" s="2" t="n">
+      <c r="AD10" s="2" t="n">
         <v>157.9</v>
+      </c>
+      <c r="AE10" s="0" t="n">
+        <f aca="false">AD10-AD9</f>
+        <v>18.930000000001</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>111</v>
+        <v>154</v>
       </c>
       <c r="B11" s="2" t="n">
         <v>4.74341171169469</v>
@@ -25655,8 +25940,12 @@
       <c r="F11" s="2" t="n">
         <v>885.129999999999</v>
       </c>
+      <c r="G11" s="0" t="n">
+        <f aca="false">F11-F10</f>
+        <v>100.629999999999</v>
+      </c>
       <c r="I11" s="1" t="s">
-        <v>111</v>
+        <v>154</v>
       </c>
       <c r="J11" s="2" t="n">
         <v>4.73656998313829</v>
@@ -25673,8 +25962,12 @@
       <c r="N11" s="2" t="n">
         <v>1727.35</v>
       </c>
+      <c r="O11" s="0" t="n">
+        <f aca="false">N11-N10</f>
+        <v>198.31</v>
+      </c>
       <c r="Q11" s="1" t="s">
-        <v>111</v>
+        <v>154</v>
       </c>
       <c r="R11" s="2" t="n">
         <v>11.5474903969739</v>
@@ -25691,23 +25984,31 @@
       <c r="V11" s="2" t="n">
         <v>440.360000000001</v>
       </c>
-      <c r="X11" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="Y11" s="2" t="n">
+      <c r="W11" s="0" t="n">
+        <f aca="false">V11-V10</f>
+        <v>51.41</v>
+      </c>
+      <c r="Y11" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="Z11" s="2" t="n">
         <v>4.7616530580448</v>
       </c>
-      <c r="Z11" s="2" t="n">
+      <c r="AA11" s="2" t="n">
         <v>0.484889808225817</v>
       </c>
-      <c r="AA11" s="2" t="n">
+      <c r="AB11" s="2" t="n">
         <v>0.0120590748985078</v>
       </c>
-      <c r="AB11" s="2" t="n">
+      <c r="AC11" s="2" t="n">
         <v>2.0224987497498</v>
       </c>
-      <c r="AC11" s="2" t="n">
+      <c r="AD11" s="2" t="n">
         <v>177.17</v>
+      </c>
+      <c r="AE11" s="0" t="n">
+        <f aca="false">AD11-AD10</f>
+        <v>19.27</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25729,6 +26030,10 @@
       <c r="F12" s="2" t="n">
         <v>984.279999999999</v>
       </c>
+      <c r="G12" s="0" t="n">
+        <f aca="false">F12-F11</f>
+        <v>99.15</v>
+      </c>
       <c r="I12" s="1" t="s">
         <v>112</v>
       </c>
@@ -25747,6 +26052,10 @@
       <c r="N12" s="2" t="n">
         <v>1929.11</v>
       </c>
+      <c r="O12" s="0" t="n">
+        <f aca="false">N12-N11</f>
+        <v>201.76</v>
+      </c>
       <c r="Q12" s="1" t="s">
         <v>112</v>
       </c>
@@ -25765,23 +26074,31 @@
       <c r="V12" s="2" t="n">
         <v>493.16</v>
       </c>
-      <c r="X12" s="1" t="s">
+      <c r="W12" s="0" t="n">
+        <f aca="false">V12-V11</f>
+        <v>52.799999999999</v>
+      </c>
+      <c r="Y12" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="Y12" s="2" t="n">
+      <c r="Z12" s="2" t="n">
         <v>5.68621616072169</v>
       </c>
-      <c r="Z12" s="2" t="n">
+      <c r="AA12" s="2" t="n">
         <v>0.550729116328858</v>
       </c>
-      <c r="AA12" s="2" t="n">
+      <c r="AB12" s="2" t="n">
         <v>0.0241401540325002</v>
       </c>
-      <c r="AB12" s="2" t="n">
+      <c r="AC12" s="2" t="n">
         <v>2.02111164912474</v>
       </c>
-      <c r="AC12" s="2" t="n">
+      <c r="AD12" s="2" t="n">
         <v>195.99</v>
+      </c>
+      <c r="AE12" s="0" t="n">
+        <f aca="false">AD12-AD11</f>
+        <v>18.82</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25803,6 +26120,10 @@
       <c r="F13" s="2" t="n">
         <v>1083.19</v>
       </c>
+      <c r="G13" s="0" t="n">
+        <f aca="false">F13-F12</f>
+        <v>98.9100000000011</v>
+      </c>
       <c r="I13" s="1" t="s">
         <v>113</v>
       </c>
@@ -25821,6 +26142,10 @@
       <c r="N13" s="2" t="n">
         <v>2130.21</v>
       </c>
+      <c r="O13" s="0" t="n">
+        <f aca="false">N13-N12</f>
+        <v>201.1</v>
+      </c>
       <c r="Q13" s="1" t="s">
         <v>113</v>
       </c>
@@ -25839,23 +26164,31 @@
       <c r="V13" s="2" t="n">
         <v>555.920000000002</v>
       </c>
-      <c r="X13" s="1" t="s">
+      <c r="W13" s="0" t="n">
+        <f aca="false">V13-V12</f>
+        <v>62.760000000002</v>
+      </c>
+      <c r="Y13" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="Y13" s="2" t="n">
+      <c r="Z13" s="2" t="n">
         <v>4.73758688292009</v>
       </c>
-      <c r="Z13" s="2" t="n">
+      <c r="AA13" s="2" t="n">
         <v>0.488527002970693</v>
       </c>
-      <c r="AA13" s="2" t="n">
+      <c r="AB13" s="2" t="n">
         <v>0.0121472607154107</v>
       </c>
-      <c r="AB13" s="2" t="n">
+      <c r="AC13" s="2" t="n">
         <v>2.02271148184962</v>
       </c>
-      <c r="AC13" s="2" t="n">
+      <c r="AD13" s="2" t="n">
         <v>215.120000000001</v>
+      </c>
+      <c r="AE13" s="0" t="n">
+        <f aca="false">AD13-AD12</f>
+        <v>19.130000000001</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25877,6 +26210,10 @@
       <c r="F14" s="2" t="n">
         <v>1183.74</v>
       </c>
+      <c r="G14" s="0" t="n">
+        <f aca="false">F14-F13</f>
+        <v>100.55</v>
+      </c>
       <c r="I14" s="1" t="s">
         <v>114</v>
       </c>
@@ -25895,6 +26232,10 @@
       <c r="N14" s="2" t="n">
         <v>2329.38</v>
       </c>
+      <c r="O14" s="0" t="n">
+        <f aca="false">N14-N13</f>
+        <v>199.17</v>
+      </c>
       <c r="Q14" s="1" t="s">
         <v>114</v>
       </c>
@@ -25913,23 +26254,31 @@
       <c r="V14" s="2" t="n">
         <v>610.59</v>
       </c>
-      <c r="X14" s="1" t="s">
+      <c r="W14" s="0" t="n">
+        <f aca="false">V14-V13</f>
+        <v>54.669999999998</v>
+      </c>
+      <c r="Y14" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="Y14" s="2" t="n">
+      <c r="Z14" s="2" t="n">
         <v>4.81435007595051</v>
       </c>
-      <c r="Z14" s="2" t="n">
+      <c r="AA14" s="2" t="n">
         <v>0.500509530146158</v>
       </c>
-      <c r="AA14" s="2" t="n">
+      <c r="AB14" s="2" t="n">
         <v>0.0146612144728454</v>
       </c>
-      <c r="AB14" s="2" t="n">
+      <c r="AC14" s="2" t="n">
         <v>2.02218110450913</v>
       </c>
-      <c r="AC14" s="2" t="n">
+      <c r="AD14" s="2" t="n">
         <v>234.93</v>
+      </c>
+      <c r="AE14" s="0" t="n">
+        <f aca="false">AD14-AD13</f>
+        <v>19.809999999999</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25951,6 +26300,10 @@
       <c r="F15" s="2" t="n">
         <v>1282.09</v>
       </c>
+      <c r="G15" s="0" t="n">
+        <f aca="false">F15-F14</f>
+        <v>98.3499999999999</v>
+      </c>
       <c r="I15" s="1" t="s">
         <v>115</v>
       </c>
@@ -25969,6 +26322,10 @@
       <c r="N15" s="2" t="n">
         <v>2536.14</v>
       </c>
+      <c r="O15" s="0" t="n">
+        <f aca="false">N15-N14</f>
+        <v>206.76</v>
+      </c>
       <c r="Q15" s="1" t="s">
         <v>115</v>
       </c>
@@ -25987,23 +26344,31 @@
       <c r="V15" s="2" t="n">
         <v>652.950000000001</v>
       </c>
-      <c r="X15" s="1" t="s">
+      <c r="W15" s="0" t="n">
+        <f aca="false">V15-V14</f>
+        <v>42.3600000000009</v>
+      </c>
+      <c r="Y15" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="Y15" s="2" t="n">
+      <c r="Z15" s="2" t="n">
         <v>5.16877539087627</v>
       </c>
-      <c r="Z15" s="2" t="n">
+      <c r="AA15" s="2" t="n">
         <v>0.526115886200987</v>
       </c>
-      <c r="AA15" s="2" t="n">
+      <c r="AB15" s="2" t="n">
         <v>0.0195758104148813</v>
       </c>
-      <c r="AB15" s="2" t="n">
+      <c r="AC15" s="2" t="n">
         <v>2.0214757228493</v>
       </c>
-      <c r="AC15" s="2" t="n">
+      <c r="AD15" s="2" t="n">
         <v>253.65</v>
+      </c>
+      <c r="AE15" s="0" t="n">
+        <f aca="false">AD15-AD14</f>
+        <v>18.72</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26025,6 +26390,10 @@
       <c r="F16" s="2" t="n">
         <v>1381.48</v>
       </c>
+      <c r="G16" s="0" t="n">
+        <f aca="false">F16-F15</f>
+        <v>99.3900000000001</v>
+      </c>
       <c r="I16" s="1" t="s">
         <v>116</v>
       </c>
@@ -26043,6 +26412,10 @@
       <c r="N16" s="2" t="n">
         <v>2731.38</v>
       </c>
+      <c r="O16" s="0" t="n">
+        <f aca="false">N16-N15</f>
+        <v>195.24</v>
+      </c>
       <c r="Q16" s="1" t="s">
         <v>116</v>
       </c>
@@ -26061,23 +26434,31 @@
       <c r="V16" s="2" t="n">
         <v>691.280000000003</v>
       </c>
-      <c r="X16" s="1" t="s">
+      <c r="W16" s="0" t="n">
+        <f aca="false">V16-V15</f>
+        <v>38.3300000000021</v>
+      </c>
+      <c r="Y16" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="Y16" s="2" t="n">
+      <c r="Z16" s="2" t="n">
         <v>4.76757257254872</v>
       </c>
-      <c r="Z16" s="2" t="n">
+      <c r="AA16" s="2" t="n">
         <v>0.494714017032156</v>
       </c>
-      <c r="AA16" s="2" t="n">
+      <c r="AB16" s="2" t="n">
         <v>0.0134696460555681</v>
       </c>
-      <c r="AB16" s="2" t="n">
+      <c r="AC16" s="2" t="n">
         <v>2.02238460546414</v>
       </c>
-      <c r="AC16" s="2" t="n">
+      <c r="AD16" s="2" t="n">
         <v>274.950000000001</v>
+      </c>
+      <c r="AE16" s="0" t="n">
+        <f aca="false">AD16-AD15</f>
+        <v>21.300000000001</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26099,6 +26480,10 @@
       <c r="F17" s="2" t="n">
         <v>1480.85</v>
       </c>
+      <c r="G17" s="0" t="n">
+        <f aca="false">F17-F16</f>
+        <v>99.3699999999999</v>
+      </c>
       <c r="I17" s="1" t="s">
         <v>117</v>
       </c>
@@ -26117,6 +26502,10 @@
       <c r="N17" s="2" t="n">
         <v>2921.38</v>
       </c>
+      <c r="O17" s="0" t="n">
+        <f aca="false">N17-N16</f>
+        <v>190</v>
+      </c>
       <c r="Q17" s="1" t="s">
         <v>117</v>
       </c>
@@ -26135,23 +26524,31 @@
       <c r="V17" s="2" t="n">
         <v>734.82</v>
       </c>
-      <c r="X17" s="1" t="s">
+      <c r="W17" s="0" t="n">
+        <f aca="false">V17-V16</f>
+        <v>43.539999999997</v>
+      </c>
+      <c r="Y17" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="Y17" s="2" t="n">
+      <c r="Z17" s="2" t="n">
         <v>5.22476421829463</v>
       </c>
-      <c r="Z17" s="2" t="n">
+      <c r="AA17" s="2" t="n">
         <v>0.529731302076161</v>
       </c>
-      <c r="AA17" s="2" t="n">
+      <c r="AB17" s="2" t="n">
         <v>0.0199028781415373</v>
       </c>
-      <c r="AB17" s="2" t="n">
+      <c r="AC17" s="2" t="n">
         <v>2.02173496437402</v>
       </c>
-      <c r="AC17" s="2" t="n">
+      <c r="AD17" s="2" t="n">
         <v>296.9</v>
+      </c>
+      <c r="AE17" s="0" t="n">
+        <f aca="false">AD17-AD16</f>
+        <v>21.949999999999</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26173,6 +26570,10 @@
       <c r="F18" s="2" t="n">
         <v>1580.12</v>
       </c>
+      <c r="G18" s="0" t="n">
+        <f aca="false">F18-F17</f>
+        <v>99.27</v>
+      </c>
       <c r="I18" s="1" t="s">
         <v>118</v>
       </c>
@@ -26191,6 +26592,10 @@
       <c r="N18" s="2" t="n">
         <v>3105.83</v>
       </c>
+      <c r="O18" s="0" t="n">
+        <f aca="false">N18-N17</f>
+        <v>184.45</v>
+      </c>
       <c r="Q18" s="1" t="s">
         <v>118</v>
       </c>
@@ -26209,23 +26614,31 @@
       <c r="V18" s="2" t="n">
         <v>786.540000000001</v>
       </c>
-      <c r="X18" s="1" t="s">
+      <c r="W18" s="0" t="n">
+        <f aca="false">V18-V17</f>
+        <v>51.7200000000009</v>
+      </c>
+      <c r="Y18" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="Y18" s="2" t="n">
+      <c r="Z18" s="2" t="n">
         <v>5.81314261535196</v>
       </c>
-      <c r="Z18" s="2" t="n">
+      <c r="AA18" s="2" t="n">
         <v>0.552438666640035</v>
       </c>
-      <c r="AA18" s="2" t="n">
+      <c r="AB18" s="2" t="n">
         <v>0.0260364439741952</v>
       </c>
-      <c r="AB18" s="2" t="n">
+      <c r="AC18" s="2" t="n">
         <v>2.02006521694369</v>
       </c>
-      <c r="AC18" s="2" t="n">
+      <c r="AD18" s="2" t="n">
         <v>314.98</v>
+      </c>
+      <c r="AE18" s="0" t="n">
+        <f aca="false">AD18-AD17</f>
+        <v>18.08</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26247,6 +26660,10 @@
       <c r="F19" s="2" t="n">
         <v>1682.39</v>
       </c>
+      <c r="G19" s="0" t="n">
+        <f aca="false">F19-F18</f>
+        <v>102.27</v>
+      </c>
       <c r="I19" s="1" t="s">
         <v>119</v>
       </c>
@@ -26265,6 +26682,10 @@
       <c r="N19" s="2" t="n">
         <v>3293.46</v>
       </c>
+      <c r="O19" s="0" t="n">
+        <f aca="false">N19-N18</f>
+        <v>187.63</v>
+      </c>
       <c r="Q19" s="1" t="s">
         <v>119</v>
       </c>
@@ -26283,23 +26704,31 @@
       <c r="V19" s="2" t="n">
         <v>828.75</v>
       </c>
-      <c r="X19" s="1" t="s">
+      <c r="W19" s="0" t="n">
+        <f aca="false">V19-V18</f>
+        <v>42.209999999999</v>
+      </c>
+      <c r="Y19" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="Y19" s="2" t="n">
+      <c r="Z19" s="2" t="n">
         <v>5.11984047261926</v>
       </c>
-      <c r="Z19" s="2" t="n">
+      <c r="AA19" s="2" t="n">
         <v>0.5237416884558</v>
       </c>
-      <c r="AA19" s="2" t="n">
+      <c r="AB19" s="2" t="n">
         <v>0.0179299563022002</v>
       </c>
-      <c r="AB19" s="2" t="n">
+      <c r="AC19" s="2" t="n">
         <v>2.0223093658777</v>
       </c>
-      <c r="AC19" s="2" t="n">
+      <c r="AD19" s="2" t="n">
         <v>333.76</v>
+      </c>
+      <c r="AE19" s="0" t="n">
+        <f aca="false">AD19-AD18</f>
+        <v>18.78</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26321,6 +26750,10 @@
       <c r="F20" s="2" t="n">
         <v>1775.63</v>
       </c>
+      <c r="G20" s="0" t="n">
+        <f aca="false">F20-F19</f>
+        <v>93.24</v>
+      </c>
       <c r="I20" s="1" t="s">
         <v>120</v>
       </c>
@@ -26339,6 +26772,10 @@
       <c r="N20" s="2" t="n">
         <v>3496.81</v>
       </c>
+      <c r="O20" s="0" t="n">
+        <f aca="false">N20-N19</f>
+        <v>203.35</v>
+      </c>
       <c r="Q20" s="1" t="s">
         <v>120</v>
       </c>
@@ -26357,23 +26794,31 @@
       <c r="V20" s="2" t="n">
         <v>868.75</v>
       </c>
-      <c r="X20" s="1" t="s">
+      <c r="W20" s="0" t="n">
+        <f aca="false">V20-V19</f>
+        <v>40</v>
+      </c>
+      <c r="Y20" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="Y20" s="2" t="n">
+      <c r="Z20" s="2" t="n">
         <v>5.53061476143937</v>
       </c>
-      <c r="Z20" s="2" t="n">
+      <c r="AA20" s="2" t="n">
         <v>0.544067303981715</v>
       </c>
-      <c r="AA20" s="2" t="n">
+      <c r="AB20" s="2" t="n">
         <v>0.0228259975865514</v>
       </c>
-      <c r="AB20" s="2" t="n">
+      <c r="AC20" s="2" t="n">
         <v>2.02110545965087</v>
       </c>
-      <c r="AC20" s="2" t="n">
+      <c r="AD20" s="2" t="n">
         <v>354.780000000001</v>
+      </c>
+      <c r="AE20" s="0" t="n">
+        <f aca="false">AD20-AD19</f>
+        <v>21.020000000001</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26395,6 +26840,10 @@
       <c r="F21" s="2" t="n">
         <v>1871.51</v>
       </c>
+      <c r="G21" s="0" t="n">
+        <f aca="false">F21-F20</f>
+        <v>95.8799999999999</v>
+      </c>
       <c r="I21" s="1" t="s">
         <v>121</v>
       </c>
@@ -26413,6 +26862,10 @@
       <c r="N21" s="2" t="n">
         <v>3694.92</v>
       </c>
+      <c r="O21" s="0" t="n">
+        <f aca="false">N21-N20</f>
+        <v>198.11</v>
+      </c>
       <c r="Q21" s="1" t="s">
         <v>121</v>
       </c>
@@ -26431,23 +26884,31 @@
       <c r="V21" s="2" t="n">
         <v>910.050000000003</v>
       </c>
-      <c r="X21" s="1" t="s">
+      <c r="W21" s="0" t="n">
+        <f aca="false">V21-V20</f>
+        <v>41.300000000003</v>
+      </c>
+      <c r="Y21" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="Y21" s="2" t="n">
+      <c r="Z21" s="2" t="n">
         <v>5.2828873580718</v>
       </c>
-      <c r="Z21" s="2" t="n">
+      <c r="AA21" s="2" t="n">
         <v>0.530037021685518</v>
       </c>
-      <c r="AA21" s="2" t="n">
+      <c r="AB21" s="2" t="n">
         <v>0.021010595448446</v>
       </c>
-      <c r="AB21" s="2" t="n">
+      <c r="AC21" s="2" t="n">
         <v>2.0205822677958</v>
       </c>
-      <c r="AC21" s="2" t="n">
+      <c r="AD21" s="2" t="n">
         <v>374.030000000001</v>
+      </c>
+      <c r="AE21" s="0" t="n">
+        <f aca="false">AD21-AD20</f>
+        <v>19.25</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26469,6 +26930,10 @@
       <c r="F22" s="2" t="n">
         <v>1970.68</v>
       </c>
+      <c r="G22" s="0" t="n">
+        <f aca="false">F22-F21</f>
+        <v>99.1700000000001</v>
+      </c>
       <c r="I22" s="1" t="s">
         <v>122</v>
       </c>
@@ -26487,6 +26952,10 @@
       <c r="N22" s="2" t="n">
         <v>3894.3</v>
       </c>
+      <c r="O22" s="0" t="n">
+        <f aca="false">N22-N21</f>
+        <v>199.38</v>
+      </c>
       <c r="Q22" s="1" t="s">
         <v>122</v>
       </c>
@@ -26505,23 +26974,31 @@
       <c r="V22" s="2" t="n">
         <v>960.57</v>
       </c>
-      <c r="X22" s="1" t="s">
+      <c r="W22" s="0" t="n">
+        <f aca="false">V22-V21</f>
+        <v>50.519999999997</v>
+      </c>
+      <c r="Y22" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="Y22" s="2" t="n">
+      <c r="Z22" s="2" t="n">
         <v>4.86966307436344</v>
       </c>
-      <c r="Z22" s="2" t="n">
+      <c r="AA22" s="2" t="n">
         <v>0.502964956823651</v>
       </c>
-      <c r="AA22" s="2" t="n">
+      <c r="AB22" s="2" t="n">
         <v>0.0156250656601103</v>
       </c>
-      <c r="AB22" s="2" t="n">
+      <c r="AC22" s="2" t="n">
         <v>2.02172328591852</v>
       </c>
-      <c r="AC22" s="2" t="n">
+      <c r="AD22" s="2" t="n">
         <v>393.49</v>
+      </c>
+      <c r="AE22" s="0" t="n">
+        <f aca="false">AD22-AD21</f>
+        <v>19.459999999999</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26543,6 +27020,10 @@
       <c r="F23" s="2" t="n">
         <v>2066</v>
       </c>
+      <c r="G23" s="0" t="n">
+        <f aca="false">F23-F22</f>
+        <v>95.3199999999999</v>
+      </c>
       <c r="I23" s="1" t="s">
         <v>123</v>
       </c>
@@ -26561,6 +27042,10 @@
       <c r="N23" s="2" t="n">
         <v>4093.77</v>
       </c>
+      <c r="O23" s="0" t="n">
+        <f aca="false">N23-N22</f>
+        <v>199.47</v>
+      </c>
       <c r="Q23" s="1" t="s">
         <v>123</v>
       </c>
@@ -26579,23 +27064,31 @@
       <c r="V23" s="2" t="n">
         <v>1000.8</v>
       </c>
-      <c r="X23" s="1" t="s">
+      <c r="W23" s="0" t="n">
+        <f aca="false">V23-V22</f>
+        <v>40.2299999999999</v>
+      </c>
+      <c r="Y23" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="Y23" s="2" t="n">
+      <c r="Z23" s="2" t="n">
         <v>5.6917015780514</v>
       </c>
-      <c r="Z23" s="2" t="n">
+      <c r="AA23" s="2" t="n">
         <v>0.551282825258859</v>
       </c>
-      <c r="AA23" s="2" t="n">
+      <c r="AB23" s="2" t="n">
         <v>0.0238474547305066</v>
       </c>
-      <c r="AB23" s="2" t="n">
+      <c r="AC23" s="2" t="n">
         <v>2.02155054029698</v>
       </c>
-      <c r="AC23" s="2" t="n">
+      <c r="AD23" s="2" t="n">
         <v>412.27</v>
+      </c>
+      <c r="AE23" s="0" t="n">
+        <f aca="false">AD23-AD22</f>
+        <v>18.78</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26617,6 +27110,10 @@
       <c r="F24" s="2" t="n">
         <v>2166.31</v>
       </c>
+      <c r="G24" s="0" t="n">
+        <f aca="false">F24-F23</f>
+        <v>100.31</v>
+      </c>
       <c r="I24" s="1" t="s">
         <v>124</v>
       </c>
@@ -26635,6 +27132,10 @@
       <c r="N24" s="2" t="n">
         <v>4291.26</v>
       </c>
+      <c r="O24" s="0" t="n">
+        <f aca="false">N24-N23</f>
+        <v>197.49</v>
+      </c>
       <c r="Q24" s="1" t="s">
         <v>124</v>
       </c>
@@ -26653,23 +27154,31 @@
       <c r="V24" s="2" t="n">
         <v>1049.83</v>
       </c>
-      <c r="X24" s="1" t="s">
+      <c r="W24" s="0" t="n">
+        <f aca="false">V24-V23</f>
+        <v>49.03</v>
+      </c>
+      <c r="Y24" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="Y24" s="2" t="n">
+      <c r="Z24" s="2" t="n">
         <v>4.75295112455731</v>
       </c>
-      <c r="Z24" s="2" t="n">
+      <c r="AA24" s="2" t="n">
         <v>0.491596896089408</v>
       </c>
-      <c r="AA24" s="2" t="n">
+      <c r="AB24" s="2" t="n">
         <v>0.0129265590049605</v>
       </c>
-      <c r="AB24" s="2" t="n">
+      <c r="AC24" s="2" t="n">
         <v>2.02249915173666</v>
       </c>
-      <c r="AC24" s="2" t="n">
+      <c r="AD24" s="2" t="n">
         <v>430.85</v>
+      </c>
+      <c r="AE24" s="0" t="n">
+        <f aca="false">AD24-AD23</f>
+        <v>18.58</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26691,6 +27200,10 @@
       <c r="F25" s="2" t="n">
         <v>2265.93</v>
       </c>
+      <c r="G25" s="0" t="n">
+        <f aca="false">F25-F24</f>
+        <v>99.6199999999999</v>
+      </c>
       <c r="I25" s="1" t="s">
         <v>125</v>
       </c>
@@ -26709,6 +27222,10 @@
       <c r="N25" s="2" t="n">
         <v>4482.82</v>
       </c>
+      <c r="O25" s="0" t="n">
+        <f aca="false">N25-N24</f>
+        <v>191.56</v>
+      </c>
       <c r="Q25" s="1" t="s">
         <v>125</v>
       </c>
@@ -26727,23 +27244,31 @@
       <c r="V25" s="2" t="n">
         <v>1099.35</v>
       </c>
-      <c r="X25" s="1" t="s">
+      <c r="W25" s="0" t="n">
+        <f aca="false">V25-V24</f>
+        <v>49.52</v>
+      </c>
+      <c r="Y25" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="Y25" s="2" t="n">
+      <c r="Z25" s="2" t="n">
         <v>5.79493054981968</v>
       </c>
-      <c r="Z25" s="2" t="n">
+      <c r="AA25" s="2" t="n">
         <v>0.552679315673452</v>
       </c>
-      <c r="AA25" s="2" t="n">
+      <c r="AB25" s="2" t="n">
         <v>0.0257898341104866</v>
       </c>
-      <c r="AB25" s="2" t="n">
+      <c r="AC25" s="2" t="n">
         <v>2.02039586868464</v>
       </c>
-      <c r="AC25" s="2" t="n">
+      <c r="AD25" s="2" t="n">
         <v>449.73</v>
+      </c>
+      <c r="AE25" s="0" t="n">
+        <f aca="false">AD25-AD24</f>
+        <v>18.88</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26765,6 +27290,10 @@
       <c r="F26" s="2" t="n">
         <v>2365.77</v>
       </c>
+      <c r="G26" s="0" t="n">
+        <f aca="false">F26-F25</f>
+        <v>99.8400000000002</v>
+      </c>
       <c r="I26" s="1" t="s">
         <v>126</v>
       </c>
@@ -26783,6 +27312,10 @@
       <c r="N26" s="2" t="n">
         <v>4668.56</v>
       </c>
+      <c r="O26" s="0" t="n">
+        <f aca="false">N26-N25</f>
+        <v>185.740000000001</v>
+      </c>
       <c r="Q26" s="1" t="s">
         <v>126</v>
       </c>
@@ -26801,23 +27334,31 @@
       <c r="V26" s="2" t="n">
         <v>1151.84</v>
       </c>
-      <c r="X26" s="1" t="s">
+      <c r="W26" s="0" t="n">
+        <f aca="false">V26-V25</f>
+        <v>52.49</v>
+      </c>
+      <c r="Y26" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="Y26" s="2" t="n">
+      <c r="Z26" s="2" t="n">
         <v>5.00942022103225</v>
       </c>
-      <c r="Z26" s="2" t="n">
+      <c r="AA26" s="2" t="n">
         <v>0.517117055651651</v>
       </c>
-      <c r="AA26" s="2" t="n">
+      <c r="AB26" s="2" t="n">
         <v>0.0175787935517858</v>
       </c>
-      <c r="AB26" s="2" t="n">
+      <c r="AC26" s="2" t="n">
         <v>2.02182923249266</v>
       </c>
-      <c r="AC26" s="2" t="n">
+      <c r="AD26" s="2" t="n">
         <v>469.289999999999</v>
+      </c>
+      <c r="AE26" s="0" t="n">
+        <f aca="false">AD26-AD25</f>
+        <v>19.559999999999</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26839,6 +27380,10 @@
       <c r="F27" s="2" t="n">
         <v>2460.03</v>
       </c>
+      <c r="G27" s="0" t="n">
+        <f aca="false">F27-F26</f>
+        <v>94.2600000000002</v>
+      </c>
       <c r="I27" s="1" t="s">
         <v>127</v>
       </c>
@@ -26857,6 +27402,10 @@
       <c r="N27" s="2" t="n">
         <v>4867.8</v>
       </c>
+      <c r="O27" s="0" t="n">
+        <f aca="false">N27-N26</f>
+        <v>199.24</v>
+      </c>
       <c r="Q27" s="1" t="s">
         <v>127</v>
       </c>
@@ -26875,23 +27424,31 @@
       <c r="V27" s="2" t="n">
         <v>1201.69</v>
       </c>
-      <c r="X27" s="1" t="s">
+      <c r="W27" s="0" t="n">
+        <f aca="false">V27-V26</f>
+        <v>49.8500000000001</v>
+      </c>
+      <c r="Y27" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="Y27" s="2" t="n">
+      <c r="Z27" s="2" t="n">
         <v>4.73365937265043</v>
       </c>
-      <c r="Z27" s="2" t="n">
+      <c r="AA27" s="2" t="n">
         <v>0.483673565939086</v>
       </c>
-      <c r="AA27" s="2" t="n">
+      <c r="AB27" s="2" t="n">
         <v>0.0111067789602397</v>
       </c>
-      <c r="AB27" s="2" t="n">
+      <c r="AC27" s="2" t="n">
         <v>2.02299936744483</v>
       </c>
-      <c r="AC27" s="2" t="n">
+      <c r="AD27" s="2" t="n">
         <v>489.35</v>
+      </c>
+      <c r="AE27" s="0" t="n">
+        <f aca="false">AD27-AD26</f>
+        <v>20.060000000001</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26913,6 +27470,10 @@
       <c r="F28" s="2" t="n">
         <v>2553.17</v>
       </c>
+      <c r="G28" s="0" t="n">
+        <f aca="false">F28-F27</f>
+        <v>93.1399999999999</v>
+      </c>
       <c r="I28" s="1" t="s">
         <v>128</v>
       </c>
@@ -26931,6 +27492,10 @@
       <c r="N28" s="2" t="n">
         <v>5061.42</v>
       </c>
+      <c r="O28" s="0" t="n">
+        <f aca="false">N28-N27</f>
+        <v>193.62</v>
+      </c>
       <c r="Q28" s="1" t="s">
         <v>128</v>
       </c>
@@ -26949,23 +27514,31 @@
       <c r="V28" s="2" t="n">
         <v>1248.62</v>
       </c>
-      <c r="X28" s="1" t="s">
+      <c r="W28" s="0" t="n">
+        <f aca="false">V28-V27</f>
+        <v>46.9299999999998</v>
+      </c>
+      <c r="Y28" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="Y28" s="2" t="n">
+      <c r="Z28" s="2" t="n">
         <v>4.99188121808989</v>
       </c>
-      <c r="Z28" s="2" t="n">
+      <c r="AA28" s="2" t="n">
         <v>0.51621370105816</v>
       </c>
-      <c r="AA28" s="2" t="n">
+      <c r="AB28" s="2" t="n">
         <v>0.0171909710769401</v>
       </c>
-      <c r="AB28" s="2" t="n">
+      <c r="AC28" s="2" t="n">
         <v>2.02205879088233</v>
       </c>
-      <c r="AC28" s="2" t="n">
+      <c r="AD28" s="2" t="n">
         <v>509.4</v>
+      </c>
+      <c r="AE28" s="0" t="n">
+        <f aca="false">AD28-AD27</f>
+        <v>20.05</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26987,6 +27560,10 @@
       <c r="F29" s="2" t="n">
         <v>2645.86</v>
       </c>
+      <c r="G29" s="0" t="n">
+        <f aca="false">F29-F28</f>
+        <v>92.6900000000001</v>
+      </c>
       <c r="I29" s="1" t="s">
         <v>129</v>
       </c>
@@ -27005,6 +27582,10 @@
       <c r="N29" s="2" t="n">
         <v>5254.36</v>
       </c>
+      <c r="O29" s="0" t="n">
+        <f aca="false">N29-N28</f>
+        <v>192.94</v>
+      </c>
       <c r="Q29" s="1" t="s">
         <v>129</v>
       </c>
@@ -27023,23 +27604,31 @@
       <c r="V29" s="2" t="n">
         <v>1291.8</v>
       </c>
-      <c r="X29" s="1" t="s">
+      <c r="W29" s="0" t="n">
+        <f aca="false">V29-V28</f>
+        <v>43.1800000000001</v>
+      </c>
+      <c r="Y29" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="Y29" s="2" t="n">
+      <c r="Z29" s="2" t="n">
         <v>4.73910454348866</v>
       </c>
-      <c r="Z29" s="2" t="n">
+      <c r="AA29" s="2" t="n">
         <v>0.488627287987745</v>
       </c>
-      <c r="AA29" s="2" t="n">
+      <c r="AB29" s="2" t="n">
         <v>0.012247400967034</v>
       </c>
-      <c r="AB29" s="2" t="n">
+      <c r="AC29" s="2" t="n">
         <v>2.02262960575295</v>
       </c>
-      <c r="AC29" s="2" t="n">
+      <c r="AD29" s="2" t="n">
         <v>529.93</v>
+      </c>
+      <c r="AE29" s="0" t="n">
+        <f aca="false">AD29-AD28</f>
+        <v>20.53</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27061,6 +27650,10 @@
       <c r="F30" s="2" t="n">
         <v>2738.61</v>
       </c>
+      <c r="G30" s="0" t="n">
+        <f aca="false">F30-F29</f>
+        <v>92.75</v>
+      </c>
       <c r="I30" s="1" t="s">
         <v>130</v>
       </c>
@@ -27079,6 +27672,10 @@
       <c r="N30" s="2" t="n">
         <v>5446.92</v>
       </c>
+      <c r="O30" s="0" t="n">
+        <f aca="false">N30-N29</f>
+        <v>192.56</v>
+      </c>
       <c r="Q30" s="1" t="s">
         <v>130</v>
       </c>
@@ -27097,23 +27694,31 @@
       <c r="V30" s="2" t="n">
         <v>1341.08</v>
       </c>
-      <c r="X30" s="1" t="s">
+      <c r="W30" s="0" t="n">
+        <f aca="false">V30-V29</f>
+        <v>49.28</v>
+      </c>
+      <c r="Y30" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="Y30" s="2" t="n">
+      <c r="Z30" s="2" t="n">
         <v>5.54636459222882</v>
       </c>
-      <c r="Z30" s="2" t="n">
+      <c r="AA30" s="2" t="n">
         <v>0.450301525598511</v>
       </c>
-      <c r="AA30" s="2" t="n">
+      <c r="AB30" s="2" t="n">
         <v>0.00439832399308458</v>
       </c>
-      <c r="AB30" s="2" t="n">
+      <c r="AC30" s="2" t="n">
         <v>2.02623292995681</v>
       </c>
-      <c r="AC30" s="2" t="n">
+      <c r="AD30" s="2" t="n">
         <v>548.75</v>
+      </c>
+      <c r="AE30" s="0" t="n">
+        <f aca="false">AD30-AD29</f>
+        <v>18.8200000000001</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27135,6 +27740,10 @@
       <c r="F31" s="2" t="n">
         <v>2833.84</v>
       </c>
+      <c r="G31" s="0" t="n">
+        <f aca="false">F31-F30</f>
+        <v>95.23</v>
+      </c>
       <c r="I31" s="1" t="s">
         <v>131</v>
       </c>
@@ -27153,6 +27762,10 @@
       <c r="N31" s="2" t="n">
         <v>5633.46</v>
       </c>
+      <c r="O31" s="0" t="n">
+        <f aca="false">N31-N30</f>
+        <v>186.54</v>
+      </c>
       <c r="Q31" s="1" t="s">
         <v>131</v>
       </c>
@@ -27171,23 +27784,31 @@
       <c r="V31" s="2" t="n">
         <v>1391.8</v>
       </c>
-      <c r="X31" s="1" t="s">
+      <c r="W31" s="0" t="n">
+        <f aca="false">V31-V30</f>
+        <v>50.72</v>
+      </c>
+      <c r="Y31" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="Y31" s="2" t="n">
+      <c r="Z31" s="2" t="n">
         <v>8.71009886078587</v>
       </c>
-      <c r="Z31" s="2" t="n">
+      <c r="AA31" s="2" t="n">
         <v>0.628011529441782</v>
       </c>
-      <c r="AA31" s="2" t="n">
+      <c r="AB31" s="2" t="n">
         <v>0.0485381822999904</v>
       </c>
-      <c r="AB31" s="2" t="n">
+      <c r="AC31" s="2" t="n">
         <v>2.01471658138896</v>
       </c>
-      <c r="AC31" s="2" t="n">
+      <c r="AD31" s="2" t="n">
         <v>567.440000000001</v>
+      </c>
+      <c r="AE31" s="0" t="n">
+        <f aca="false">AD31-AD30</f>
+        <v>18.690000000001</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27209,6 +27830,10 @@
       <c r="F32" s="2" t="n">
         <v>2942.52</v>
       </c>
+      <c r="G32" s="0" t="n">
+        <f aca="false">F32-F31</f>
+        <v>108.68</v>
+      </c>
       <c r="I32" s="1" t="s">
         <v>132</v>
       </c>
@@ -27227,6 +27852,10 @@
       <c r="N32" s="2" t="n">
         <v>5819.25</v>
       </c>
+      <c r="O32" s="0" t="n">
+        <f aca="false">N32-N31</f>
+        <v>185.79</v>
+      </c>
       <c r="Q32" s="1" t="s">
         <v>132</v>
       </c>
@@ -27245,23 +27874,31 @@
       <c r="V32" s="2" t="n">
         <v>1438.69</v>
       </c>
-      <c r="X32" s="1" t="s">
+      <c r="W32" s="0" t="n">
+        <f aca="false">V32-V31</f>
+        <v>46.8900000000001</v>
+      </c>
+      <c r="Y32" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="Y32" s="2" t="n">
+      <c r="Z32" s="2" t="n">
         <v>5.29161793897107</v>
       </c>
-      <c r="Z32" s="2" t="n">
+      <c r="AA32" s="2" t="n">
         <v>0.532915414088237</v>
       </c>
-      <c r="AA32" s="2" t="n">
+      <c r="AB32" s="2" t="n">
         <v>0.0200434216808821</v>
       </c>
-      <c r="AB32" s="2" t="n">
+      <c r="AC32" s="2" t="n">
         <v>2.02112866865988</v>
       </c>
-      <c r="AC32" s="2" t="n">
+      <c r="AD32" s="2" t="n">
         <v>586.110000000001</v>
+      </c>
+      <c r="AE32" s="0" t="n">
+        <f aca="false">AD32-AD31</f>
+        <v>18.6700000000001</v>
       </c>
     </row>
   </sheetData>
@@ -27276,13 +27913,13 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="M15" activeCellId="0" sqref="M15"/>
     </sheetView>
   </sheetViews>
@@ -27328,10 +27965,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="2" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28486,19 +29123,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AC32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="6.71"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29180,19 +29817,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="7.98"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
add min and average obj and time
</commit_message>
<xml_diff>
--- a/results_from_all_algos.xlsx
+++ b/results_from_all_algos.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="159">
   <si>
     <t xml:space="preserve">ITER#</t>
   </si>
@@ -491,6 +491,12 @@
     <t xml:space="preserve">r09</t>
   </si>
   <si>
+    <t xml:space="preserve">MIN:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AVG:</t>
+  </si>
+  <si>
     <t xml:space="preserve">Population 40</t>
   </si>
   <si>
@@ -504,7 +510,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -532,6 +538,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -576,7 +587,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -586,6 +597,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -25083,18 +25098,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AE32"/>
+  <dimension ref="A1:AE35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="bottomRight" activeCell="A34" activeCellId="0" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="10.65"/>
   </cols>
   <sheetData>
@@ -27899,6 +27916,121 @@
       <c r="AE32" s="0" t="n">
         <f aca="false">AD32-AD31</f>
         <v>18.6700000000001</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <f aca="false">MIN(B3:B32)</f>
+        <v>4.73248753274178</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="G34" s="0" t="n">
+        <f aca="false">MIN(G3:G32)</f>
+        <v>92.51</v>
+      </c>
+      <c r="I34" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="J34" s="3" t="n">
+        <v>4.73248753274178</v>
+      </c>
+      <c r="N34" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="O34" s="0" t="n">
+        <f aca="false">MIN(O3:O32)</f>
+        <v>184.45</v>
+      </c>
+      <c r="Q34" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="R34" s="0" t="n">
+        <f aca="false">MIN(R3:R32)</f>
+        <v>4.7331248630718</v>
+      </c>
+      <c r="V34" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="W34" s="0" t="n">
+        <f aca="false">MIN(W3:W32)</f>
+        <v>38.3300000000021</v>
+      </c>
+      <c r="Y34" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z34" s="0" t="n">
+        <f aca="false">MIN(Z3:Z32)</f>
+        <v>4.73365937265043</v>
+      </c>
+      <c r="AD34" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="AE34" s="0" t="n">
+        <f aca="false">MIN(AE3:AE32)</f>
+        <v>18.08</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <f aca="false">AVERAGE(B3:B32)</f>
+        <v>4.73756836745389</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="G35" s="0" t="n">
+        <f aca="false">AVERAGE(G3:G32)</f>
+        <v>98.084</v>
+      </c>
+      <c r="I35" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="J35" s="0" t="n">
+        <f aca="false">AVERAGE(J3:J32)</f>
+        <v>4.74954683785947</v>
+      </c>
+      <c r="N35" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="O35" s="0" t="n">
+        <f aca="false">AVERAGE(O3:O32)</f>
+        <v>193.975</v>
+      </c>
+      <c r="Q35" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="R35" s="0" t="n">
+        <f aca="false">AVERAGE(R3:R32)</f>
+        <v>7.80846874577006</v>
+      </c>
+      <c r="V35" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="W35" s="0" t="n">
+        <f aca="false">AVERAGE(W3:W32)</f>
+        <v>47.9563333333333</v>
+      </c>
+      <c r="Y35" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="Z35" s="0" t="n">
+        <f aca="false">AVERAGE(Z3:Z32)</f>
+        <v>5.3321773375202</v>
+      </c>
+      <c r="AD35" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="AE35" s="0" t="n">
+        <f aca="false">AVERAGE(AE3:AE32)</f>
+        <v>19.537</v>
       </c>
     </row>
   </sheetData>
@@ -27965,10 +28097,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="2" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
WOA results sorted and times saved as literals
</commit_message>
<xml_diff>
--- a/results_from_all_algos.xlsx
+++ b/results_from_all_algos.xlsx
@@ -8,11 +8,11 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="WOA_CONV" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="WOA_RESULTS" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="GA" sheetId="3" state="visible" r:id="rId5"/>
-    <sheet name="SA" sheetId="4" state="visible" r:id="rId6"/>
-    <sheet name="CSA" sheetId="5" state="visible" r:id="rId7"/>
+    <sheet name="WOA_CONV" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="WOA_RESULTS" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="GA" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="SA" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="CSA" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -464,31 +464,31 @@
     <t xml:space="preserve">Agents 300 iters 30</t>
   </si>
   <si>
-    <t xml:space="preserve">r01</t>
-  </si>
-  <si>
     <t xml:space="preserve">r02</t>
   </si>
   <si>
     <t xml:space="preserve">r03</t>
   </si>
   <si>
-    <t xml:space="preserve">r04</t>
+    <t xml:space="preserve">r05</t>
   </si>
   <si>
-    <t xml:space="preserve">r05</t>
+    <t xml:space="preserve">r09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r08</t>
   </si>
   <si>
     <t xml:space="preserve">r06</t>
   </si>
   <si>
-    <t xml:space="preserve">r07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">r08</t>
-  </si>
-  <si>
-    <t xml:space="preserve">r09</t>
+    <t xml:space="preserve">r04</t>
   </si>
   <si>
     <t xml:space="preserve">MIN:</t>
@@ -507,10 +507,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -538,11 +539,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -587,7 +583,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -600,7 +596,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -617,7 +617,7 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <bgColor rgb="FF000000"/>
+          <fgColor rgb="00FFFFFF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -625,120 +625,14 @@
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
-  <a:themeElements>
-    <a:clrScheme name="LibreOffice">
-      <a:dk1>
-        <a:srgbClr val="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:srgbClr val="ffffff"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="000000"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="ffffff"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="18a303"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="0369a3"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="a33e03"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8e03a3"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="c99c00"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="c9211e"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000ee"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="551a8b"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme>
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:CW132"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="Y2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="Y1" activeCellId="0" sqref="Y1"/>
@@ -746,7 +640,7 @@
       <selection pane="bottomRight" activeCell="B102" activeCellId="0" sqref="B102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="6.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.77"/>
   </cols>
@@ -25094,25 +24988,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AE35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topRight" activeCell="H1" activeCellId="0" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A34" activeCellId="0" sqref="A34"/>
+      <selection pane="bottomRight" activeCell="N26" activeCellId="0" sqref="N26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="6.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="10.65"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="6.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="8.37"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="15" min="15" style="3" width="6.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="23" min="23" style="3" width="6.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="31" min="31" style="3" width="6.53"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25131,7 +25029,7 @@
       <c r="F1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>141</v>
       </c>
       <c r="J1" s="1" t="s">
@@ -25149,7 +25047,7 @@
       <c r="N1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="4" t="s">
         <v>141</v>
       </c>
       <c r="R1" s="1" t="s">
@@ -25167,7 +25065,7 @@
       <c r="V1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="4" t="s">
         <v>141</v>
       </c>
       <c r="Z1" s="1" t="s">
@@ -25185,7 +25083,7 @@
       <c r="AD1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AE1" s="4" t="s">
         <v>141</v>
       </c>
     </row>
@@ -25220,97 +25118,93 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>4.73282705256699</v>
+        <v>4.73248753274178</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>0.483995014449269</v>
+        <v>0.48485401527131</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>0.0112592656129446</v>
+        <v>0.0114020830898292</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>2.02294816843838</v>
+        <v>2.022881086327</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>113.549999999999</v>
-      </c>
-      <c r="G3" s="0" t="n">
-        <f aca="false">F3-F2</f>
-        <v>113.549999999999</v>
+        <v>1580.12</v>
+      </c>
+      <c r="G3" s="3" t="n">
+        <v>99.27</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>146</v>
+        <v>117</v>
       </c>
       <c r="J3" s="2" t="n">
-        <v>4.73384437044199</v>
+        <v>4.73241918756398</v>
       </c>
       <c r="K3" s="2" t="n">
-        <v>0.486686723823064</v>
+        <v>0.484993264429524</v>
       </c>
       <c r="L3" s="2" t="n">
-        <v>0.0117550885940693</v>
+        <v>0.0114695858242343</v>
       </c>
       <c r="M3" s="2" t="n">
-        <v>2.0227828178733</v>
+        <v>2.02284937300368</v>
       </c>
       <c r="N3" s="2" t="n">
-        <v>200.299999999999</v>
-      </c>
-      <c r="O3" s="0" t="n">
-        <f aca="false">N3-N2</f>
-        <v>200.299999999999</v>
+        <v>2921.38</v>
+      </c>
+      <c r="O3" s="3" t="n">
+        <v>190</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>146</v>
+        <v>121</v>
       </c>
       <c r="R3" s="2" t="n">
-        <v>10.7344618261651</v>
+        <v>4.7331248630718</v>
       </c>
       <c r="S3" s="2" t="n">
-        <v>0.70250555215571</v>
+        <v>0.485272347057502</v>
       </c>
       <c r="T3" s="2" t="n">
-        <v>0.0639060190144499</v>
+        <v>0.011406013099693</v>
       </c>
       <c r="U3" s="2" t="n">
-        <v>2.01687084448769</v>
+        <v>2.02293723685077</v>
       </c>
       <c r="V3" s="2" t="n">
-        <v>49.380000000001</v>
-      </c>
-      <c r="W3" s="0" t="n">
-        <f aca="false">V3-V2</f>
-        <v>49.380000000001</v>
+        <v>910.050000000003</v>
+      </c>
+      <c r="W3" s="3" t="n">
+        <v>41.3</v>
       </c>
       <c r="Y3" s="1" t="s">
-        <v>146</v>
+        <v>127</v>
       </c>
       <c r="Z3" s="2" t="n">
-        <v>6.69584862019204</v>
+        <v>4.73365937265043</v>
       </c>
       <c r="AA3" s="2" t="n">
-        <v>0.573781261508616</v>
+        <v>0.483673565939086</v>
       </c>
       <c r="AB3" s="2" t="n">
-        <v>0.0333309402681</v>
+        <v>0.0111067789602397</v>
       </c>
       <c r="AC3" s="2" t="n">
-        <v>2.01851960457967</v>
+        <v>2.02299936744483</v>
       </c>
       <c r="AD3" s="2" t="n">
-        <v>22.7600000000002</v>
-      </c>
-      <c r="AE3" s="0" t="n">
-        <f aca="false">AD3-AD2</f>
-        <v>22.7600000000002</v>
+        <v>489.35</v>
+      </c>
+      <c r="AE3" s="3" t="n">
+        <v>20.1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>4.73251624066684</v>
@@ -25327,440 +25221,420 @@
       <c r="F4" s="2" t="n">
         <v>211.469999999999</v>
       </c>
-      <c r="G4" s="0" t="n">
-        <f aca="false">F4-F3</f>
+      <c r="G4" s="3" t="n">
         <v>97.92</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>147</v>
+        <v>125</v>
       </c>
       <c r="J4" s="2" t="n">
-        <v>4.84794027256065</v>
+        <v>4.73258144253468</v>
       </c>
       <c r="K4" s="2" t="n">
-        <v>0.501964506312286</v>
+        <v>0.485378310158194</v>
       </c>
       <c r="L4" s="2" t="n">
-        <v>0.0152840476580599</v>
+        <v>0.0114412614119393</v>
       </c>
       <c r="M4" s="2" t="n">
-        <v>2.02184590448036</v>
+        <v>2.02289234955163</v>
       </c>
       <c r="N4" s="2" t="n">
-        <v>391.849999999999</v>
-      </c>
-      <c r="O4" s="0" t="n">
-        <f aca="false">N4-N3</f>
-        <v>191.55</v>
+        <v>4482.82</v>
+      </c>
+      <c r="O4" s="3" t="n">
+        <v>191.56</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>147</v>
+        <v>116</v>
       </c>
       <c r="R4" s="2" t="n">
-        <v>14.5297619190541</v>
+        <v>4.73468742483637</v>
       </c>
       <c r="S4" s="2" t="n">
-        <v>0.762478631397603</v>
+        <v>0.487292801271241</v>
       </c>
       <c r="T4" s="2" t="n">
-        <v>0.0953098289247004</v>
+        <v>0.0118434914597135</v>
       </c>
       <c r="U4" s="2" t="n">
-        <v>2.01261747116299</v>
+        <v>2.0228137742823</v>
       </c>
       <c r="V4" s="2" t="n">
-        <v>103.880000000001</v>
-      </c>
-      <c r="W4" s="0" t="n">
-        <f aca="false">V4-V3</f>
-        <v>54.5</v>
+        <v>691.280000000003</v>
+      </c>
+      <c r="W4" s="3" t="n">
+        <v>38.3</v>
       </c>
       <c r="Y4" s="1" t="s">
         <v>147</v>
       </c>
       <c r="Z4" s="2" t="n">
-        <v>4.93002892499933</v>
+        <v>4.73609256977679</v>
       </c>
       <c r="AA4" s="2" t="n">
-        <v>0.510256231968616</v>
+        <v>0.487641598070697</v>
       </c>
       <c r="AB4" s="2" t="n">
-        <v>0.0167051762212759</v>
+        <v>0.0120176090070576</v>
       </c>
       <c r="AC4" s="2" t="n">
-        <v>2.02173487369732</v>
+        <v>2.02271261361793</v>
       </c>
       <c r="AD4" s="2" t="n">
-        <v>43.3400000000001</v>
-      </c>
-      <c r="AE4" s="0" t="n">
-        <f aca="false">AD4-AD3</f>
-        <v>20.5799999999999</v>
+        <v>62.2899999999991</v>
+      </c>
+      <c r="AE4" s="3" t="n">
+        <v>18.9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>148</v>
+        <v>116</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>4.73750625719472</v>
+        <v>4.73255095728732</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>0.488255319227011</v>
+        <v>0.485266574729285</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>0.0121396899075259</v>
+        <v>0.0114431495749795</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>2.02269208900668</v>
+        <v>2.02299536134802</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>305</v>
-      </c>
-      <c r="G5" s="0" t="n">
-        <f aca="false">F5-F4</f>
-        <v>93.530000000001</v>
+        <v>1381.48</v>
+      </c>
+      <c r="G5" s="3" t="n">
+        <v>99.3900000000001</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="J5" s="2" t="n">
-        <v>4.73605216732573</v>
+        <v>4.73271698603789</v>
       </c>
       <c r="K5" s="2" t="n">
-        <v>0.481902460643336</v>
+        <v>0.485055177965332</v>
       </c>
       <c r="L5" s="2" t="n">
-        <v>0.0107935163956716</v>
+        <v>0.0114707863057356</v>
       </c>
       <c r="M5" s="2" t="n">
-        <v>2.02304612788988</v>
+        <v>2.02285745534938</v>
       </c>
       <c r="N5" s="2" t="n">
-        <v>580.74</v>
-      </c>
-      <c r="O5" s="0" t="n">
-        <f aca="false">N5-N4</f>
-        <v>188.890000000001</v>
+        <v>5446.92</v>
+      </c>
+      <c r="O5" s="3" t="n">
+        <v>192.56</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>148</v>
+        <v>120</v>
       </c>
       <c r="R5" s="2" t="n">
-        <v>4.84804171549978</v>
+        <v>4.75755084223834</v>
       </c>
       <c r="S5" s="2" t="n">
-        <v>0.504907264556651</v>
+        <v>0.4937422846595</v>
       </c>
       <c r="T5" s="2" t="n">
-        <v>0.0151636060931207</v>
+        <v>0.0130622540715576</v>
       </c>
       <c r="U5" s="2" t="n">
-        <v>2.0222645194372</v>
+        <v>2.02259009753887</v>
       </c>
       <c r="V5" s="2" t="n">
-        <v>145.140000000003</v>
-      </c>
-      <c r="W5" s="0" t="n">
-        <f aca="false">V5-V4</f>
-        <v>41.260000000002</v>
+        <v>868.75</v>
+      </c>
+      <c r="W5" s="3" t="n">
+        <v>40</v>
       </c>
       <c r="Y5" s="1" t="s">
-        <v>148</v>
+        <v>113</v>
       </c>
       <c r="Z5" s="2" t="n">
-        <v>4.73609256977679</v>
+        <v>4.73758688292009</v>
       </c>
       <c r="AA5" s="2" t="n">
-        <v>0.487641598070697</v>
+        <v>0.488527002970693</v>
       </c>
       <c r="AB5" s="2" t="n">
-        <v>0.0120176090070576</v>
+        <v>0.0121472607154107</v>
       </c>
       <c r="AC5" s="2" t="n">
-        <v>2.02271261361793</v>
+        <v>2.02271148184962</v>
       </c>
       <c r="AD5" s="2" t="n">
-        <v>62.2899999999991</v>
-      </c>
-      <c r="AE5" s="0" t="n">
-        <f aca="false">AD5-AD4</f>
-        <v>18.949999999999</v>
+        <v>215.120000000001</v>
+      </c>
+      <c r="AE5" s="3" t="n">
+        <v>19.1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>4.73482989807527</v>
+        <v>4.73256901104308</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>0.486920727836057</v>
+        <v>0.484369816622317</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>0.0118805081393316</v>
+        <v>0.0113165593622519</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>2.02273985286532</v>
+        <v>2.0228363511855</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>397.769999999999</v>
-      </c>
-      <c r="G6" s="0" t="n">
-        <f aca="false">F6-F5</f>
-        <v>92.769999999999</v>
+        <v>490.279999999999</v>
+      </c>
+      <c r="G6" s="3" t="n">
+        <v>92.51</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J6" s="2" t="n">
-        <v>4.74029720513826</v>
+        <v>4.73272127602358</v>
       </c>
       <c r="K6" s="2" t="n">
-        <v>0.488586469425249</v>
+        <v>0.483923166804581</v>
       </c>
       <c r="L6" s="2" t="n">
-        <v>0.0122937737971205</v>
+        <v>0.0112759683315727</v>
       </c>
       <c r="M6" s="2" t="n">
-        <v>2.02259988299427</v>
+        <v>2.02291384221503</v>
       </c>
       <c r="N6" s="2" t="n">
-        <v>765.299999999999</v>
-      </c>
-      <c r="O6" s="0" t="n">
-        <f aca="false">N6-N5</f>
-        <v>184.559999999999</v>
+        <v>954.009999999998</v>
+      </c>
+      <c r="O6" s="3" t="n">
+        <v>188.709999999999</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="R6" s="2" t="n">
-        <v>7.76741733991397</v>
+        <v>4.77334183599085</v>
       </c>
       <c r="S6" s="2" t="n">
-        <v>0.596774641811278</v>
+        <v>0.474399476808662</v>
       </c>
       <c r="T6" s="2" t="n">
-        <v>0.0410998544992935</v>
+        <v>0.0094660091812013</v>
       </c>
       <c r="U6" s="2" t="n">
-        <v>2.01726506829025</v>
+        <v>2.02332243348813</v>
       </c>
       <c r="V6" s="2" t="n">
-        <v>193.170000000002</v>
-      </c>
-      <c r="W6" s="0" t="n">
-        <f aca="false">V6-V5</f>
-        <v>48.029999999999</v>
+        <v>237.940000000002</v>
+      </c>
+      <c r="W6" s="3" t="n">
+        <v>44.8</v>
       </c>
       <c r="Y6" s="1" t="s">
-        <v>149</v>
+        <v>129</v>
       </c>
       <c r="Z6" s="2" t="n">
-        <v>4.86063198429821</v>
+        <v>4.73910454348866</v>
       </c>
       <c r="AA6" s="2" t="n">
-        <v>0.505927587799093</v>
+        <v>0.488627287987745</v>
       </c>
       <c r="AB6" s="2" t="n">
-        <v>0.0154304267644149</v>
+        <v>0.012247400967034</v>
       </c>
       <c r="AC6" s="2" t="n">
-        <v>2.02210058835512</v>
+        <v>2.02262960575295</v>
       </c>
       <c r="AD6" s="2" t="n">
-        <v>81.3600000000006</v>
-      </c>
-      <c r="AE6" s="0" t="n">
-        <f aca="false">AD6-AD5</f>
-        <v>19.0700000000015</v>
+        <v>529.93</v>
+      </c>
+      <c r="AE6" s="3" t="n">
+        <v>20.5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>150</v>
+        <v>127</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>4.73256901104308</v>
+        <v>4.73264681850242</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>0.484369816622317</v>
+        <v>0.484773766799881</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>0.0113165593622519</v>
+        <v>0.011396574020999</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>2.0228363511855</v>
+        <v>2.02288556575111</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>490.279999999999</v>
-      </c>
-      <c r="G7" s="0" t="n">
-        <f aca="false">F7-F6</f>
-        <v>92.51</v>
+        <v>2460.03</v>
+      </c>
+      <c r="G7" s="3" t="n">
+        <v>94.2600000000002</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>150</v>
+        <v>123</v>
       </c>
       <c r="J7" s="2" t="n">
-        <v>4.73272127602358</v>
+        <v>4.73292971435406</v>
       </c>
       <c r="K7" s="2" t="n">
-        <v>0.483923166804581</v>
+        <v>0.485850592996181</v>
       </c>
       <c r="L7" s="2" t="n">
-        <v>0.0112759683315727</v>
+        <v>0.011634890946519</v>
       </c>
       <c r="M7" s="2" t="n">
-        <v>2.02291384221503</v>
+        <v>2.02282266987091</v>
       </c>
       <c r="N7" s="2" t="n">
-        <v>954.009999999998</v>
-      </c>
-      <c r="O7" s="0" t="n">
-        <f aca="false">N7-N6</f>
-        <v>188.709999999999</v>
+        <v>4093.77</v>
+      </c>
+      <c r="O7" s="3" t="n">
+        <v>199.47</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="R7" s="2" t="n">
-        <v>4.77334183599085</v>
+        <v>4.84804171549978</v>
       </c>
       <c r="S7" s="2" t="n">
-        <v>0.474399476808662</v>
+        <v>0.504907264556651</v>
       </c>
       <c r="T7" s="2" t="n">
-        <v>0.0094660091812013</v>
+        <v>0.0151636060931207</v>
       </c>
       <c r="U7" s="2" t="n">
-        <v>2.02332243348813</v>
+        <v>2.0222645194372</v>
       </c>
       <c r="V7" s="2" t="n">
-        <v>237.940000000002</v>
-      </c>
-      <c r="W7" s="0" t="n">
-        <f aca="false">V7-V6</f>
-        <v>44.77</v>
+        <v>145.140000000003</v>
+      </c>
+      <c r="W7" s="3" t="n">
+        <v>41.3</v>
       </c>
       <c r="Y7" s="1" t="s">
-        <v>150</v>
+        <v>124</v>
       </c>
       <c r="Z7" s="2" t="n">
-        <v>6.60147190401879</v>
+        <v>4.75295112455731</v>
       </c>
       <c r="AA7" s="2" t="n">
-        <v>0.581859590187604</v>
+        <v>0.491596896089408</v>
       </c>
       <c r="AB7" s="2" t="n">
-        <v>0.0322061123393598</v>
+        <v>0.0129265590049605</v>
       </c>
       <c r="AC7" s="2" t="n">
-        <v>2.01971131920745</v>
+        <v>2.02249915173666</v>
       </c>
       <c r="AD7" s="2" t="n">
-        <v>100.67</v>
-      </c>
-      <c r="AE7" s="0" t="n">
-        <f aca="false">AD7-AD6</f>
-        <v>19.3099999999994</v>
+        <v>430.85</v>
+      </c>
+      <c r="AE7" s="3" t="n">
+        <v>18.6</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>151</v>
+        <v>117</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>4.73561216373413</v>
+        <v>4.73264797386738</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>0.482080680682704</v>
+        <v>0.484852986525434</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>0.0108364418800382</v>
+        <v>0.011409496541767</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>2.02303898337413</v>
+        <v>2.02288566607849</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>585.82</v>
-      </c>
-      <c r="G8" s="0" t="n">
-        <f aca="false">F8-F7</f>
-        <v>95.540000000001</v>
+        <v>1480.85</v>
+      </c>
+      <c r="G8" s="3" t="n">
+        <v>99.3699999999999</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>151</v>
+        <v>126</v>
       </c>
       <c r="J8" s="2" t="n">
-        <v>4.7333403236908</v>
+        <v>4.73297046133708</v>
       </c>
       <c r="K8" s="2" t="n">
-        <v>0.48349900778137</v>
+        <v>0.48568067262847</v>
       </c>
       <c r="L8" s="2" t="n">
-        <v>0.0111101068358233</v>
+        <v>0.0115256045417603</v>
       </c>
       <c r="M8" s="2" t="n">
-        <v>2.02297873418055</v>
+        <v>2.02288651364477</v>
       </c>
       <c r="N8" s="2" t="n">
-        <v>1143.98</v>
-      </c>
-      <c r="O8" s="0" t="n">
-        <f aca="false">N8-N7</f>
-        <v>189.970000000002</v>
+        <v>4668.56</v>
+      </c>
+      <c r="O8" s="3" t="n">
+        <v>185.740000000001</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>151</v>
+        <v>126</v>
       </c>
       <c r="R8" s="2" t="n">
-        <v>5.9514484943827</v>
+        <v>5.02478243838729</v>
       </c>
       <c r="S8" s="2" t="n">
-        <v>0.537463043234561</v>
+        <v>0.463375459734602</v>
       </c>
       <c r="T8" s="2" t="n">
-        <v>0.0258729206168746</v>
+        <v>0.00674916970178051</v>
       </c>
       <c r="U8" s="2" t="n">
-        <v>2.01905457190039</v>
+        <v>2.02465660221152</v>
       </c>
       <c r="V8" s="2" t="n">
-        <v>290.600000000002</v>
-      </c>
-      <c r="W8" s="0" t="n">
-        <f aca="false">V8-V7</f>
-        <v>52.66</v>
+        <v>1151.84</v>
+      </c>
+      <c r="W8" s="3" t="n">
+        <v>52.5</v>
       </c>
       <c r="Y8" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="Z8" s="2" t="n">
-        <v>5.32508805696527</v>
+        <v>4.7616530580448</v>
       </c>
       <c r="AA8" s="2" t="n">
-        <v>0.52391739504947</v>
+        <v>0.484889808225817</v>
       </c>
       <c r="AB8" s="2" t="n">
-        <v>0.0211143002626029</v>
+        <v>0.0120590748985078</v>
       </c>
       <c r="AC8" s="2" t="n">
-        <v>2.02032324216094</v>
+        <v>2.0224987497498</v>
       </c>
       <c r="AD8" s="2" t="n">
-        <v>119.77</v>
-      </c>
-      <c r="AE8" s="0" t="n">
-        <f aca="false">AD8-AD7</f>
-        <v>19.1</v>
+        <v>177.17</v>
+      </c>
+      <c r="AE8" s="3" t="n">
+        <v>19.3</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B9" s="2" t="n">
         <v>4.73264877533292</v>
@@ -25777,146 +25651,139 @@
       <c r="F9" s="2" t="n">
         <v>685.15</v>
       </c>
-      <c r="G9" s="0" t="n">
-        <f aca="false">F9-F8</f>
+      <c r="G9" s="3" t="n">
         <v>99.3299999999999</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>152</v>
+        <v>112</v>
       </c>
       <c r="J9" s="2" t="n">
-        <v>4.79325080296581</v>
+        <v>4.73301559715109</v>
       </c>
       <c r="K9" s="2" t="n">
-        <v>0.498072195395889</v>
+        <v>0.485915675625117</v>
       </c>
       <c r="L9" s="2" t="n">
-        <v>0.0141764024557666</v>
+        <v>0.0116649147933046</v>
       </c>
       <c r="M9" s="2" t="n">
-        <v>2.02222982573153</v>
+        <v>2.02278694356013</v>
       </c>
       <c r="N9" s="2" t="n">
-        <v>1333.63</v>
-      </c>
-      <c r="O9" s="0" t="n">
-        <f aca="false">N9-N8</f>
-        <v>189.65</v>
+        <v>1929.11</v>
+      </c>
+      <c r="O9" s="3" t="n">
+        <v>201.76</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>152</v>
+        <v>129</v>
       </c>
       <c r="R9" s="2" t="n">
-        <v>5.34689717187448</v>
+        <v>5.19172872965442</v>
       </c>
       <c r="S9" s="2" t="n">
-        <v>0.535495712555746</v>
+        <v>0.519151033991847</v>
       </c>
       <c r="T9" s="2" t="n">
-        <v>0.0212835570985228</v>
+        <v>0.0197758268825193</v>
       </c>
       <c r="U9" s="2" t="n">
-        <v>2.02138301988147</v>
+        <v>2.02069997880961</v>
       </c>
       <c r="V9" s="2" t="n">
-        <v>337.170000000002</v>
-      </c>
-      <c r="W9" s="0" t="n">
-        <f aca="false">V9-V8</f>
-        <v>46.57</v>
+        <v>1291.8</v>
+      </c>
+      <c r="W9" s="3" t="n">
+        <v>43.2</v>
       </c>
       <c r="Y9" s="1" t="s">
-        <v>152</v>
+        <v>116</v>
       </c>
       <c r="Z9" s="2" t="n">
-        <v>5.00113948180471</v>
+        <v>4.76757257254872</v>
       </c>
       <c r="AA9" s="2" t="n">
-        <v>0.509737160282644</v>
+        <v>0.494714017032156</v>
       </c>
       <c r="AB9" s="2" t="n">
-        <v>0.0174673638832025</v>
+        <v>0.0134696460555681</v>
       </c>
       <c r="AC9" s="2" t="n">
-        <v>2.02103148452504</v>
+        <v>2.02238460546414</v>
       </c>
       <c r="AD9" s="2" t="n">
-        <v>138.969999999999</v>
-      </c>
-      <c r="AE9" s="0" t="n">
-        <f aca="false">AD9-AD8</f>
-        <v>19.199999999999</v>
+        <v>274.950000000001</v>
+      </c>
+      <c r="AE9" s="3" t="n">
+        <v>21.3</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B10" s="2" t="n">
-        <v>4.74131495839404</v>
+        <v>4.73282705256699</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>0.489956988361554</v>
+        <v>0.483995014449269</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>0.012368679977516</v>
+        <v>0.0112592656129446</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>2.02266395137885</v>
+        <v>2.02294816843838</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>784.5</v>
-      </c>
-      <c r="G10" s="0" t="n">
-        <f aca="false">F10-F9</f>
-        <v>99.35</v>
+        <v>113.549999999999</v>
+      </c>
+      <c r="G10" s="3" t="n">
+        <v>113.549999999999</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>153</v>
+        <v>127</v>
       </c>
       <c r="J10" s="2" t="n">
-        <v>4.73735478004939</v>
+        <v>4.73333615333202</v>
       </c>
       <c r="K10" s="2" t="n">
-        <v>0.488077030100962</v>
+        <v>0.486125326235334</v>
       </c>
       <c r="L10" s="2" t="n">
-        <v>0.012121624921767</v>
+        <v>0.0116741122706659</v>
       </c>
       <c r="M10" s="2" t="n">
-        <v>2.02267908532667</v>
+        <v>2.02281552024105</v>
       </c>
       <c r="N10" s="2" t="n">
-        <v>1529.04</v>
-      </c>
-      <c r="O10" s="0" t="n">
-        <f aca="false">N10-N9</f>
-        <v>195.41</v>
+        <v>4867.8</v>
+      </c>
+      <c r="O10" s="3" t="n">
+        <v>199.24</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>153</v>
+        <v>118</v>
       </c>
       <c r="R10" s="2" t="n">
-        <v>6.30863179469164</v>
+        <v>5.28134539080513</v>
       </c>
       <c r="S10" s="2" t="n">
-        <v>0.566669859201638</v>
+        <v>0.531357198793434</v>
       </c>
       <c r="T10" s="2" t="n">
-        <v>0.030344388859594</v>
+        <v>0.0208859953286733</v>
       </c>
       <c r="U10" s="2" t="n">
-        <v>2.01940093529176</v>
+        <v>2.0212254148495</v>
       </c>
       <c r="V10" s="2" t="n">
-        <v>388.950000000001</v>
-      </c>
-      <c r="W10" s="0" t="n">
-        <f aca="false">V10-V9</f>
-        <v>51.779999999999</v>
+        <v>786.540000000001</v>
+      </c>
+      <c r="W10" s="3" t="n">
+        <v>51.7</v>
       </c>
       <c r="Y10" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="Z10" s="2" t="n">
         <v>4.77622194267296</v>
@@ -25933,977 +25800,933 @@
       <c r="AD10" s="2" t="n">
         <v>157.9</v>
       </c>
-      <c r="AE10" s="0" t="n">
-        <f aca="false">AD10-AD9</f>
-        <v>18.930000000001</v>
+      <c r="AE10" s="3" t="n">
+        <v>18.9</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>154</v>
+        <v>131</v>
       </c>
       <c r="B11" s="2" t="n">
-        <v>4.74341171169469</v>
+        <v>4.73297207839648</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>0.490042199680028</v>
+        <v>0.485639831322016</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>0.0125160431424966</v>
+        <v>0.0115843482428836</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>2.02259340337452</v>
+        <v>2.02283240445411</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>885.129999999999</v>
-      </c>
-      <c r="G11" s="0" t="n">
-        <f aca="false">F11-F10</f>
-        <v>100.629999999999</v>
+        <v>2833.84</v>
+      </c>
+      <c r="G11" s="3" t="n">
+        <v>95.23</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J11" s="2" t="n">
-        <v>4.73656998313829</v>
+        <v>4.7333403236908</v>
       </c>
       <c r="K11" s="2" t="n">
-        <v>0.487590201683967</v>
+        <v>0.48349900778137</v>
       </c>
       <c r="L11" s="2" t="n">
-        <v>0.0120429467435466</v>
+        <v>0.0111101068358233</v>
       </c>
       <c r="M11" s="2" t="n">
-        <v>2.02268585798644</v>
+        <v>2.02297873418055</v>
       </c>
       <c r="N11" s="2" t="n">
-        <v>1727.35</v>
-      </c>
-      <c r="O11" s="0" t="n">
-        <f aca="false">N11-N10</f>
-        <v>198.31</v>
+        <v>1143.98</v>
+      </c>
+      <c r="O11" s="3" t="n">
+        <v>189.970000000002</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>154</v>
+        <v>112</v>
       </c>
       <c r="R11" s="2" t="n">
-        <v>11.5474903969739</v>
+        <v>5.28169354702721</v>
       </c>
       <c r="S11" s="2" t="n">
-        <v>0.705731959158286</v>
+        <v>0.526519624734034</v>
       </c>
       <c r="T11" s="2" t="n">
-        <v>0.0713197949829187</v>
+        <v>0.0209980096030192</v>
       </c>
       <c r="U11" s="2" t="n">
-        <v>2.01507962508213</v>
+        <v>2.02069182087361</v>
       </c>
       <c r="V11" s="2" t="n">
-        <v>440.360000000001</v>
-      </c>
-      <c r="W11" s="0" t="n">
-        <f aca="false">V11-V10</f>
-        <v>51.41</v>
+        <v>493.16</v>
+      </c>
+      <c r="W11" s="3" t="n">
+        <v>52.8</v>
       </c>
       <c r="Y11" s="1" t="s">
-        <v>154</v>
+        <v>114</v>
       </c>
       <c r="Z11" s="2" t="n">
-        <v>4.7616530580448</v>
+        <v>4.81435007595051</v>
       </c>
       <c r="AA11" s="2" t="n">
-        <v>0.484889808225817</v>
+        <v>0.500509530146158</v>
       </c>
       <c r="AB11" s="2" t="n">
-        <v>0.0120590748985078</v>
+        <v>0.0146612144728454</v>
       </c>
       <c r="AC11" s="2" t="n">
-        <v>2.0224987497498</v>
+        <v>2.02218110450913</v>
       </c>
       <c r="AD11" s="2" t="n">
-        <v>177.17</v>
-      </c>
-      <c r="AE11" s="0" t="n">
-        <f aca="false">AD11-AD10</f>
-        <v>19.27</v>
+        <v>234.93</v>
+      </c>
+      <c r="AE11" s="3" t="n">
+        <v>19.8</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="B12" s="2" t="n">
-        <v>4.73648664066337</v>
+        <v>4.7330864373861</v>
       </c>
       <c r="C12" s="2" t="n">
-        <v>0.487487705243317</v>
+        <v>0.485753589303298</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>0.0120295958192213</v>
+        <v>0.0116133013856941</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>2.02268541474894</v>
+        <v>2.02282259261874</v>
       </c>
       <c r="F12" s="2" t="n">
-        <v>984.279999999999</v>
-      </c>
-      <c r="G12" s="0" t="n">
-        <f aca="false">F12-F11</f>
-        <v>99.15</v>
+        <v>1682.39</v>
+      </c>
+      <c r="G12" s="3" t="n">
+        <v>102.27</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="J12" s="2" t="n">
-        <v>4.73301559715109</v>
+        <v>4.73334886183427</v>
       </c>
       <c r="K12" s="2" t="n">
-        <v>0.485915675625117</v>
+        <v>0.486182458278899</v>
       </c>
       <c r="L12" s="2" t="n">
-        <v>0.0116649147933046</v>
+        <v>0.0116140901791884</v>
       </c>
       <c r="M12" s="2" t="n">
-        <v>2.02278694356013</v>
+        <v>2.02287216569605</v>
       </c>
       <c r="N12" s="2" t="n">
-        <v>1929.11</v>
-      </c>
-      <c r="O12" s="0" t="n">
-        <f aca="false">N12-N11</f>
-        <v>201.76</v>
+        <v>3894.3</v>
+      </c>
+      <c r="O12" s="3" t="n">
+        <v>199.38</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>112</v>
+        <v>150</v>
       </c>
       <c r="R12" s="2" t="n">
-        <v>5.28169354702721</v>
+        <v>5.34689717187448</v>
       </c>
       <c r="S12" s="2" t="n">
-        <v>0.526519624734034</v>
+        <v>0.535495712555746</v>
       </c>
       <c r="T12" s="2" t="n">
-        <v>0.0209980096030192</v>
+        <v>0.0212835570985228</v>
       </c>
       <c r="U12" s="2" t="n">
-        <v>2.02069182087361</v>
+        <v>2.02138301988147</v>
       </c>
       <c r="V12" s="2" t="n">
-        <v>493.16</v>
-      </c>
-      <c r="W12" s="0" t="n">
-        <f aca="false">V12-V11</f>
-        <v>52.799999999999</v>
+        <v>337.170000000002</v>
+      </c>
+      <c r="W12" s="3" t="n">
+        <v>46.6</v>
       </c>
       <c r="Y12" s="1" t="s">
-        <v>112</v>
+        <v>154</v>
       </c>
       <c r="Z12" s="2" t="n">
-        <v>5.68621616072169</v>
+        <v>4.86063198429821</v>
       </c>
       <c r="AA12" s="2" t="n">
-        <v>0.550729116328858</v>
+        <v>0.505927587799093</v>
       </c>
       <c r="AB12" s="2" t="n">
-        <v>0.0241401540325002</v>
+        <v>0.0154304267644149</v>
       </c>
       <c r="AC12" s="2" t="n">
-        <v>2.02111164912474</v>
+        <v>2.02210058835512</v>
       </c>
       <c r="AD12" s="2" t="n">
-        <v>195.99</v>
-      </c>
-      <c r="AE12" s="0" t="n">
-        <f aca="false">AD12-AD11</f>
-        <v>18.82</v>
+        <v>81.3600000000006</v>
+      </c>
+      <c r="AE12" s="3" t="n">
+        <v>19.1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B13" s="2" t="n">
-        <v>4.73692276540307</v>
+        <v>4.73314513055998</v>
       </c>
       <c r="C13" s="2" t="n">
-        <v>0.481925785181409</v>
+        <v>0.483570944580916</v>
       </c>
       <c r="D13" s="2" t="n">
-        <v>0.0107468659146244</v>
+        <v>0.0111843226277482</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>2.02309831256724</v>
+        <v>2.02292081791604</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>1083.19</v>
-      </c>
-      <c r="G13" s="0" t="n">
-        <f aca="false">F13-F12</f>
-        <v>98.9100000000011</v>
+        <v>1183.74</v>
+      </c>
+      <c r="G13" s="3" t="n">
+        <v>100.55</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="J13" s="2" t="n">
-        <v>4.80216798492102</v>
+        <v>4.73354898677983</v>
       </c>
       <c r="K13" s="2" t="n">
-        <v>0.498435743334862</v>
+        <v>0.483253573307956</v>
       </c>
       <c r="L13" s="2" t="n">
-        <v>0.014375442657964</v>
+        <v>0.0110852178796879</v>
       </c>
       <c r="M13" s="2" t="n">
-        <v>2.02212274654092</v>
+        <v>2.02296716033847</v>
       </c>
       <c r="N13" s="2" t="n">
-        <v>2130.21</v>
-      </c>
-      <c r="O13" s="0" t="n">
-        <f aca="false">N13-N12</f>
-        <v>201.1</v>
+        <v>3694.92</v>
+      </c>
+      <c r="O13" s="3" t="n">
+        <v>198.11</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="R13" s="2" t="n">
-        <v>5.88178503180781</v>
+        <v>5.79392894754167</v>
       </c>
       <c r="S13" s="2" t="n">
-        <v>0.541847904581337</v>
+        <v>0.555308152273156</v>
       </c>
       <c r="T13" s="2" t="n">
-        <v>0.026088534008324</v>
+        <v>0.0239942955300447</v>
       </c>
       <c r="U13" s="2" t="n">
-        <v>2.01933686811595</v>
+        <v>2.02162093489613</v>
       </c>
       <c r="V13" s="2" t="n">
-        <v>555.920000000002</v>
-      </c>
-      <c r="W13" s="0" t="n">
-        <f aca="false">V13-V12</f>
-        <v>62.760000000002</v>
+        <v>1049.83</v>
+      </c>
+      <c r="W13" s="3" t="n">
+        <v>49</v>
       </c>
       <c r="Y13" s="1" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="Z13" s="2" t="n">
-        <v>4.73758688292009</v>
+        <v>4.86966307436344</v>
       </c>
       <c r="AA13" s="2" t="n">
-        <v>0.488527002970693</v>
+        <v>0.502964956823651</v>
       </c>
       <c r="AB13" s="2" t="n">
-        <v>0.0121472607154107</v>
+        <v>0.0156250656601103</v>
       </c>
       <c r="AC13" s="2" t="n">
-        <v>2.02271148184962</v>
+        <v>2.02172328591852</v>
       </c>
       <c r="AD13" s="2" t="n">
-        <v>215.120000000001</v>
-      </c>
-      <c r="AE13" s="0" t="n">
-        <f aca="false">AD13-AD12</f>
-        <v>19.130000000001</v>
+        <v>393.49</v>
+      </c>
+      <c r="AE13" s="3" t="n">
+        <v>19.5</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="B14" s="2" t="n">
-        <v>4.73314513055998</v>
+        <v>4.73319867607468</v>
       </c>
       <c r="C14" s="2" t="n">
-        <v>0.483570944580916</v>
+        <v>0.483607385815407</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>0.0111843226277482</v>
+        <v>0.0111483072722219</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>2.02292081791604</v>
+        <v>2.02292645232688</v>
       </c>
       <c r="F14" s="2" t="n">
-        <v>1183.74</v>
-      </c>
-      <c r="G14" s="0" t="n">
-        <f aca="false">F14-F13</f>
-        <v>100.55</v>
+        <v>1871.51</v>
+      </c>
+      <c r="G14" s="3" t="n">
+        <v>95.8799999999999</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="J14" s="2" t="n">
-        <v>4.73751039481966</v>
+        <v>4.73358870609277</v>
       </c>
       <c r="K14" s="2" t="n">
-        <v>0.481313787145444</v>
+        <v>0.486334908535697</v>
       </c>
       <c r="L14" s="2" t="n">
-        <v>0.0106823516658476</v>
+        <v>0.0117210764837736</v>
       </c>
       <c r="M14" s="2" t="n">
-        <v>2.02307948539383</v>
+        <v>2.02279777580486</v>
       </c>
       <c r="N14" s="2" t="n">
-        <v>2329.38</v>
-      </c>
-      <c r="O14" s="0" t="n">
-        <f aca="false">N14-N13</f>
-        <v>199.17</v>
+        <v>2731.38</v>
+      </c>
+      <c r="O14" s="3" t="n">
+        <v>195.24</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="R14" s="2" t="n">
-        <v>14.5582643173828</v>
+        <v>5.80647672017915</v>
       </c>
       <c r="S14" s="2" t="n">
-        <v>0.774988228655992</v>
+        <v>0.535307628931789</v>
       </c>
       <c r="T14" s="2" t="n">
-        <v>0.096873528581999</v>
+        <v>0.0249516928823957</v>
       </c>
       <c r="U14" s="2" t="n">
-        <v>2.0129974060995</v>
+        <v>2.01933193331388</v>
       </c>
       <c r="V14" s="2" t="n">
-        <v>610.59</v>
-      </c>
-      <c r="W14" s="0" t="n">
-        <f aca="false">V14-V13</f>
-        <v>54.669999999998</v>
+        <v>1248.62</v>
+      </c>
+      <c r="W14" s="3" t="n">
+        <v>46.9</v>
       </c>
       <c r="Y14" s="1" t="s">
-        <v>114</v>
+        <v>146</v>
       </c>
       <c r="Z14" s="2" t="n">
-        <v>4.81435007595051</v>
+        <v>4.93002892499933</v>
       </c>
       <c r="AA14" s="2" t="n">
-        <v>0.500509530146158</v>
+        <v>0.510256231968616</v>
       </c>
       <c r="AB14" s="2" t="n">
-        <v>0.0146612144728454</v>
+        <v>0.0167051762212759</v>
       </c>
       <c r="AC14" s="2" t="n">
-        <v>2.02218110450913</v>
+        <v>2.02173487369732</v>
       </c>
       <c r="AD14" s="2" t="n">
-        <v>234.93</v>
-      </c>
-      <c r="AE14" s="0" t="n">
-        <f aca="false">AD14-AD13</f>
-        <v>19.809999999999</v>
+        <v>43.3400000000001</v>
+      </c>
+      <c r="AE14" s="3" t="n">
+        <v>20.6</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="B15" s="2" t="n">
-        <v>4.73375992424785</v>
+        <v>4.73324406483686</v>
       </c>
       <c r="C15" s="2" t="n">
-        <v>0.486452638339125</v>
+        <v>0.485726345949523</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>0.0117491433047291</v>
+        <v>0.0116259150426616</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>2.02279010691657</v>
+        <v>2.02270430880762</v>
       </c>
       <c r="F15" s="2" t="n">
-        <v>1282.09</v>
-      </c>
-      <c r="G15" s="0" t="n">
-        <f aca="false">F15-F14</f>
-        <v>98.3499999999999</v>
+        <v>2365.77</v>
+      </c>
+      <c r="G15" s="3" t="n">
+        <v>99.8400000000002</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>115</v>
+        <v>151</v>
       </c>
       <c r="J15" s="2" t="n">
-        <v>4.73560747462796</v>
+        <v>4.73384437044199</v>
       </c>
       <c r="K15" s="2" t="n">
-        <v>0.487195090834307</v>
+        <v>0.486686723823064</v>
       </c>
       <c r="L15" s="2" t="n">
-        <v>0.0119547932618644</v>
+        <v>0.0117550885940693</v>
       </c>
       <c r="M15" s="2" t="n">
-        <v>2.02271116492208</v>
+        <v>2.0227828178733</v>
       </c>
       <c r="N15" s="2" t="n">
-        <v>2536.14</v>
-      </c>
-      <c r="O15" s="0" t="n">
-        <f aca="false">N15-N14</f>
-        <v>206.76</v>
+        <v>200.299999999999</v>
+      </c>
+      <c r="O15" s="3" t="n">
+        <v>200.299999999999</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="R15" s="2" t="n">
-        <v>11.8556919869248</v>
+        <v>5.88178503180781</v>
       </c>
       <c r="S15" s="2" t="n">
-        <v>0.715741418893173</v>
+        <v>0.541847904581337</v>
       </c>
       <c r="T15" s="2" t="n">
-        <v>0.0739514877525552</v>
+        <v>0.026088534008324</v>
       </c>
       <c r="U15" s="2" t="n">
-        <v>2.01497036629778</v>
+        <v>2.01933686811595</v>
       </c>
       <c r="V15" s="2" t="n">
-        <v>652.950000000001</v>
-      </c>
-      <c r="W15" s="0" t="n">
-        <f aca="false">V15-V14</f>
-        <v>42.3600000000009</v>
+        <v>555.920000000002</v>
+      </c>
+      <c r="W15" s="3" t="n">
+        <v>62.8</v>
       </c>
       <c r="Y15" s="1" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
       <c r="Z15" s="2" t="n">
-        <v>5.16877539087627</v>
+        <v>4.99188121808989</v>
       </c>
       <c r="AA15" s="2" t="n">
-        <v>0.526115886200987</v>
+        <v>0.51621370105816</v>
       </c>
       <c r="AB15" s="2" t="n">
-        <v>0.0195758104148813</v>
+        <v>0.0171909710769401</v>
       </c>
       <c r="AC15" s="2" t="n">
-        <v>2.0214757228493</v>
+        <v>2.02205879088233</v>
       </c>
       <c r="AD15" s="2" t="n">
-        <v>253.65</v>
-      </c>
-      <c r="AE15" s="0" t="n">
-        <f aca="false">AD15-AD14</f>
-        <v>18.72</v>
+        <v>509.4</v>
+      </c>
+      <c r="AE15" s="3" t="n">
+        <v>20.1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B16" s="2" t="n">
-        <v>4.73255095728732</v>
+        <v>4.73375992424785</v>
       </c>
       <c r="C16" s="2" t="n">
-        <v>0.485266574729285</v>
+        <v>0.486452638339125</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>0.0114431495749795</v>
+        <v>0.0117491433047291</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>2.02299536134802</v>
+        <v>2.02279010691657</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>1381.48</v>
-      </c>
-      <c r="G16" s="0" t="n">
-        <f aca="false">F16-F15</f>
-        <v>99.3900000000001</v>
+        <v>1282.09</v>
+      </c>
+      <c r="G16" s="3" t="n">
+        <v>98.3499999999999</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J16" s="2" t="n">
-        <v>4.73358870609277</v>
+        <v>4.73560747462796</v>
       </c>
       <c r="K16" s="2" t="n">
-        <v>0.486334908535697</v>
+        <v>0.487195090834307</v>
       </c>
       <c r="L16" s="2" t="n">
-        <v>0.0117210764837736</v>
+        <v>0.0119547932618644</v>
       </c>
       <c r="M16" s="2" t="n">
-        <v>2.02279777580486</v>
+        <v>2.02271116492208</v>
       </c>
       <c r="N16" s="2" t="n">
-        <v>2731.38</v>
-      </c>
-      <c r="O16" s="0" t="n">
-        <f aca="false">N16-N15</f>
-        <v>195.24</v>
+        <v>2536.14</v>
+      </c>
+      <c r="O16" s="3" t="n">
+        <v>206.76</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>116</v>
+        <v>153</v>
       </c>
       <c r="R16" s="2" t="n">
-        <v>4.73468742483637</v>
+        <v>5.9514484943827</v>
       </c>
       <c r="S16" s="2" t="n">
-        <v>0.487292801271241</v>
+        <v>0.537463043234561</v>
       </c>
       <c r="T16" s="2" t="n">
-        <v>0.0118434914597135</v>
+        <v>0.0258729206168746</v>
       </c>
       <c r="U16" s="2" t="n">
-        <v>2.0228137742823</v>
+        <v>2.01905457190039</v>
       </c>
       <c r="V16" s="2" t="n">
-        <v>691.280000000003</v>
-      </c>
-      <c r="W16" s="0" t="n">
-        <f aca="false">V16-V15</f>
-        <v>38.3300000000021</v>
+        <v>290.600000000002</v>
+      </c>
+      <c r="W16" s="3" t="n">
+        <v>52.7</v>
       </c>
       <c r="Y16" s="1" t="s">
-        <v>116</v>
+        <v>150</v>
       </c>
       <c r="Z16" s="2" t="n">
-        <v>4.76757257254872</v>
+        <v>5.00113948180471</v>
       </c>
       <c r="AA16" s="2" t="n">
-        <v>0.494714017032156</v>
+        <v>0.509737160282644</v>
       </c>
       <c r="AB16" s="2" t="n">
-        <v>0.0134696460555681</v>
+        <v>0.0174673638832025</v>
       </c>
       <c r="AC16" s="2" t="n">
-        <v>2.02238460546414</v>
+        <v>2.02103148452504</v>
       </c>
       <c r="AD16" s="2" t="n">
-        <v>274.950000000001</v>
-      </c>
-      <c r="AE16" s="0" t="n">
-        <f aca="false">AD16-AD15</f>
-        <v>21.300000000001</v>
+        <v>138.969999999999</v>
+      </c>
+      <c r="AE16" s="3" t="n">
+        <v>19.2</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="B17" s="2" t="n">
-        <v>4.73264797386738</v>
+        <v>4.73379934517056</v>
       </c>
       <c r="C17" s="2" t="n">
-        <v>0.484852986525434</v>
+        <v>0.482953623448318</v>
       </c>
       <c r="D17" s="2" t="n">
-        <v>0.011409496541767</v>
+        <v>0.0110631897345459</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>2.02288566607849</v>
+        <v>2.02297437402652</v>
       </c>
       <c r="F17" s="2" t="n">
-        <v>1480.85</v>
-      </c>
-      <c r="G17" s="0" t="n">
-        <f aca="false">F17-F16</f>
-        <v>99.3699999999999</v>
+        <v>2738.61</v>
+      </c>
+      <c r="G17" s="3" t="n">
+        <v>92.75</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>117</v>
+        <v>147</v>
       </c>
       <c r="J17" s="2" t="n">
-        <v>4.73241918756398</v>
+        <v>4.73605216732573</v>
       </c>
       <c r="K17" s="2" t="n">
-        <v>0.484993264429524</v>
+        <v>0.481902460643336</v>
       </c>
       <c r="L17" s="2" t="n">
-        <v>0.0114695858242343</v>
+        <v>0.0107935163956716</v>
       </c>
       <c r="M17" s="2" t="n">
-        <v>2.02284937300368</v>
+        <v>2.02304612788988</v>
       </c>
       <c r="N17" s="2" t="n">
-        <v>2921.38</v>
-      </c>
-      <c r="O17" s="0" t="n">
-        <f aca="false">N17-N16</f>
-        <v>190</v>
+        <v>580.74</v>
+      </c>
+      <c r="O17" s="3" t="n">
+        <v>188.890000000001</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="R17" s="2" t="n">
-        <v>6.18732062337219</v>
+        <v>5.9803077113851</v>
       </c>
       <c r="S17" s="2" t="n">
-        <v>0.554872470932307</v>
+        <v>0.556150212218715</v>
       </c>
       <c r="T17" s="2" t="n">
-        <v>0.0289854704792675</v>
+        <v>0.0275960798838708</v>
       </c>
       <c r="U17" s="2" t="n">
-        <v>2.01904941973475</v>
+        <v>2.01983412262115</v>
       </c>
       <c r="V17" s="2" t="n">
-        <v>734.82</v>
-      </c>
-      <c r="W17" s="0" t="n">
-        <f aca="false">V17-V16</f>
-        <v>43.539999999997</v>
+        <v>828.75</v>
+      </c>
+      <c r="W17" s="3" t="n">
+        <v>42.2</v>
       </c>
       <c r="Y17" s="1" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="Z17" s="2" t="n">
-        <v>5.22476421829463</v>
+        <v>5.00942022103225</v>
       </c>
       <c r="AA17" s="2" t="n">
-        <v>0.529731302076161</v>
+        <v>0.517117055651651</v>
       </c>
       <c r="AB17" s="2" t="n">
-        <v>0.0199028781415373</v>
+        <v>0.0175787935517858</v>
       </c>
       <c r="AC17" s="2" t="n">
-        <v>2.02173496437402</v>
+        <v>2.02182923249266</v>
       </c>
       <c r="AD17" s="2" t="n">
-        <v>296.9</v>
-      </c>
-      <c r="AE17" s="0" t="n">
-        <f aca="false">AD17-AD16</f>
-        <v>21.949999999999</v>
+        <v>469.289999999999</v>
+      </c>
+      <c r="AE17" s="3" t="n">
+        <v>19.6</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="B18" s="2" t="n">
-        <v>4.73248753274178</v>
+        <v>4.73449635107517</v>
       </c>
       <c r="C18" s="2" t="n">
-        <v>0.48485401527131</v>
+        <v>0.486680336522834</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>0.0114020830898292</v>
+        <v>0.0118370228419102</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>2.022881086327</v>
+        <v>2.02269567770149</v>
       </c>
       <c r="F18" s="2" t="n">
-        <v>1580.12</v>
-      </c>
-      <c r="G18" s="0" t="n">
-        <f aca="false">F18-F17</f>
-        <v>99.27</v>
+        <v>2645.86</v>
+      </c>
+      <c r="G18" s="3" t="n">
+        <v>92.6900000000001</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="J18" s="2" t="n">
-        <v>4.77669216311506</v>
+        <v>4.73617492678719</v>
       </c>
       <c r="K18" s="2" t="n">
-        <v>0.495414479181898</v>
+        <v>0.487942072183846</v>
       </c>
       <c r="L18" s="2" t="n">
-        <v>0.0137246373502613</v>
+        <v>0.0120623962489738</v>
       </c>
       <c r="M18" s="2" t="n">
-        <v>2.0222695728743</v>
+        <v>2.02267222431049</v>
       </c>
       <c r="N18" s="2" t="n">
-        <v>3105.83</v>
-      </c>
-      <c r="O18" s="0" t="n">
-        <f aca="false">N18-N17</f>
-        <v>184.45</v>
+        <v>5061.42</v>
+      </c>
+      <c r="O18" s="3" t="n">
+        <v>193.62</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="R18" s="2" t="n">
-        <v>5.28134539080513</v>
+        <v>6.18732062337219</v>
       </c>
       <c r="S18" s="2" t="n">
-        <v>0.531357198793434</v>
+        <v>0.554872470932307</v>
       </c>
       <c r="T18" s="2" t="n">
-        <v>0.0208859953286733</v>
+        <v>0.0289854704792675</v>
       </c>
       <c r="U18" s="2" t="n">
-        <v>2.0212254148495</v>
+        <v>2.01904941973475</v>
       </c>
       <c r="V18" s="2" t="n">
-        <v>786.540000000001</v>
-      </c>
-      <c r="W18" s="0" t="n">
-        <f aca="false">V18-V17</f>
-        <v>51.7200000000009</v>
+        <v>734.82</v>
+      </c>
+      <c r="W18" s="3" t="n">
+        <v>43.5</v>
       </c>
       <c r="Y18" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="Z18" s="2" t="n">
-        <v>5.81314261535196</v>
+        <v>5.11984047261926</v>
       </c>
       <c r="AA18" s="2" t="n">
-        <v>0.552438666640035</v>
+        <v>0.5237416884558</v>
       </c>
       <c r="AB18" s="2" t="n">
-        <v>0.0260364439741952</v>
+        <v>0.0179299563022002</v>
       </c>
       <c r="AC18" s="2" t="n">
-        <v>2.02006521694369</v>
+        <v>2.0223093658777</v>
       </c>
       <c r="AD18" s="2" t="n">
-        <v>314.98</v>
-      </c>
-      <c r="AE18" s="0" t="n">
-        <f aca="false">AD18-AD17</f>
-        <v>18.08</v>
+        <v>333.76</v>
+      </c>
+      <c r="AE18" s="3" t="n">
+        <v>18.8</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>119</v>
+        <v>154</v>
       </c>
       <c r="B19" s="2" t="n">
-        <v>4.7330864373861</v>
+        <v>4.73482989807527</v>
       </c>
       <c r="C19" s="2" t="n">
-        <v>0.485753589303298</v>
+        <v>0.486920727836057</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>0.0116133013856941</v>
+        <v>0.0118805081393316</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>2.02282259261874</v>
+        <v>2.02273985286532</v>
       </c>
       <c r="F19" s="2" t="n">
-        <v>1682.39</v>
-      </c>
-      <c r="G19" s="0" t="n">
-        <f aca="false">F19-F18</f>
-        <v>102.27</v>
+        <v>397.769999999999</v>
+      </c>
+      <c r="G19" s="3" t="n">
+        <v>92.769999999999</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>119</v>
+        <v>149</v>
       </c>
       <c r="J19" s="2" t="n">
-        <v>4.73834933861092</v>
+        <v>4.73656998313829</v>
       </c>
       <c r="K19" s="2" t="n">
-        <v>0.481105786305422</v>
+        <v>0.487590201683967</v>
       </c>
       <c r="L19" s="2" t="n">
-        <v>0.0106260503903813</v>
+        <v>0.0120429467435466</v>
       </c>
       <c r="M19" s="2" t="n">
-        <v>2.02310321175238</v>
+        <v>2.02268585798644</v>
       </c>
       <c r="N19" s="2" t="n">
-        <v>3293.46</v>
-      </c>
-      <c r="O19" s="0" t="n">
-        <f aca="false">N19-N18</f>
-        <v>187.63</v>
+        <v>1727.35</v>
+      </c>
+      <c r="O19" s="3" t="n">
+        <v>198.31</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>119</v>
+        <v>152</v>
       </c>
       <c r="R19" s="2" t="n">
-        <v>5.9803077113851</v>
+        <v>6.30863179469164</v>
       </c>
       <c r="S19" s="2" t="n">
-        <v>0.556150212218715</v>
+        <v>0.566669859201638</v>
       </c>
       <c r="T19" s="2" t="n">
-        <v>0.0275960798838708</v>
+        <v>0.030344388859594</v>
       </c>
       <c r="U19" s="2" t="n">
-        <v>2.01983412262115</v>
+        <v>2.01940093529176</v>
       </c>
       <c r="V19" s="2" t="n">
-        <v>828.75</v>
-      </c>
-      <c r="W19" s="0" t="n">
-        <f aca="false">V19-V18</f>
-        <v>42.209999999999</v>
+        <v>388.950000000001</v>
+      </c>
+      <c r="W19" s="3" t="n">
+        <v>51.8</v>
       </c>
       <c r="Y19" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="Z19" s="2" t="n">
-        <v>5.11984047261926</v>
+        <v>5.16877539087627</v>
       </c>
       <c r="AA19" s="2" t="n">
-        <v>0.5237416884558</v>
+        <v>0.526115886200987</v>
       </c>
       <c r="AB19" s="2" t="n">
-        <v>0.0179299563022002</v>
+        <v>0.0195758104148813</v>
       </c>
       <c r="AC19" s="2" t="n">
-        <v>2.0223093658777</v>
+        <v>2.0214757228493</v>
       </c>
       <c r="AD19" s="2" t="n">
-        <v>333.76</v>
-      </c>
-      <c r="AE19" s="0" t="n">
-        <f aca="false">AD19-AD18</f>
-        <v>18.78</v>
+        <v>253.65</v>
+      </c>
+      <c r="AE19" s="3" t="n">
+        <v>18.7</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>120</v>
+        <v>153</v>
       </c>
       <c r="B20" s="2" t="n">
-        <v>4.73579054858861</v>
+        <v>4.73561216373413</v>
       </c>
       <c r="C20" s="2" t="n">
-        <v>0.487839966860063</v>
+        <v>0.482080680682704</v>
       </c>
       <c r="D20" s="2" t="n">
-        <v>0.011984052181976</v>
+        <v>0.0108364418800382</v>
       </c>
       <c r="E20" s="2" t="n">
-        <v>2.02274278922304</v>
+        <v>2.02303898337413</v>
       </c>
       <c r="F20" s="2" t="n">
-        <v>1775.63</v>
-      </c>
-      <c r="G20" s="0" t="n">
-        <f aca="false">F20-F19</f>
-        <v>93.24</v>
+        <v>585.82</v>
+      </c>
+      <c r="G20" s="3" t="n">
+        <v>95.540000000001</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>120</v>
+        <v>152</v>
       </c>
       <c r="J20" s="2" t="n">
-        <v>4.73849025987369</v>
+        <v>4.73735478004939</v>
       </c>
       <c r="K20" s="2" t="n">
-        <v>0.481280083277685</v>
+        <v>0.488077030100962</v>
       </c>
       <c r="L20" s="2" t="n">
-        <v>0.0106273021604792</v>
+        <v>0.012121624921767</v>
       </c>
       <c r="M20" s="2" t="n">
-        <v>2.02312322928082</v>
+        <v>2.02267908532667</v>
       </c>
       <c r="N20" s="2" t="n">
-        <v>3496.81</v>
-      </c>
-      <c r="O20" s="0" t="n">
-        <f aca="false">N20-N19</f>
-        <v>203.35</v>
+        <v>1529.04</v>
+      </c>
+      <c r="O20" s="3" t="n">
+        <v>195.41</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="R20" s="2" t="n">
-        <v>4.75755084223834</v>
+        <v>6.59016356265067</v>
       </c>
       <c r="S20" s="2" t="n">
-        <v>0.4937422846595</v>
+        <v>0.572825057677677</v>
       </c>
       <c r="T20" s="2" t="n">
-        <v>0.0130622540715576</v>
+        <v>0.032583147575317</v>
       </c>
       <c r="U20" s="2" t="n">
-        <v>2.02259009753887</v>
+        <v>2.01888770499756</v>
       </c>
       <c r="V20" s="2" t="n">
-        <v>868.75</v>
-      </c>
-      <c r="W20" s="0" t="n">
-        <f aca="false">V20-V19</f>
-        <v>40</v>
+        <v>1000.8</v>
+      </c>
+      <c r="W20" s="3" t="n">
+        <v>40.2</v>
       </c>
       <c r="Y20" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="Z20" s="2" t="n">
-        <v>5.53061476143937</v>
+        <v>5.22476421829463</v>
       </c>
       <c r="AA20" s="2" t="n">
-        <v>0.544067303981715</v>
+        <v>0.529731302076161</v>
       </c>
       <c r="AB20" s="2" t="n">
-        <v>0.0228259975865514</v>
+        <v>0.0199028781415373</v>
       </c>
       <c r="AC20" s="2" t="n">
-        <v>2.02110545965087</v>
+        <v>2.02173496437402</v>
       </c>
       <c r="AD20" s="2" t="n">
-        <v>354.780000000001</v>
-      </c>
-      <c r="AE20" s="0" t="n">
-        <f aca="false">AD20-AD19</f>
-        <v>21.020000000001</v>
+        <v>296.9</v>
+      </c>
+      <c r="AE20" s="3" t="n">
+        <v>21.9</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B21" s="2" t="n">
-        <v>4.73319867607468</v>
+        <v>4.73579054858861</v>
       </c>
       <c r="C21" s="2" t="n">
-        <v>0.483607385815407</v>
+        <v>0.487839966860063</v>
       </c>
       <c r="D21" s="2" t="n">
-        <v>0.0111483072722219</v>
+        <v>0.011984052181976</v>
       </c>
       <c r="E21" s="2" t="n">
-        <v>2.02292645232688</v>
+        <v>2.02274278922304</v>
       </c>
       <c r="F21" s="2" t="n">
-        <v>1871.51</v>
-      </c>
-      <c r="G21" s="0" t="n">
-        <f aca="false">F21-F20</f>
-        <v>95.8799999999999</v>
+        <v>1775.63</v>
+      </c>
+      <c r="G21" s="3" t="n">
+        <v>93.24</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="J21" s="2" t="n">
-        <v>4.73354898677983</v>
+        <v>4.73751039481966</v>
       </c>
       <c r="K21" s="2" t="n">
-        <v>0.483253573307956</v>
+        <v>0.481313787145444</v>
       </c>
       <c r="L21" s="2" t="n">
-        <v>0.0110852178796879</v>
+        <v>0.0106823516658476</v>
       </c>
       <c r="M21" s="2" t="n">
-        <v>2.02296716033847</v>
+        <v>2.02307948539383</v>
       </c>
       <c r="N21" s="2" t="n">
-        <v>3694.92</v>
-      </c>
-      <c r="O21" s="0" t="n">
-        <f aca="false">N21-N20</f>
-        <v>198.11</v>
+        <v>2329.38</v>
+      </c>
+      <c r="O21" s="3" t="n">
+        <v>199.17</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="R21" s="2" t="n">
-        <v>4.7331248630718</v>
+        <v>6.79126082662106</v>
       </c>
       <c r="S21" s="2" t="n">
-        <v>0.485272347057502</v>
+        <v>0.587057909370176</v>
       </c>
       <c r="T21" s="2" t="n">
-        <v>0.011406013099693</v>
+        <v>0.0338481485476043</v>
       </c>
       <c r="U21" s="2" t="n">
-        <v>2.02293723685077</v>
+        <v>2.01945480387697</v>
       </c>
       <c r="V21" s="2" t="n">
-        <v>910.050000000003</v>
-      </c>
-      <c r="W21" s="0" t="n">
-        <f aca="false">V21-V20</f>
-        <v>41.300000000003</v>
+        <v>1438.69</v>
+      </c>
+      <c r="W21" s="3" t="n">
+        <v>46.9</v>
       </c>
       <c r="Y21" s="1" t="s">
         <v>121</v>
@@ -26923,549 +26746,524 @@
       <c r="AD21" s="2" t="n">
         <v>374.030000000001</v>
       </c>
-      <c r="AE21" s="0" t="n">
-        <f aca="false">AD21-AD20</f>
-        <v>19.25</v>
+      <c r="AE21" s="3" t="n">
+        <v>19.3</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="B22" s="2" t="n">
-        <v>4.79348280829329</v>
+        <v>4.73648664066337</v>
       </c>
       <c r="C22" s="2" t="n">
-        <v>0.498066450857373</v>
+        <v>0.487487705243317</v>
       </c>
       <c r="D22" s="2" t="n">
-        <v>0.0141821487240554</v>
+        <v>0.0120295958192213</v>
       </c>
       <c r="E22" s="2" t="n">
-        <v>2.02223163265957</v>
+        <v>2.02268541474894</v>
       </c>
       <c r="F22" s="2" t="n">
-        <v>1970.68</v>
-      </c>
-      <c r="G22" s="0" t="n">
-        <f aca="false">F22-F21</f>
-        <v>99.1700000000001</v>
+        <v>984.279999999999</v>
+      </c>
+      <c r="G22" s="3" t="n">
+        <v>99.15</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="J22" s="2" t="n">
-        <v>4.73334886183427</v>
+        <v>4.73834933861092</v>
       </c>
       <c r="K22" s="2" t="n">
-        <v>0.486182458278899</v>
+        <v>0.481105786305422</v>
       </c>
       <c r="L22" s="2" t="n">
-        <v>0.0116140901791884</v>
+        <v>0.0106260503903813</v>
       </c>
       <c r="M22" s="2" t="n">
-        <v>2.02287216569605</v>
+        <v>2.02310321175238</v>
       </c>
       <c r="N22" s="2" t="n">
-        <v>3894.3</v>
-      </c>
-      <c r="O22" s="0" t="n">
-        <f aca="false">N22-N21</f>
-        <v>199.38</v>
+        <v>3293.46</v>
+      </c>
+      <c r="O22" s="3" t="n">
+        <v>187.63</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="R22" s="2" t="n">
-        <v>11.7694177170813</v>
+        <v>7.23738434138332</v>
       </c>
       <c r="S22" s="2" t="n">
-        <v>0.705382587214474</v>
+        <v>0.563485655514734</v>
       </c>
       <c r="T22" s="2" t="n">
-        <v>0.0728133047891965</v>
+        <v>0.0345598346150393</v>
       </c>
       <c r="U22" s="2" t="n">
-        <v>2.01466901234254</v>
+        <v>2.01727669965836</v>
       </c>
       <c r="V22" s="2" t="n">
-        <v>960.57</v>
-      </c>
-      <c r="W22" s="0" t="n">
-        <f aca="false">V22-V21</f>
-        <v>50.519999999997</v>
+        <v>1391.8</v>
+      </c>
+      <c r="W22" s="3" t="n">
+        <v>50.7</v>
       </c>
       <c r="Y22" s="1" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="Z22" s="2" t="n">
-        <v>4.86966307436344</v>
+        <v>5.29161793897107</v>
       </c>
       <c r="AA22" s="2" t="n">
-        <v>0.502964956823651</v>
+        <v>0.532915414088237</v>
       </c>
       <c r="AB22" s="2" t="n">
-        <v>0.0156250656601103</v>
+        <v>0.0200434216808821</v>
       </c>
       <c r="AC22" s="2" t="n">
-        <v>2.02172328591852</v>
+        <v>2.02112866865988</v>
       </c>
       <c r="AD22" s="2" t="n">
-        <v>393.49</v>
-      </c>
-      <c r="AE22" s="0" t="n">
-        <f aca="false">AD22-AD21</f>
-        <v>19.459999999999</v>
+        <v>586.110000000001</v>
+      </c>
+      <c r="AE22" s="3" t="n">
+        <v>18.7</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="B23" s="2" t="n">
-        <v>4.74378462377099</v>
+        <v>4.73692276540307</v>
       </c>
       <c r="C23" s="2" t="n">
-        <v>0.490241466189082</v>
+        <v>0.481925785181409</v>
       </c>
       <c r="D23" s="2" t="n">
-        <v>0.0125382278713031</v>
+        <v>0.0107468659146244</v>
       </c>
       <c r="E23" s="2" t="n">
-        <v>2.02258031008103</v>
+        <v>2.02309831256724</v>
       </c>
       <c r="F23" s="2" t="n">
-        <v>2066</v>
-      </c>
-      <c r="G23" s="0" t="n">
-        <f aca="false">F23-F22</f>
-        <v>95.3199999999999</v>
+        <v>1083.19</v>
+      </c>
+      <c r="G23" s="3" t="n">
+        <v>98.9100000000011</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="J23" s="2" t="n">
-        <v>4.73292971435406</v>
+        <v>4.73849025987369</v>
       </c>
       <c r="K23" s="2" t="n">
-        <v>0.485850592996181</v>
+        <v>0.481280083277685</v>
       </c>
       <c r="L23" s="2" t="n">
-        <v>0.011634890946519</v>
+        <v>0.0106273021604792</v>
       </c>
       <c r="M23" s="2" t="n">
-        <v>2.02282266987091</v>
+        <v>2.02312322928082</v>
       </c>
       <c r="N23" s="2" t="n">
-        <v>4093.77</v>
-      </c>
-      <c r="O23" s="0" t="n">
-        <f aca="false">N23-N22</f>
-        <v>199.47</v>
+        <v>3496.81</v>
+      </c>
+      <c r="O23" s="3" t="n">
+        <v>203.35</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>123</v>
+        <v>154</v>
       </c>
       <c r="R23" s="2" t="n">
-        <v>6.59016356265067</v>
+        <v>7.76741733991397</v>
       </c>
       <c r="S23" s="2" t="n">
-        <v>0.572825057677677</v>
+        <v>0.596774641811278</v>
       </c>
       <c r="T23" s="2" t="n">
-        <v>0.032583147575317</v>
+        <v>0.0410998544992935</v>
       </c>
       <c r="U23" s="2" t="n">
-        <v>2.01888770499756</v>
+        <v>2.01726506829025</v>
       </c>
       <c r="V23" s="2" t="n">
-        <v>1000.8</v>
-      </c>
-      <c r="W23" s="0" t="n">
-        <f aca="false">V23-V22</f>
-        <v>40.2299999999999</v>
+        <v>193.170000000002</v>
+      </c>
+      <c r="W23" s="3" t="n">
+        <v>48</v>
       </c>
       <c r="Y23" s="1" t="s">
-        <v>123</v>
+        <v>153</v>
       </c>
       <c r="Z23" s="2" t="n">
-        <v>5.6917015780514</v>
+        <v>5.32508805696527</v>
       </c>
       <c r="AA23" s="2" t="n">
-        <v>0.551282825258859</v>
+        <v>0.52391739504947</v>
       </c>
       <c r="AB23" s="2" t="n">
-        <v>0.0238474547305066</v>
+        <v>0.0211143002626029</v>
       </c>
       <c r="AC23" s="2" t="n">
-        <v>2.02155054029698</v>
+        <v>2.02032324216094</v>
       </c>
       <c r="AD23" s="2" t="n">
-        <v>412.27</v>
-      </c>
-      <c r="AE23" s="0" t="n">
-        <f aca="false">AD23-AD22</f>
-        <v>18.78</v>
+        <v>119.77</v>
+      </c>
+      <c r="AE23" s="3" t="n">
+        <v>19.1</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="B24" s="2" t="n">
-        <v>4.73989285970444</v>
+        <v>4.73750625719472</v>
       </c>
       <c r="C24" s="2" t="n">
-        <v>0.488713970621203</v>
+        <v>0.488255319227011</v>
       </c>
       <c r="D24" s="2" t="n">
-        <v>0.0122874029570318</v>
+        <v>0.0121396899075259</v>
       </c>
       <c r="E24" s="2" t="n">
-        <v>2.02251799986116</v>
+        <v>2.02269208900668</v>
       </c>
       <c r="F24" s="2" t="n">
-        <v>2166.31</v>
-      </c>
-      <c r="G24" s="0" t="n">
-        <f aca="false">F24-F23</f>
-        <v>100.31</v>
+        <v>305</v>
+      </c>
+      <c r="G24" s="3" t="n">
+        <v>93.530000000001</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>124</v>
+        <v>154</v>
       </c>
       <c r="J24" s="2" t="n">
-        <v>4.83921510655197</v>
+        <v>4.74029720513826</v>
       </c>
       <c r="K24" s="2" t="n">
-        <v>0.469664186585207</v>
+        <v>0.488586469425249</v>
       </c>
       <c r="L24" s="2" t="n">
-        <v>0.0083181625092688</v>
+        <v>0.0122937737971205</v>
       </c>
       <c r="M24" s="2" t="n">
-        <v>2.02383834605996</v>
+        <v>2.02259988299427</v>
       </c>
       <c r="N24" s="2" t="n">
-        <v>4291.26</v>
-      </c>
-      <c r="O24" s="0" t="n">
-        <f aca="false">N24-N23</f>
-        <v>197.49</v>
+        <v>765.299999999999</v>
+      </c>
+      <c r="O24" s="3" t="n">
+        <v>184.559999999999</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="R24" s="2" t="n">
-        <v>5.79392894754167</v>
+        <v>10.4142054699306</v>
       </c>
       <c r="S24" s="2" t="n">
-        <v>0.555308152273156</v>
+        <v>0.521703161691092</v>
       </c>
       <c r="T24" s="2" t="n">
-        <v>0.0239942955300447</v>
+        <v>0.00451780384737546</v>
       </c>
       <c r="U24" s="2" t="n">
-        <v>2.02162093489613</v>
+        <v>2.03293730079954</v>
       </c>
       <c r="V24" s="2" t="n">
-        <v>1049.83</v>
-      </c>
-      <c r="W24" s="0" t="n">
-        <f aca="false">V24-V23</f>
-        <v>49.03</v>
+        <v>1341.08</v>
+      </c>
+      <c r="W24" s="3" t="n">
+        <v>49.3</v>
       </c>
       <c r="Y24" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="Z24" s="2" t="n">
-        <v>4.75295112455731</v>
+        <v>5.53061476143937</v>
       </c>
       <c r="AA24" s="2" t="n">
-        <v>0.491596896089408</v>
+        <v>0.544067303981715</v>
       </c>
       <c r="AB24" s="2" t="n">
-        <v>0.0129265590049605</v>
+        <v>0.0228259975865514</v>
       </c>
       <c r="AC24" s="2" t="n">
-        <v>2.02249915173666</v>
+        <v>2.02110545965087</v>
       </c>
       <c r="AD24" s="2" t="n">
-        <v>430.85</v>
-      </c>
-      <c r="AE24" s="0" t="n">
-        <f aca="false">AD24-AD23</f>
-        <v>18.58</v>
+        <v>354.780000000001</v>
+      </c>
+      <c r="AE24" s="3" t="n">
+        <v>21</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="B25" s="2" t="n">
-        <v>4.74077023018602</v>
+        <v>4.73772845282572</v>
       </c>
       <c r="C25" s="2" t="n">
-        <v>0.489806441724872</v>
+        <v>0.48847252756799</v>
       </c>
       <c r="D25" s="2" t="n">
-        <v>0.0123675024655646</v>
+        <v>0.0121601160878525</v>
       </c>
       <c r="E25" s="2" t="n">
-        <v>2.0226003735816</v>
+        <v>2.02269325556195</v>
       </c>
       <c r="F25" s="2" t="n">
-        <v>2265.93</v>
-      </c>
-      <c r="G25" s="0" t="n">
-        <f aca="false">F25-F24</f>
-        <v>99.6199999999999</v>
+        <v>2942.52</v>
+      </c>
+      <c r="G25" s="3" t="n">
+        <v>108.68</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="J25" s="2" t="n">
-        <v>4.73258144253468</v>
+        <v>4.7412878728931</v>
       </c>
       <c r="K25" s="2" t="n">
-        <v>0.485378310158194</v>
+        <v>0.489500503965415</v>
       </c>
       <c r="L25" s="2" t="n">
-        <v>0.0114412614119393</v>
+        <v>0.0123967756173097</v>
       </c>
       <c r="M25" s="2" t="n">
-        <v>2.02289234955163</v>
+        <v>2.0226239150409</v>
       </c>
       <c r="N25" s="2" t="n">
-        <v>4482.82</v>
-      </c>
-      <c r="O25" s="0" t="n">
-        <f aca="false">N25-N24</f>
-        <v>191.56</v>
+        <v>5254.36</v>
+      </c>
+      <c r="O25" s="3" t="n">
+        <v>192.94</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>125</v>
+        <v>151</v>
       </c>
       <c r="R25" s="2" t="n">
-        <v>14.5864054153343</v>
+        <v>10.7344618261651</v>
       </c>
       <c r="S25" s="2" t="n">
-        <v>0.766995285607553</v>
+        <v>0.70250555215571</v>
       </c>
       <c r="T25" s="2" t="n">
-        <v>0.0961933523526666</v>
+        <v>0.0639060190144499</v>
       </c>
       <c r="U25" s="2" t="n">
-        <v>2.01266208930023</v>
+        <v>2.01687084448769</v>
       </c>
       <c r="V25" s="2" t="n">
-        <v>1099.35</v>
-      </c>
-      <c r="W25" s="0" t="n">
-        <f aca="false">V25-V24</f>
-        <v>49.52</v>
+        <v>49.380000000001</v>
+      </c>
+      <c r="W25" s="3" t="n">
+        <v>49.4</v>
       </c>
       <c r="Y25" s="1" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Z25" s="2" t="n">
-        <v>5.79493054981968</v>
+        <v>5.54636459222882</v>
       </c>
       <c r="AA25" s="2" t="n">
-        <v>0.552679315673452</v>
+        <v>0.450301525598511</v>
       </c>
       <c r="AB25" s="2" t="n">
-        <v>0.0257898341104866</v>
+        <v>0.00439832399308458</v>
       </c>
       <c r="AC25" s="2" t="n">
-        <v>2.02039586868464</v>
+        <v>2.02623292995681</v>
       </c>
       <c r="AD25" s="2" t="n">
-        <v>449.73</v>
-      </c>
-      <c r="AE25" s="0" t="n">
-        <f aca="false">AD25-AD24</f>
-        <v>18.88</v>
+        <v>548.75</v>
+      </c>
+      <c r="AE25" s="3" t="n">
+        <v>18.8</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B26" s="2" t="n">
-        <v>4.73324406483686</v>
+        <v>4.73989285970444</v>
       </c>
       <c r="C26" s="2" t="n">
-        <v>0.485726345949523</v>
+        <v>0.488713970621203</v>
       </c>
       <c r="D26" s="2" t="n">
-        <v>0.0116259150426616</v>
+        <v>0.0122874029570318</v>
       </c>
       <c r="E26" s="2" t="n">
-        <v>2.02270430880762</v>
+        <v>2.02251799986116</v>
       </c>
       <c r="F26" s="2" t="n">
-        <v>2365.77</v>
-      </c>
-      <c r="G26" s="0" t="n">
-        <f aca="false">F26-F25</f>
-        <v>99.8400000000002</v>
+        <v>2166.31</v>
+      </c>
+      <c r="G26" s="3" t="n">
+        <v>100.31</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="J26" s="2" t="n">
-        <v>4.73297046133708</v>
+        <v>4.75586731408389</v>
       </c>
       <c r="K26" s="2" t="n">
-        <v>0.48568067262847</v>
+        <v>0.492406089094184</v>
       </c>
       <c r="L26" s="2" t="n">
-        <v>0.0115256045417603</v>
+        <v>0.0130653479416265</v>
       </c>
       <c r="M26" s="2" t="n">
-        <v>2.02288651364477</v>
+        <v>2.02241876561011</v>
       </c>
       <c r="N26" s="2" t="n">
-        <v>4668.56</v>
-      </c>
-      <c r="O26" s="0" t="n">
-        <f aca="false">N26-N25</f>
-        <v>185.740000000001</v>
+        <v>5819.25</v>
+      </c>
+      <c r="O26" s="3" t="n">
+        <v>185.79</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>126</v>
+        <v>149</v>
       </c>
       <c r="R26" s="2" t="n">
-        <v>5.02478243838729</v>
+        <v>11.5474903969739</v>
       </c>
       <c r="S26" s="2" t="n">
-        <v>0.463375459734602</v>
+        <v>0.705731959158286</v>
       </c>
       <c r="T26" s="2" t="n">
-        <v>0.00674916970178051</v>
+        <v>0.0713197949829187</v>
       </c>
       <c r="U26" s="2" t="n">
-        <v>2.02465660221152</v>
+        <v>2.01507962508213</v>
       </c>
       <c r="V26" s="2" t="n">
-        <v>1151.84</v>
-      </c>
-      <c r="W26" s="0" t="n">
-        <f aca="false">V26-V25</f>
-        <v>52.49</v>
+        <v>440.360000000001</v>
+      </c>
+      <c r="W26" s="3" t="n">
+        <v>51.4</v>
       </c>
       <c r="Y26" s="1" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="Z26" s="2" t="n">
-        <v>5.00942022103225</v>
+        <v>5.68621616072169</v>
       </c>
       <c r="AA26" s="2" t="n">
-        <v>0.517117055651651</v>
+        <v>0.550729116328858</v>
       </c>
       <c r="AB26" s="2" t="n">
-        <v>0.0175787935517858</v>
+        <v>0.0241401540325002</v>
       </c>
       <c r="AC26" s="2" t="n">
-        <v>2.02182923249266</v>
+        <v>2.02111164912474</v>
       </c>
       <c r="AD26" s="2" t="n">
-        <v>469.289999999999</v>
-      </c>
-      <c r="AE26" s="0" t="n">
-        <f aca="false">AD26-AD25</f>
-        <v>19.559999999999</v>
+        <v>195.99</v>
+      </c>
+      <c r="AE26" s="3" t="n">
+        <v>18.8</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B27" s="2" t="n">
-        <v>4.73264681850242</v>
+        <v>4.74077023018602</v>
       </c>
       <c r="C27" s="2" t="n">
-        <v>0.484773766799881</v>
+        <v>0.489806441724872</v>
       </c>
       <c r="D27" s="2" t="n">
-        <v>0.011396574020999</v>
+        <v>0.0123675024655646</v>
       </c>
       <c r="E27" s="2" t="n">
-        <v>2.02288556575111</v>
+        <v>2.0226003735816</v>
       </c>
       <c r="F27" s="2" t="n">
-        <v>2460.03</v>
-      </c>
-      <c r="G27" s="0" t="n">
-        <f aca="false">F27-F26</f>
-        <v>94.2600000000002</v>
+        <v>2265.93</v>
+      </c>
+      <c r="G27" s="3" t="n">
+        <v>99.6199999999999</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="J27" s="2" t="n">
-        <v>4.73333615333202</v>
+        <v>4.76321502114731</v>
       </c>
       <c r="K27" s="2" t="n">
-        <v>0.486125326235334</v>
+        <v>0.476441730908921</v>
       </c>
       <c r="L27" s="2" t="n">
-        <v>0.0116741122706659</v>
+        <v>0.00966693539404089</v>
       </c>
       <c r="M27" s="2" t="n">
-        <v>2.02281552024105</v>
+        <v>2.02338793186904</v>
       </c>
       <c r="N27" s="2" t="n">
-        <v>4867.8</v>
-      </c>
-      <c r="O27" s="0" t="n">
-        <f aca="false">N27-N26</f>
-        <v>199.24</v>
+        <v>5633.46</v>
+      </c>
+      <c r="O27" s="3" t="n">
+        <v>186.54</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="R27" s="2" t="n">
-        <v>13.98904397094</v>
+        <v>11.7694177170813</v>
       </c>
       <c r="S27" s="2" t="n">
-        <v>0.763619639914303</v>
+        <v>0.705382587214474</v>
       </c>
       <c r="T27" s="2" t="n">
-        <v>0.0920100943790351</v>
+        <v>0.0728133047891965</v>
       </c>
       <c r="U27" s="2" t="n">
-        <v>2.01332784278771</v>
+        <v>2.01466901234254</v>
       </c>
       <c r="V27" s="2" t="n">
-        <v>1201.69</v>
-      </c>
-      <c r="W27" s="0" t="n">
-        <f aca="false">V27-V26</f>
-        <v>49.8500000000001</v>
+        <v>960.57</v>
+      </c>
+      <c r="W27" s="3" t="n">
+        <v>50.5</v>
       </c>
       <c r="Y27" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="Z27" s="2" t="n">
-        <v>4.73365937265043</v>
+        <v>5.6917015780514</v>
       </c>
       <c r="AA27" s="2" t="n">
-        <v>0.483673565939086</v>
+        <v>0.551282825258859</v>
       </c>
       <c r="AB27" s="2" t="n">
-        <v>0.0111067789602397</v>
+        <v>0.0238474547305066</v>
       </c>
       <c r="AC27" s="2" t="n">
-        <v>2.02299936744483</v>
+        <v>2.02155054029698</v>
       </c>
       <c r="AD27" s="2" t="n">
-        <v>489.35</v>
-      </c>
-      <c r="AE27" s="0" t="n">
-        <f aca="false">AD27-AD26</f>
-        <v>20.060000000001</v>
+        <v>412.27</v>
+      </c>
+      <c r="AE27" s="3" t="n">
+        <v>18.8</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27487,435 +27285,415 @@
       <c r="F28" s="2" t="n">
         <v>2553.17</v>
       </c>
-      <c r="G28" s="0" t="n">
-        <f aca="false">F28-F27</f>
+      <c r="G28" s="3" t="n">
         <v>93.1399999999999</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="J28" s="2" t="n">
-        <v>4.73617492678719</v>
+        <v>4.77669216311506</v>
       </c>
       <c r="K28" s="2" t="n">
-        <v>0.487942072183846</v>
+        <v>0.495414479181898</v>
       </c>
       <c r="L28" s="2" t="n">
-        <v>0.0120623962489738</v>
+        <v>0.0137246373502613</v>
       </c>
       <c r="M28" s="2" t="n">
-        <v>2.02267222431049</v>
+        <v>2.0222695728743</v>
       </c>
       <c r="N28" s="2" t="n">
-        <v>5061.42</v>
-      </c>
-      <c r="O28" s="0" t="n">
-        <f aca="false">N28-N27</f>
-        <v>193.62</v>
+        <v>3105.83</v>
+      </c>
+      <c r="O28" s="3" t="n">
+        <v>184.45</v>
       </c>
       <c r="Q28" s="1" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="R28" s="2" t="n">
-        <v>5.80647672017915</v>
+        <v>11.8556919869248</v>
       </c>
       <c r="S28" s="2" t="n">
-        <v>0.535307628931789</v>
+        <v>0.715741418893173</v>
       </c>
       <c r="T28" s="2" t="n">
-        <v>0.0249516928823957</v>
+        <v>0.0739514877525552</v>
       </c>
       <c r="U28" s="2" t="n">
-        <v>2.01933193331388</v>
+        <v>2.01497036629778</v>
       </c>
       <c r="V28" s="2" t="n">
-        <v>1248.62</v>
-      </c>
-      <c r="W28" s="0" t="n">
-        <f aca="false">V28-V27</f>
-        <v>46.9299999999998</v>
+        <v>652.950000000001</v>
+      </c>
+      <c r="W28" s="3" t="n">
+        <v>42.4</v>
       </c>
       <c r="Y28" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="Z28" s="2" t="n">
-        <v>4.99188121808989</v>
+        <v>5.79493054981968</v>
       </c>
       <c r="AA28" s="2" t="n">
-        <v>0.51621370105816</v>
+        <v>0.552679315673452</v>
       </c>
       <c r="AB28" s="2" t="n">
-        <v>0.0171909710769401</v>
+        <v>0.0257898341104866</v>
       </c>
       <c r="AC28" s="2" t="n">
-        <v>2.02205879088233</v>
+        <v>2.02039586868464</v>
       </c>
       <c r="AD28" s="2" t="n">
-        <v>509.4</v>
-      </c>
-      <c r="AE28" s="0" t="n">
-        <f aca="false">AD28-AD27</f>
-        <v>20.05</v>
+        <v>449.73</v>
+      </c>
+      <c r="AE28" s="3" t="n">
+        <v>18.9</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>129</v>
+        <v>152</v>
       </c>
       <c r="B29" s="2" t="n">
-        <v>4.73449635107517</v>
+        <v>4.74131495839404</v>
       </c>
       <c r="C29" s="2" t="n">
-        <v>0.486680336522834</v>
+        <v>0.489956988361554</v>
       </c>
       <c r="D29" s="2" t="n">
-        <v>0.0118370228419102</v>
+        <v>0.012368679977516</v>
       </c>
       <c r="E29" s="2" t="n">
-        <v>2.02269567770149</v>
+        <v>2.02266395137885</v>
       </c>
       <c r="F29" s="2" t="n">
-        <v>2645.86</v>
-      </c>
-      <c r="G29" s="0" t="n">
-        <f aca="false">F29-F28</f>
-        <v>92.6900000000001</v>
+        <v>784.5</v>
+      </c>
+      <c r="G29" s="3" t="n">
+        <v>99.35</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>129</v>
+        <v>150</v>
       </c>
       <c r="J29" s="2" t="n">
-        <v>4.7412878728931</v>
+        <v>4.79325080296581</v>
       </c>
       <c r="K29" s="2" t="n">
-        <v>0.489500503965415</v>
+        <v>0.498072195395889</v>
       </c>
       <c r="L29" s="2" t="n">
-        <v>0.0123967756173097</v>
+        <v>0.0141764024557666</v>
       </c>
       <c r="M29" s="2" t="n">
-        <v>2.0226239150409</v>
+        <v>2.02222982573153</v>
       </c>
       <c r="N29" s="2" t="n">
-        <v>5254.36</v>
-      </c>
-      <c r="O29" s="0" t="n">
-        <f aca="false">N29-N28</f>
-        <v>192.94</v>
+        <v>1333.63</v>
+      </c>
+      <c r="O29" s="3" t="n">
+        <v>189.65</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="R29" s="2" t="n">
-        <v>5.19172872965442</v>
+        <v>13.98904397094</v>
       </c>
       <c r="S29" s="2" t="n">
-        <v>0.519151033991847</v>
+        <v>0.763619639914303</v>
       </c>
       <c r="T29" s="2" t="n">
-        <v>0.0197758268825193</v>
+        <v>0.0920100943790351</v>
       </c>
       <c r="U29" s="2" t="n">
-        <v>2.02069997880961</v>
+        <v>2.01332784278771</v>
       </c>
       <c r="V29" s="2" t="n">
-        <v>1291.8</v>
-      </c>
-      <c r="W29" s="0" t="n">
-        <f aca="false">V29-V28</f>
-        <v>43.1800000000001</v>
+        <v>1201.69</v>
+      </c>
+      <c r="W29" s="3" t="n">
+        <v>49.9</v>
       </c>
       <c r="Y29" s="1" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="Z29" s="2" t="n">
-        <v>4.73910454348866</v>
+        <v>5.81314261535196</v>
       </c>
       <c r="AA29" s="2" t="n">
-        <v>0.488627287987745</v>
+        <v>0.552438666640035</v>
       </c>
       <c r="AB29" s="2" t="n">
-        <v>0.012247400967034</v>
+        <v>0.0260364439741952</v>
       </c>
       <c r="AC29" s="2" t="n">
-        <v>2.02262960575295</v>
+        <v>2.02006521694369</v>
       </c>
       <c r="AD29" s="2" t="n">
-        <v>529.93</v>
-      </c>
-      <c r="AE29" s="0" t="n">
-        <f aca="false">AD29-AD28</f>
-        <v>20.53</v>
+        <v>314.98</v>
+      </c>
+      <c r="AE29" s="3" t="n">
+        <v>18.1</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>130</v>
+        <v>149</v>
       </c>
       <c r="B30" s="2" t="n">
-        <v>4.73379934517056</v>
+        <v>4.74341171169469</v>
       </c>
       <c r="C30" s="2" t="n">
-        <v>0.482953623448318</v>
+        <v>0.490042199680028</v>
       </c>
       <c r="D30" s="2" t="n">
-        <v>0.0110631897345459</v>
+        <v>0.0125160431424966</v>
       </c>
       <c r="E30" s="2" t="n">
-        <v>2.02297437402652</v>
+        <v>2.02259340337452</v>
       </c>
       <c r="F30" s="2" t="n">
-        <v>2738.61</v>
-      </c>
-      <c r="G30" s="0" t="n">
-        <f aca="false">F30-F29</f>
-        <v>92.75</v>
+        <v>885.129999999999</v>
+      </c>
+      <c r="G30" s="3" t="n">
+        <v>100.629999999999</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="J30" s="2" t="n">
-        <v>4.73271698603789</v>
+        <v>4.80216798492102</v>
       </c>
       <c r="K30" s="2" t="n">
-        <v>0.485055177965332</v>
+        <v>0.498435743334862</v>
       </c>
       <c r="L30" s="2" t="n">
-        <v>0.0114707863057356</v>
+        <v>0.014375442657964</v>
       </c>
       <c r="M30" s="2" t="n">
-        <v>2.02285745534938</v>
+        <v>2.02212274654092</v>
       </c>
       <c r="N30" s="2" t="n">
-        <v>5446.92</v>
-      </c>
-      <c r="O30" s="0" t="n">
-        <f aca="false">N30-N29</f>
-        <v>192.56</v>
+        <v>2130.21</v>
+      </c>
+      <c r="O30" s="3" t="n">
+        <v>201.1</v>
       </c>
       <c r="Q30" s="1" t="s">
-        <v>130</v>
+        <v>146</v>
       </c>
       <c r="R30" s="2" t="n">
-        <v>10.4142054699306</v>
+        <v>14.5297619190541</v>
       </c>
       <c r="S30" s="2" t="n">
-        <v>0.521703161691092</v>
+        <v>0.762478631397603</v>
       </c>
       <c r="T30" s="2" t="n">
-        <v>0.00451780384737546</v>
+        <v>0.0953098289247004</v>
       </c>
       <c r="U30" s="2" t="n">
-        <v>2.03293730079954</v>
+        <v>2.01261747116299</v>
       </c>
       <c r="V30" s="2" t="n">
-        <v>1341.08</v>
-      </c>
-      <c r="W30" s="0" t="n">
-        <f aca="false">V30-V29</f>
-        <v>49.28</v>
+        <v>103.880000000001</v>
+      </c>
+      <c r="W30" s="3" t="n">
+        <v>54.5</v>
       </c>
       <c r="Y30" s="1" t="s">
-        <v>130</v>
+        <v>148</v>
       </c>
       <c r="Z30" s="2" t="n">
-        <v>5.54636459222882</v>
+        <v>6.60147190401879</v>
       </c>
       <c r="AA30" s="2" t="n">
-        <v>0.450301525598511</v>
+        <v>0.581859590187604</v>
       </c>
       <c r="AB30" s="2" t="n">
-        <v>0.00439832399308458</v>
+        <v>0.0322061123393598</v>
       </c>
       <c r="AC30" s="2" t="n">
-        <v>2.02623292995681</v>
+        <v>2.01971131920745</v>
       </c>
       <c r="AD30" s="2" t="n">
-        <v>548.75</v>
-      </c>
-      <c r="AE30" s="0" t="n">
-        <f aca="false">AD30-AD29</f>
-        <v>18.8200000000001</v>
+        <v>100.67</v>
+      </c>
+      <c r="AE30" s="3" t="n">
+        <v>19.3</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="B31" s="2" t="n">
-        <v>4.73297207839648</v>
+        <v>4.74378462377099</v>
       </c>
       <c r="C31" s="2" t="n">
-        <v>0.485639831322016</v>
+        <v>0.490241466189082</v>
       </c>
       <c r="D31" s="2" t="n">
-        <v>0.0115843482428836</v>
+        <v>0.0125382278713031</v>
       </c>
       <c r="E31" s="2" t="n">
-        <v>2.02283240445411</v>
+        <v>2.02258031008103</v>
       </c>
       <c r="F31" s="2" t="n">
-        <v>2833.84</v>
-      </c>
-      <c r="G31" s="0" t="n">
-        <f aca="false">F31-F30</f>
-        <v>95.23</v>
+        <v>2066</v>
+      </c>
+      <c r="G31" s="3" t="n">
+        <v>95.3199999999999</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="J31" s="2" t="n">
-        <v>4.76321502114731</v>
+        <v>4.83921510655197</v>
       </c>
       <c r="K31" s="2" t="n">
-        <v>0.476441730908921</v>
+        <v>0.469664186585207</v>
       </c>
       <c r="L31" s="2" t="n">
-        <v>0.00966693539404089</v>
+        <v>0.0083181625092688</v>
       </c>
       <c r="M31" s="2" t="n">
-        <v>2.02338793186904</v>
+        <v>2.02383834605996</v>
       </c>
       <c r="N31" s="2" t="n">
-        <v>5633.46</v>
-      </c>
-      <c r="O31" s="0" t="n">
-        <f aca="false">N31-N30</f>
-        <v>186.54</v>
+        <v>4291.26</v>
+      </c>
+      <c r="O31" s="3" t="n">
+        <v>197.49</v>
       </c>
       <c r="Q31" s="1" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="R31" s="2" t="n">
-        <v>7.23738434138332</v>
+        <v>14.5582643173828</v>
       </c>
       <c r="S31" s="2" t="n">
-        <v>0.563485655514734</v>
+        <v>0.774988228655992</v>
       </c>
       <c r="T31" s="2" t="n">
-        <v>0.0345598346150393</v>
+        <v>0.096873528581999</v>
       </c>
       <c r="U31" s="2" t="n">
-        <v>2.01727669965836</v>
+        <v>2.0129974060995</v>
       </c>
       <c r="V31" s="2" t="n">
-        <v>1391.8</v>
-      </c>
-      <c r="W31" s="0" t="n">
-        <f aca="false">V31-V30</f>
-        <v>50.72</v>
+        <v>610.59</v>
+      </c>
+      <c r="W31" s="3" t="n">
+        <v>54.7</v>
       </c>
       <c r="Y31" s="1" t="s">
-        <v>131</v>
+        <v>151</v>
       </c>
       <c r="Z31" s="2" t="n">
-        <v>8.71009886078587</v>
+        <v>6.69584862019204</v>
       </c>
       <c r="AA31" s="2" t="n">
-        <v>0.628011529441782</v>
+        <v>0.573781261508616</v>
       </c>
       <c r="AB31" s="2" t="n">
-        <v>0.0485381822999904</v>
+        <v>0.0333309402681</v>
       </c>
       <c r="AC31" s="2" t="n">
-        <v>2.01471658138896</v>
+        <v>2.01851960457967</v>
       </c>
       <c r="AD31" s="2" t="n">
-        <v>567.440000000001</v>
-      </c>
-      <c r="AE31" s="0" t="n">
-        <f aca="false">AD31-AD30</f>
-        <v>18.690000000001</v>
+        <v>22.7600000000002</v>
+      </c>
+      <c r="AE31" s="3" t="n">
+        <v>22.8</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="B32" s="2" t="n">
-        <v>4.73772845282572</v>
+        <v>4.79348280829329</v>
       </c>
       <c r="C32" s="2" t="n">
-        <v>0.48847252756799</v>
+        <v>0.498066450857373</v>
       </c>
       <c r="D32" s="2" t="n">
-        <v>0.0121601160878525</v>
+        <v>0.0141821487240554</v>
       </c>
       <c r="E32" s="2" t="n">
-        <v>2.02269325556195</v>
+        <v>2.02223163265957</v>
       </c>
       <c r="F32" s="2" t="n">
-        <v>2942.52</v>
-      </c>
-      <c r="G32" s="0" t="n">
-        <f aca="false">F32-F31</f>
-        <v>108.68</v>
+        <v>1970.68</v>
+      </c>
+      <c r="G32" s="3" t="n">
+        <v>99.1700000000001</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>132</v>
+        <v>146</v>
       </c>
       <c r="J32" s="2" t="n">
-        <v>4.75586731408389</v>
+        <v>4.84794027256065</v>
       </c>
       <c r="K32" s="2" t="n">
-        <v>0.492406089094184</v>
+        <v>0.501964506312286</v>
       </c>
       <c r="L32" s="2" t="n">
-        <v>0.0130653479416265</v>
+        <v>0.0152840476580599</v>
       </c>
       <c r="M32" s="2" t="n">
-        <v>2.02241876561011</v>
+        <v>2.02184590448036</v>
       </c>
       <c r="N32" s="2" t="n">
-        <v>5819.25</v>
-      </c>
-      <c r="O32" s="0" t="n">
-        <f aca="false">N32-N31</f>
-        <v>185.79</v>
+        <v>391.849999999999</v>
+      </c>
+      <c r="O32" s="3" t="n">
+        <v>191.55</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="R32" s="2" t="n">
-        <v>6.79126082662106</v>
+        <v>14.5864054153343</v>
       </c>
       <c r="S32" s="2" t="n">
-        <v>0.587057909370176</v>
+        <v>0.766995285607553</v>
       </c>
       <c r="T32" s="2" t="n">
-        <v>0.0338481485476043</v>
+        <v>0.0961933523526666</v>
       </c>
       <c r="U32" s="2" t="n">
-        <v>2.01945480387697</v>
+        <v>2.01266208930023</v>
       </c>
       <c r="V32" s="2" t="n">
-        <v>1438.69</v>
-      </c>
-      <c r="W32" s="0" t="n">
-        <f aca="false">V32-V31</f>
-        <v>46.8900000000001</v>
+        <v>1099.35</v>
+      </c>
+      <c r="W32" s="3" t="n">
+        <v>49.5</v>
       </c>
       <c r="Y32" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Z32" s="2" t="n">
-        <v>5.29161793897107</v>
+        <v>8.71009886078587</v>
       </c>
       <c r="AA32" s="2" t="n">
-        <v>0.532915414088237</v>
+        <v>0.628011529441782</v>
       </c>
       <c r="AB32" s="2" t="n">
-        <v>0.0200434216808821</v>
+        <v>0.0485381822999904</v>
       </c>
       <c r="AC32" s="2" t="n">
-        <v>2.02112866865988</v>
+        <v>2.01471658138896</v>
       </c>
       <c r="AD32" s="2" t="n">
-        <v>586.110000000001</v>
-      </c>
-      <c r="AE32" s="0" t="n">
-        <f aca="false">AD32-AD31</f>
-        <v>18.6700000000001</v>
+        <v>567.440000000001</v>
+      </c>
+      <c r="AE32" s="3" t="n">
+        <v>18.7</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27929,20 +27707,21 @@
       <c r="F34" s="0" t="s">
         <v>155</v>
       </c>
-      <c r="G34" s="0" t="n">
+      <c r="G34" s="3" t="n">
         <f aca="false">MIN(G3:G32)</f>
         <v>92.51</v>
       </c>
       <c r="I34" s="0" t="s">
         <v>155</v>
       </c>
-      <c r="J34" s="3" t="n">
-        <v>4.73248753274178</v>
+      <c r="J34" s="0" t="n">
+        <f aca="false">MIN(J3:J32)</f>
+        <v>4.73241918756398</v>
       </c>
       <c r="N34" s="0" t="s">
         <v>155</v>
       </c>
-      <c r="O34" s="0" t="n">
+      <c r="O34" s="3" t="n">
         <f aca="false">MIN(O3:O32)</f>
         <v>184.45</v>
       </c>
@@ -27956,9 +27735,9 @@
       <c r="V34" s="0" t="s">
         <v>155</v>
       </c>
-      <c r="W34" s="0" t="n">
+      <c r="W34" s="3" t="n">
         <f aca="false">MIN(W3:W32)</f>
-        <v>38.3300000000021</v>
+        <v>38.3</v>
       </c>
       <c r="Y34" s="0" t="s">
         <v>155</v>
@@ -27970,9 +27749,9 @@
       <c r="AD34" s="0" t="s">
         <v>155</v>
       </c>
-      <c r="AE34" s="0" t="n">
+      <c r="AE34" s="3" t="n">
         <f aca="false">MIN(AE3:AE32)</f>
-        <v>18.08</v>
+        <v>18.1</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27986,7 +27765,7 @@
       <c r="F35" s="0" t="s">
         <v>156</v>
       </c>
-      <c r="G35" s="0" t="n">
+      <c r="G35" s="3" t="n">
         <f aca="false">AVERAGE(G3:G32)</f>
         <v>98.084</v>
       </c>
@@ -28000,7 +27779,7 @@
       <c r="N35" s="0" t="s">
         <v>156</v>
       </c>
-      <c r="O35" s="0" t="n">
+      <c r="O35" s="3" t="n">
         <f aca="false">AVERAGE(O3:O32)</f>
         <v>193.975</v>
       </c>
@@ -28014,9 +27793,9 @@
       <c r="V35" s="0" t="s">
         <v>156</v>
       </c>
-      <c r="W35" s="0" t="n">
+      <c r="W35" s="3" t="n">
         <f aca="false">AVERAGE(W3:W32)</f>
-        <v>47.9563333333333</v>
+        <v>47.96</v>
       </c>
       <c r="Y35" s="0" t="s">
         <v>156</v>
@@ -28028,9 +27807,9 @@
       <c r="AD35" s="0" t="s">
         <v>156</v>
       </c>
-      <c r="AE35" s="0" t="n">
+      <c r="AE35" s="3" t="n">
         <f aca="false">AVERAGE(AE3:AE32)</f>
-        <v>19.537</v>
+        <v>19.5433333333333</v>
       </c>
     </row>
   </sheetData>
@@ -28045,17 +27824,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="M15" activeCellId="0" sqref="M15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.1640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="6.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -29255,17 +29034,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AC32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="6.71"/>
   </cols>
@@ -29949,17 +29728,17 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="7.98"/>
   </cols>

</xml_diff>

<commit_message>
add 300/30 results from ubuntu to use in final paper
</commit_message>
<xml_diff>
--- a/results_from_all_algos.xlsx
+++ b/results_from_all_algos.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="161">
   <si>
     <t xml:space="preserve">ITER#</t>
   </si>
@@ -452,6 +452,12 @@
     <t xml:space="preserve">time d</t>
   </si>
   <si>
+    <t xml:space="preserve">Ubuntu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OSX</t>
+  </si>
+  <si>
     <t xml:space="preserve">Agents 1000 iters 30</t>
   </si>
   <si>
@@ -464,6 +470,9 @@
     <t xml:space="preserve">Agents 300 iters 30</t>
   </si>
   <si>
+    <t xml:space="preserve">r01</t>
+  </si>
+  <si>
     <t xml:space="preserve">r02</t>
   </si>
   <si>
@@ -473,22 +482,19 @@
     <t xml:space="preserve">r05</t>
   </si>
   <si>
+    <t xml:space="preserve">r04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r06</t>
+  </si>
+  <si>
     <t xml:space="preserve">r09</t>
   </si>
   <si>
     <t xml:space="preserve">r07</t>
   </si>
   <si>
-    <t xml:space="preserve">r01</t>
-  </si>
-  <si>
     <t xml:space="preserve">r08</t>
-  </si>
-  <si>
-    <t xml:space="preserve">r06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">r04</t>
   </si>
   <si>
     <t xml:space="preserve">MIN:</t>
@@ -640,7 +646,7 @@
       <selection pane="bottomRight" activeCell="B102" activeCellId="0" sqref="B102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="6.8125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.77"/>
   </cols>
@@ -24992,25 +24998,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AE35"/>
+  <dimension ref="A1:AM78"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="topRight" activeCell="N1" activeCellId="0" sqref="N1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N26" activeCellId="0" sqref="N26"/>
+      <selection pane="bottomRight" activeCell="T14" activeCellId="0" sqref="T14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="6.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.42"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="6.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="6.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="8.37"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="15" min="15" style="3" width="6.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="23" min="23" style="3" width="6.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="31" min="31" style="3" width="6.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="15" min="15" style="3" width="6.54"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="23" min="23" style="3" width="6.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="7.34"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="31" min="31" style="3" width="6.54"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25068,6 +25075,9 @@
       <c r="W1" s="4" t="s">
         <v>141</v>
       </c>
+      <c r="Y1" s="1" t="s">
+        <v>142</v>
+      </c>
       <c r="Z1" s="1" t="s">
         <v>136</v>
       </c>
@@ -25084,6 +25094,27 @@
         <v>140</v>
       </c>
       <c r="AE1" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AM1" s="4" t="s">
         <v>141</v>
       </c>
     </row>
@@ -25092,29 +25123,39 @@
         <v>101</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>101</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>101</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="Y2" s="1" t="s">
         <v>101</v>
       </c>
       <c r="Z2" s="1"/>
       <c r="AA2" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="AB2" s="1"/>
       <c r="AC2" s="1"/>
+      <c r="AG2" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AH2" s="1"/>
+      <c r="AI2" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="AJ2" s="1"/>
+      <c r="AK2" s="1"/>
+      <c r="AM2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
@@ -25181,30 +25222,51 @@
         <v>41.3</v>
       </c>
       <c r="Y3" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="Z3" s="2" t="n">
+        <v>4.86356438852961</v>
+      </c>
+      <c r="AA3" s="2" t="n">
+        <v>0.504327450355697</v>
+      </c>
+      <c r="AB3" s="2" t="n">
+        <v>0.0156192840811044</v>
+      </c>
+      <c r="AC3" s="2" t="n">
+        <v>2.02187308174304</v>
+      </c>
+      <c r="AD3" s="2" t="n">
+        <v>65.1999999999999</v>
+      </c>
+      <c r="AE3" s="3" t="n">
+        <v>65.2</v>
+      </c>
+      <c r="AG3" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="Z3" s="2" t="n">
+      <c r="AH3" s="2" t="n">
         <v>4.73365937265043</v>
       </c>
-      <c r="AA3" s="2" t="n">
+      <c r="AI3" s="2" t="n">
         <v>0.483673565939086</v>
       </c>
-      <c r="AB3" s="2" t="n">
+      <c r="AJ3" s="2" t="n">
         <v>0.0111067789602397</v>
       </c>
-      <c r="AC3" s="2" t="n">
+      <c r="AK3" s="2" t="n">
         <v>2.02299936744483</v>
       </c>
-      <c r="AD3" s="2" t="n">
+      <c r="AL3" s="2" t="n">
         <v>489.35</v>
       </c>
-      <c r="AE3" s="3" t="n">
+      <c r="AM3" s="3" t="n">
         <v>20.1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>4.73251624066684</v>
@@ -25267,24 +25329,45 @@
         <v>38.3</v>
       </c>
       <c r="Y4" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="Z4" s="2" t="n">
+        <v>7.28021806479377</v>
+      </c>
+      <c r="AA4" s="2" t="n">
+        <v>0.598369533687176</v>
+      </c>
+      <c r="AB4" s="2" t="n">
+        <v>0.0379497203548564</v>
+      </c>
+      <c r="AC4" s="2" t="n">
+        <v>2.01859903118994</v>
+      </c>
+      <c r="AD4" s="2" t="n">
+        <v>97.89</v>
+      </c>
+      <c r="AE4" s="3" t="n">
+        <v>32.7</v>
+      </c>
+      <c r="AG4" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="AH4" s="2" t="n">
         <v>4.73609256977679</v>
       </c>
-      <c r="AA4" s="2" t="n">
+      <c r="AI4" s="2" t="n">
         <v>0.487641598070697</v>
       </c>
-      <c r="AB4" s="2" t="n">
+      <c r="AJ4" s="2" t="n">
         <v>0.0120176090070576</v>
       </c>
-      <c r="AC4" s="2" t="n">
+      <c r="AK4" s="2" t="n">
         <v>2.02271261361793</v>
       </c>
-      <c r="AD4" s="2" t="n">
+      <c r="AL4" s="2" t="n">
         <v>62.2899999999991</v>
       </c>
-      <c r="AE4" s="3" t="n">
+      <c r="AM4" s="3" t="n">
         <v>18.9</v>
       </c>
     </row>
@@ -25353,30 +25436,51 @@
         <v>40</v>
       </c>
       <c r="Y5" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="Z5" s="2" t="n">
+        <v>4.7524336666441</v>
+      </c>
+      <c r="AA5" s="2" t="n">
+        <v>0.477368553310623</v>
+      </c>
+      <c r="AB5" s="2" t="n">
+        <v>0.0100558370758962</v>
+      </c>
+      <c r="AC5" s="2" t="n">
+        <v>2.0231548857447</v>
+      </c>
+      <c r="AD5" s="2" t="n">
+        <v>130.97</v>
+      </c>
+      <c r="AE5" s="3" t="n">
+        <v>33.1</v>
+      </c>
+      <c r="AG5" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="Z5" s="2" t="n">
+      <c r="AH5" s="2" t="n">
         <v>4.73758688292009</v>
       </c>
-      <c r="AA5" s="2" t="n">
+      <c r="AI5" s="2" t="n">
         <v>0.488527002970693</v>
       </c>
-      <c r="AB5" s="2" t="n">
+      <c r="AJ5" s="2" t="n">
         <v>0.0121472607154107</v>
       </c>
-      <c r="AC5" s="2" t="n">
+      <c r="AK5" s="2" t="n">
         <v>2.02271148184962</v>
       </c>
-      <c r="AD5" s="2" t="n">
+      <c r="AL5" s="2" t="n">
         <v>215.120000000001</v>
       </c>
-      <c r="AE5" s="3" t="n">
+      <c r="AM5" s="3" t="n">
         <v>19.1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>4.73256901104308</v>
@@ -25397,7 +25501,7 @@
         <v>92.51</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="J6" s="2" t="n">
         <v>4.73272127602358</v>
@@ -25418,7 +25522,7 @@
         <v>188.709999999999</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="R6" s="2" t="n">
         <v>4.77334183599085</v>
@@ -25439,24 +25543,45 @@
         <v>44.8</v>
       </c>
       <c r="Y6" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="Z6" s="2" t="n">
+        <v>5.48662926647256</v>
+      </c>
+      <c r="AA6" s="2" t="n">
+        <v>0.542184416506497</v>
+      </c>
+      <c r="AB6" s="2" t="n">
+        <v>0.0212980650626486</v>
+      </c>
+      <c r="AC6" s="2" t="n">
+        <v>2.02203990812736</v>
+      </c>
+      <c r="AD6" s="2" t="n">
+        <v>164.59</v>
+      </c>
+      <c r="AE6" s="3" t="n">
+        <v>33.6</v>
+      </c>
+      <c r="AG6" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="Z6" s="2" t="n">
+      <c r="AH6" s="2" t="n">
         <v>4.73910454348866</v>
       </c>
-      <c r="AA6" s="2" t="n">
+      <c r="AI6" s="2" t="n">
         <v>0.488627287987745</v>
       </c>
-      <c r="AB6" s="2" t="n">
+      <c r="AJ6" s="2" t="n">
         <v>0.012247400967034</v>
       </c>
-      <c r="AC6" s="2" t="n">
+      <c r="AK6" s="2" t="n">
         <v>2.02262960575295</v>
       </c>
-      <c r="AD6" s="2" t="n">
+      <c r="AL6" s="2" t="n">
         <v>529.93</v>
       </c>
-      <c r="AE6" s="3" t="n">
+      <c r="AM6" s="3" t="n">
         <v>20.5</v>
       </c>
     </row>
@@ -25504,7 +25629,7 @@
         <v>199.47</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="R7" s="2" t="n">
         <v>4.84804171549978</v>
@@ -25525,24 +25650,45 @@
         <v>41.3</v>
       </c>
       <c r="Y7" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="Z7" s="2" t="n">
+        <v>5.09305097312991</v>
+      </c>
+      <c r="AA7" s="2" t="n">
+        <v>0.517771688199338</v>
+      </c>
+      <c r="AB7" s="2" t="n">
+        <v>0.0188648082114728</v>
+      </c>
+      <c r="AC7" s="2" t="n">
+        <v>2.02079930590026</v>
+      </c>
+      <c r="AD7" s="2" t="n">
+        <v>200.63</v>
+      </c>
+      <c r="AE7" s="3" t="n">
+        <v>36</v>
+      </c>
+      <c r="AG7" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="Z7" s="2" t="n">
+      <c r="AH7" s="2" t="n">
         <v>4.75295112455731</v>
       </c>
-      <c r="AA7" s="2" t="n">
+      <c r="AI7" s="2" t="n">
         <v>0.491596896089408</v>
       </c>
-      <c r="AB7" s="2" t="n">
+      <c r="AJ7" s="2" t="n">
         <v>0.0129265590049605</v>
       </c>
-      <c r="AC7" s="2" t="n">
+      <c r="AK7" s="2" t="n">
         <v>2.02249915173666</v>
       </c>
-      <c r="AD7" s="2" t="n">
+      <c r="AL7" s="2" t="n">
         <v>430.85</v>
       </c>
-      <c r="AE7" s="3" t="n">
+      <c r="AM7" s="3" t="n">
         <v>18.6</v>
       </c>
     </row>
@@ -25611,30 +25757,51 @@
         <v>52.5</v>
       </c>
       <c r="Y8" s="1" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="Z8" s="2" t="n">
+        <v>9.35380705222917</v>
+      </c>
+      <c r="AA8" s="2" t="n">
+        <v>0.647801052334451</v>
+      </c>
+      <c r="AB8" s="2" t="n">
+        <v>0.0538128231268597</v>
+      </c>
+      <c r="AC8" s="2" t="n">
+        <v>2.01689846802921</v>
+      </c>
+      <c r="AD8" s="2" t="n">
+        <v>233.92</v>
+      </c>
+      <c r="AE8" s="3" t="n">
+        <v>33.3</v>
+      </c>
+      <c r="AG8" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="AH8" s="2" t="n">
         <v>4.7616530580448</v>
       </c>
-      <c r="AA8" s="2" t="n">
+      <c r="AI8" s="2" t="n">
         <v>0.484889808225817</v>
       </c>
-      <c r="AB8" s="2" t="n">
+      <c r="AJ8" s="2" t="n">
         <v>0.0120590748985078</v>
       </c>
-      <c r="AC8" s="2" t="n">
+      <c r="AK8" s="2" t="n">
         <v>2.0224987497498</v>
       </c>
-      <c r="AD8" s="2" t="n">
+      <c r="AL8" s="2" t="n">
         <v>177.17</v>
       </c>
-      <c r="AE8" s="3" t="n">
+      <c r="AM8" s="3" t="n">
         <v>19.3</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="B9" s="2" t="n">
         <v>4.73264877533292</v>
@@ -25697,30 +25864,51 @@
         <v>43.2</v>
       </c>
       <c r="Y9" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z9" s="2" t="n">
+        <v>4.74324957927919</v>
+      </c>
+      <c r="AA9" s="2" t="n">
+        <v>0.488850859455097</v>
+      </c>
+      <c r="AB9" s="2" t="n">
+        <v>0.0124140993857067</v>
+      </c>
+      <c r="AC9" s="2" t="n">
+        <v>2.02253155646686</v>
+      </c>
+      <c r="AD9" s="2" t="n">
+        <v>266.6</v>
+      </c>
+      <c r="AE9" s="3" t="n">
+        <v>32.7</v>
+      </c>
+      <c r="AG9" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="Z9" s="2" t="n">
+      <c r="AH9" s="2" t="n">
         <v>4.76757257254872</v>
       </c>
-      <c r="AA9" s="2" t="n">
+      <c r="AI9" s="2" t="n">
         <v>0.494714017032156</v>
       </c>
-      <c r="AB9" s="2" t="n">
+      <c r="AJ9" s="2" t="n">
         <v>0.0134696460555681</v>
       </c>
-      <c r="AC9" s="2" t="n">
+      <c r="AK9" s="2" t="n">
         <v>2.02238460546414</v>
       </c>
-      <c r="AD9" s="2" t="n">
+      <c r="AL9" s="2" t="n">
         <v>274.950000000001</v>
       </c>
-      <c r="AE9" s="3" t="n">
+      <c r="AM9" s="3" t="n">
         <v>21.3</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B10" s="2" t="n">
         <v>4.73282705256699</v>
@@ -25783,24 +25971,45 @@
         <v>51.7</v>
       </c>
       <c r="Y10" s="1" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="Z10" s="2" t="n">
+        <v>4.73266263880405</v>
+      </c>
+      <c r="AA10" s="2" t="n">
+        <v>0.484997268353348</v>
+      </c>
+      <c r="AB10" s="2" t="n">
+        <v>0.0114389330008822</v>
+      </c>
+      <c r="AC10" s="2" t="n">
+        <v>2.02287735189339</v>
+      </c>
+      <c r="AD10" s="2" t="n">
+        <v>299.06</v>
+      </c>
+      <c r="AE10" s="3" t="n">
+        <v>32.5</v>
+      </c>
+      <c r="AG10" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AH10" s="2" t="n">
         <v>4.77622194267296</v>
       </c>
-      <c r="AA10" s="2" t="n">
+      <c r="AI10" s="2" t="n">
         <v>0.494577810189531</v>
       </c>
-      <c r="AB10" s="2" t="n">
+      <c r="AJ10" s="2" t="n">
         <v>0.013660038381724</v>
       </c>
-      <c r="AC10" s="2" t="n">
+      <c r="AK10" s="2" t="n">
         <v>2.02214118791182</v>
       </c>
-      <c r="AD10" s="2" t="n">
+      <c r="AL10" s="2" t="n">
         <v>157.9</v>
       </c>
-      <c r="AE10" s="3" t="n">
+      <c r="AM10" s="3" t="n">
         <v>18.9</v>
       </c>
     </row>
@@ -25869,24 +26078,45 @@
         <v>52.8</v>
       </c>
       <c r="Y11" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="Z11" s="2" t="n">
+        <v>4.74661936612423</v>
+      </c>
+      <c r="AA11" s="2" t="n">
+        <v>0.490697904641289</v>
+      </c>
+      <c r="AB11" s="2" t="n">
+        <v>0.0126739534959147</v>
+      </c>
+      <c r="AC11" s="2" t="n">
+        <v>2.02254496690695</v>
+      </c>
+      <c r="AD11" s="2" t="n">
+        <v>330.86</v>
+      </c>
+      <c r="AE11" s="3" t="n">
+        <v>31.8</v>
+      </c>
+      <c r="AG11" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="Z11" s="2" t="n">
+      <c r="AH11" s="2" t="n">
         <v>4.81435007595051</v>
       </c>
-      <c r="AA11" s="2" t="n">
+      <c r="AI11" s="2" t="n">
         <v>0.500509530146158</v>
       </c>
-      <c r="AB11" s="2" t="n">
+      <c r="AJ11" s="2" t="n">
         <v>0.0146612144728454</v>
       </c>
-      <c r="AC11" s="2" t="n">
+      <c r="AK11" s="2" t="n">
         <v>2.02218110450913</v>
       </c>
-      <c r="AD11" s="2" t="n">
+      <c r="AL11" s="2" t="n">
         <v>234.93</v>
       </c>
-      <c r="AE11" s="3" t="n">
+      <c r="AM11" s="3" t="n">
         <v>19.8</v>
       </c>
     </row>
@@ -25934,7 +26164,7 @@
         <v>199.38</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="R12" s="2" t="n">
         <v>5.34689717187448</v>
@@ -25955,24 +26185,45 @@
         <v>46.6</v>
       </c>
       <c r="Y12" s="1" t="s">
-        <v>154</v>
+        <v>112</v>
       </c>
       <c r="Z12" s="2" t="n">
+        <v>4.73469303823187</v>
+      </c>
+      <c r="AA12" s="2" t="n">
+        <v>0.487095598471187</v>
+      </c>
+      <c r="AB12" s="2" t="n">
+        <v>0.0118772039865056</v>
+      </c>
+      <c r="AC12" s="2" t="n">
+        <v>2.02276366398417</v>
+      </c>
+      <c r="AD12" s="2" t="n">
+        <v>363.26</v>
+      </c>
+      <c r="AE12" s="3" t="n">
+        <v>32.4</v>
+      </c>
+      <c r="AG12" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AH12" s="2" t="n">
         <v>4.86063198429821</v>
       </c>
-      <c r="AA12" s="2" t="n">
+      <c r="AI12" s="2" t="n">
         <v>0.505927587799093</v>
       </c>
-      <c r="AB12" s="2" t="n">
+      <c r="AJ12" s="2" t="n">
         <v>0.0154304267644149</v>
       </c>
-      <c r="AC12" s="2" t="n">
+      <c r="AK12" s="2" t="n">
         <v>2.02210058835512</v>
       </c>
-      <c r="AD12" s="2" t="n">
+      <c r="AL12" s="2" t="n">
         <v>81.3600000000006</v>
       </c>
-      <c r="AE12" s="3" t="n">
+      <c r="AM12" s="3" t="n">
         <v>19.1</v>
       </c>
     </row>
@@ -26041,24 +26292,45 @@
         <v>49</v>
       </c>
       <c r="Y13" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z13" s="2" t="n">
+        <v>4.76529694877274</v>
+      </c>
+      <c r="AA13" s="2" t="n">
+        <v>0.495132989352963</v>
+      </c>
+      <c r="AB13" s="2" t="n">
+        <v>0.0132952541770227</v>
+      </c>
+      <c r="AC13" s="2" t="n">
+        <v>2.0225856494745</v>
+      </c>
+      <c r="AD13" s="2" t="n">
+        <v>396.35</v>
+      </c>
+      <c r="AE13" s="3" t="n">
+        <v>33.1</v>
+      </c>
+      <c r="AG13" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="Z13" s="2" t="n">
+      <c r="AH13" s="2" t="n">
         <v>4.86966307436344</v>
       </c>
-      <c r="AA13" s="2" t="n">
+      <c r="AI13" s="2" t="n">
         <v>0.502964956823651</v>
       </c>
-      <c r="AB13" s="2" t="n">
+      <c r="AJ13" s="2" t="n">
         <v>0.0156250656601103</v>
       </c>
-      <c r="AC13" s="2" t="n">
+      <c r="AK13" s="2" t="n">
         <v>2.02172328591852</v>
       </c>
-      <c r="AD13" s="2" t="n">
+      <c r="AL13" s="2" t="n">
         <v>393.49</v>
       </c>
-      <c r="AE13" s="3" t="n">
+      <c r="AM13" s="3" t="n">
         <v>19.5</v>
       </c>
     </row>
@@ -26127,24 +26399,45 @@
         <v>46.9</v>
       </c>
       <c r="Y14" s="1" t="s">
-        <v>146</v>
+        <v>114</v>
       </c>
       <c r="Z14" s="2" t="n">
+        <v>5.04995954226894</v>
+      </c>
+      <c r="AA14" s="2" t="n">
+        <v>0.460323892187751</v>
+      </c>
+      <c r="AB14" s="2" t="n">
+        <v>0.00648283140461326</v>
+      </c>
+      <c r="AC14" s="2" t="n">
+        <v>2.02455660055288</v>
+      </c>
+      <c r="AD14" s="2" t="n">
+        <v>431</v>
+      </c>
+      <c r="AE14" s="3" t="n">
+        <v>34.7</v>
+      </c>
+      <c r="AG14" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="AH14" s="2" t="n">
         <v>4.93002892499933</v>
       </c>
-      <c r="AA14" s="2" t="n">
+      <c r="AI14" s="2" t="n">
         <v>0.510256231968616</v>
       </c>
-      <c r="AB14" s="2" t="n">
+      <c r="AJ14" s="2" t="n">
         <v>0.0167051762212759</v>
       </c>
-      <c r="AC14" s="2" t="n">
+      <c r="AK14" s="2" t="n">
         <v>2.02173487369732</v>
       </c>
-      <c r="AD14" s="2" t="n">
+      <c r="AL14" s="2" t="n">
         <v>43.3400000000001</v>
       </c>
-      <c r="AE14" s="3" t="n">
+      <c r="AM14" s="3" t="n">
         <v>20.6</v>
       </c>
     </row>
@@ -26171,7 +26464,7 @@
         <v>99.8400000000002</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J15" s="2" t="n">
         <v>4.73384437044199</v>
@@ -26213,24 +26506,45 @@
         <v>62.8</v>
       </c>
       <c r="Y15" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="Z15" s="2" t="n">
+        <v>4.86539203629354</v>
+      </c>
+      <c r="AA15" s="2" t="n">
+        <v>0.500056796188537</v>
+      </c>
+      <c r="AB15" s="2" t="n">
+        <v>0.0152918667408611</v>
+      </c>
+      <c r="AC15" s="2" t="n">
+        <v>2.02160984848279</v>
+      </c>
+      <c r="AD15" s="2" t="n">
+        <v>463.7</v>
+      </c>
+      <c r="AE15" s="3" t="n">
+        <v>32.7</v>
+      </c>
+      <c r="AG15" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="Z15" s="2" t="n">
+      <c r="AH15" s="2" t="n">
         <v>4.99188121808989</v>
       </c>
-      <c r="AA15" s="2" t="n">
+      <c r="AI15" s="2" t="n">
         <v>0.51621370105816</v>
       </c>
-      <c r="AB15" s="2" t="n">
+      <c r="AJ15" s="2" t="n">
         <v>0.0171909710769401</v>
       </c>
-      <c r="AC15" s="2" t="n">
+      <c r="AK15" s="2" t="n">
         <v>2.02205879088233</v>
       </c>
-      <c r="AD15" s="2" t="n">
+      <c r="AL15" s="2" t="n">
         <v>509.4</v>
       </c>
-      <c r="AE15" s="3" t="n">
+      <c r="AM15" s="3" t="n">
         <v>20.1</v>
       </c>
     </row>
@@ -26299,24 +26613,45 @@
         <v>52.7</v>
       </c>
       <c r="Y16" s="1" t="s">
-        <v>150</v>
+        <v>116</v>
       </c>
       <c r="Z16" s="2" t="n">
+        <v>5.6660097928394</v>
+      </c>
+      <c r="AA16" s="2" t="n">
+        <v>0.546767591444701</v>
+      </c>
+      <c r="AB16" s="2" t="n">
+        <v>0.0247173882295023</v>
+      </c>
+      <c r="AC16" s="2" t="n">
+        <v>2.02013387440375</v>
+      </c>
+      <c r="AD16" s="2" t="n">
+        <v>496.53</v>
+      </c>
+      <c r="AE16" s="3" t="n">
+        <v>32.8</v>
+      </c>
+      <c r="AG16" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="AH16" s="2" t="n">
         <v>5.00113948180471</v>
       </c>
-      <c r="AA16" s="2" t="n">
+      <c r="AI16" s="2" t="n">
         <v>0.509737160282644</v>
       </c>
-      <c r="AB16" s="2" t="n">
+      <c r="AJ16" s="2" t="n">
         <v>0.0174673638832025</v>
       </c>
-      <c r="AC16" s="2" t="n">
+      <c r="AK16" s="2" t="n">
         <v>2.02103148452504</v>
       </c>
-      <c r="AD16" s="2" t="n">
+      <c r="AL16" s="2" t="n">
         <v>138.969999999999</v>
       </c>
-      <c r="AE16" s="3" t="n">
+      <c r="AM16" s="3" t="n">
         <v>19.2</v>
       </c>
     </row>
@@ -26343,7 +26678,7 @@
         <v>92.75</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="J17" s="2" t="n">
         <v>4.73605216732573</v>
@@ -26385,24 +26720,45 @@
         <v>42.2</v>
       </c>
       <c r="Y17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z17" s="2" t="n">
+        <v>5.11570901472011</v>
+      </c>
+      <c r="AA17" s="2" t="n">
+        <v>0.518979393499904</v>
+      </c>
+      <c r="AB17" s="2" t="n">
+        <v>0.0191454512046032</v>
+      </c>
+      <c r="AC17" s="2" t="n">
+        <v>2.02093556719077</v>
+      </c>
+      <c r="AD17" s="2" t="n">
+        <v>528.65</v>
+      </c>
+      <c r="AE17" s="3" t="n">
+        <v>32.1</v>
+      </c>
+      <c r="AG17" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="Z17" s="2" t="n">
+      <c r="AH17" s="2" t="n">
         <v>5.00942022103225</v>
       </c>
-      <c r="AA17" s="2" t="n">
+      <c r="AI17" s="2" t="n">
         <v>0.517117055651651</v>
       </c>
-      <c r="AB17" s="2" t="n">
+      <c r="AJ17" s="2" t="n">
         <v>0.0175787935517858</v>
       </c>
-      <c r="AC17" s="2" t="n">
+      <c r="AK17" s="2" t="n">
         <v>2.02182923249266</v>
       </c>
-      <c r="AD17" s="2" t="n">
+      <c r="AL17" s="2" t="n">
         <v>469.289999999999</v>
       </c>
-      <c r="AE17" s="3" t="n">
+      <c r="AM17" s="3" t="n">
         <v>19.6</v>
       </c>
     </row>
@@ -26471,30 +26827,51 @@
         <v>43.5</v>
       </c>
       <c r="Y18" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="Z18" s="2" t="n">
+        <v>4.99787427727374</v>
+      </c>
+      <c r="AA18" s="2" t="n">
+        <v>0.5131276650924</v>
+      </c>
+      <c r="AB18" s="2" t="n">
+        <v>0.0176722064977306</v>
+      </c>
+      <c r="AC18" s="2" t="n">
+        <v>2.02140424707388</v>
+      </c>
+      <c r="AD18" s="2" t="n">
+        <v>561.21</v>
+      </c>
+      <c r="AE18" s="3" t="n">
+        <v>32.6</v>
+      </c>
+      <c r="AG18" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="Z18" s="2" t="n">
+      <c r="AH18" s="2" t="n">
         <v>5.11984047261926</v>
       </c>
-      <c r="AA18" s="2" t="n">
+      <c r="AI18" s="2" t="n">
         <v>0.5237416884558</v>
       </c>
-      <c r="AB18" s="2" t="n">
+      <c r="AJ18" s="2" t="n">
         <v>0.0179299563022002</v>
       </c>
-      <c r="AC18" s="2" t="n">
+      <c r="AK18" s="2" t="n">
         <v>2.0223093658777</v>
       </c>
-      <c r="AD18" s="2" t="n">
+      <c r="AL18" s="2" t="n">
         <v>333.76</v>
       </c>
-      <c r="AE18" s="3" t="n">
+      <c r="AM18" s="3" t="n">
         <v>18.8</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B19" s="2" t="n">
         <v>4.73482989807527</v>
@@ -26515,7 +26892,7 @@
         <v>92.769999999999</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="J19" s="2" t="n">
         <v>4.73656998313829</v>
@@ -26536,7 +26913,7 @@
         <v>198.31</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="R19" s="2" t="n">
         <v>6.30863179469164</v>
@@ -26557,24 +26934,45 @@
         <v>51.8</v>
       </c>
       <c r="Y19" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="Z19" s="2" t="n">
+        <v>5.03890360428101</v>
+      </c>
+      <c r="AA19" s="2" t="n">
+        <v>0.519142660340031</v>
+      </c>
+      <c r="AB19" s="2" t="n">
+        <v>0.0178760115639695</v>
+      </c>
+      <c r="AC19" s="2" t="n">
+        <v>2.02190055651252</v>
+      </c>
+      <c r="AD19" s="2" t="n">
+        <v>600.45</v>
+      </c>
+      <c r="AE19" s="3" t="n">
+        <v>39.2</v>
+      </c>
+      <c r="AG19" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="Z19" s="2" t="n">
+      <c r="AH19" s="2" t="n">
         <v>5.16877539087627</v>
       </c>
-      <c r="AA19" s="2" t="n">
+      <c r="AI19" s="2" t="n">
         <v>0.526115886200987</v>
       </c>
-      <c r="AB19" s="2" t="n">
+      <c r="AJ19" s="2" t="n">
         <v>0.0195758104148813</v>
       </c>
-      <c r="AC19" s="2" t="n">
+      <c r="AK19" s="2" t="n">
         <v>2.0214757228493</v>
       </c>
-      <c r="AD19" s="2" t="n">
+      <c r="AL19" s="2" t="n">
         <v>253.65</v>
       </c>
-      <c r="AE19" s="3" t="n">
+      <c r="AM19" s="3" t="n">
         <v>18.7</v>
       </c>
     </row>
@@ -26601,7 +26999,7 @@
         <v>95.540000000001</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="J20" s="2" t="n">
         <v>4.73735478004939</v>
@@ -26643,24 +27041,45 @@
         <v>40.2</v>
       </c>
       <c r="Y20" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z20" s="2" t="n">
+        <v>4.73467225629083</v>
+      </c>
+      <c r="AA20" s="2" t="n">
+        <v>0.487283479183184</v>
+      </c>
+      <c r="AB20" s="2" t="n">
+        <v>0.0118387867765975</v>
+      </c>
+      <c r="AC20" s="2" t="n">
+        <v>2.02281770477151</v>
+      </c>
+      <c r="AD20" s="2" t="n">
+        <v>633.37</v>
+      </c>
+      <c r="AE20" s="3" t="n">
+        <v>32.9</v>
+      </c>
+      <c r="AG20" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="Z20" s="2" t="n">
+      <c r="AH20" s="2" t="n">
         <v>5.22476421829463</v>
       </c>
-      <c r="AA20" s="2" t="n">
+      <c r="AI20" s="2" t="n">
         <v>0.529731302076161</v>
       </c>
-      <c r="AB20" s="2" t="n">
+      <c r="AJ20" s="2" t="n">
         <v>0.0199028781415373</v>
       </c>
-      <c r="AC20" s="2" t="n">
+      <c r="AK20" s="2" t="n">
         <v>2.02173496437402</v>
       </c>
-      <c r="AD20" s="2" t="n">
+      <c r="AL20" s="2" t="n">
         <v>296.9</v>
       </c>
-      <c r="AE20" s="3" t="n">
+      <c r="AM20" s="3" t="n">
         <v>21.9</v>
       </c>
     </row>
@@ -26732,21 +27151,42 @@
         <v>121</v>
       </c>
       <c r="Z21" s="2" t="n">
+        <v>5.02518532294795</v>
+      </c>
+      <c r="AA21" s="2" t="n">
+        <v>0.518468650383405</v>
+      </c>
+      <c r="AB21" s="2" t="n">
+        <v>0.0173766761796799</v>
+      </c>
+      <c r="AC21" s="2" t="n">
+        <v>2.02235178388191</v>
+      </c>
+      <c r="AD21" s="2" t="n">
+        <v>665.65</v>
+      </c>
+      <c r="AE21" s="3" t="n">
+        <v>32.3</v>
+      </c>
+      <c r="AG21" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="AH21" s="2" t="n">
         <v>5.2828873580718</v>
       </c>
-      <c r="AA21" s="2" t="n">
+      <c r="AI21" s="2" t="n">
         <v>0.530037021685518</v>
       </c>
-      <c r="AB21" s="2" t="n">
+      <c r="AJ21" s="2" t="n">
         <v>0.021010595448446</v>
       </c>
-      <c r="AC21" s="2" t="n">
+      <c r="AK21" s="2" t="n">
         <v>2.0205822677958</v>
       </c>
-      <c r="AD21" s="2" t="n">
+      <c r="AL21" s="2" t="n">
         <v>374.030000000001</v>
       </c>
-      <c r="AE21" s="3" t="n">
+      <c r="AM21" s="3" t="n">
         <v>19.3</v>
       </c>
     </row>
@@ -26815,24 +27255,45 @@
         <v>50.7</v>
       </c>
       <c r="Y22" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="Z22" s="2" t="n">
+        <v>4.7884982880119</v>
+      </c>
+      <c r="AA22" s="2" t="n">
+        <v>0.496735106011394</v>
+      </c>
+      <c r="AB22" s="2" t="n">
+        <v>0.0140341747421385</v>
+      </c>
+      <c r="AC22" s="2" t="n">
+        <v>2.02222893465662</v>
+      </c>
+      <c r="AD22" s="2" t="n">
+        <v>698.29</v>
+      </c>
+      <c r="AE22" s="3" t="n">
+        <v>32.6</v>
+      </c>
+      <c r="AG22" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="Z22" s="2" t="n">
+      <c r="AH22" s="2" t="n">
         <v>5.29161793897107</v>
       </c>
-      <c r="AA22" s="2" t="n">
+      <c r="AI22" s="2" t="n">
         <v>0.532915414088237</v>
       </c>
-      <c r="AB22" s="2" t="n">
+      <c r="AJ22" s="2" t="n">
         <v>0.0200434216808821</v>
       </c>
-      <c r="AC22" s="2" t="n">
+      <c r="AK22" s="2" t="n">
         <v>2.02112866865988</v>
       </c>
-      <c r="AD22" s="2" t="n">
+      <c r="AL22" s="2" t="n">
         <v>586.110000000001</v>
       </c>
-      <c r="AE22" s="3" t="n">
+      <c r="AM22" s="3" t="n">
         <v>18.7</v>
       </c>
     </row>
@@ -26880,7 +27341,7 @@
         <v>203.35</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="R23" s="2" t="n">
         <v>7.76741733991397</v>
@@ -26901,30 +27362,51 @@
         <v>48</v>
       </c>
       <c r="Y23" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="Z23" s="2" t="n">
+        <v>5.14275774119359</v>
+      </c>
+      <c r="AA23" s="2" t="n">
+        <v>0.521303097036831</v>
+      </c>
+      <c r="AB23" s="2" t="n">
+        <v>0.0194985340404082</v>
+      </c>
+      <c r="AC23" s="2" t="n">
+        <v>2.02101150622722</v>
+      </c>
+      <c r="AD23" s="2" t="n">
+        <v>728.97</v>
+      </c>
+      <c r="AE23" s="3" t="n">
+        <v>30.7</v>
+      </c>
+      <c r="AG23" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="Z23" s="2" t="n">
+      <c r="AH23" s="2" t="n">
         <v>5.32508805696527</v>
       </c>
-      <c r="AA23" s="2" t="n">
+      <c r="AI23" s="2" t="n">
         <v>0.52391739504947</v>
       </c>
-      <c r="AB23" s="2" t="n">
+      <c r="AJ23" s="2" t="n">
         <v>0.0211143002626029</v>
       </c>
-      <c r="AC23" s="2" t="n">
+      <c r="AK23" s="2" t="n">
         <v>2.02032324216094</v>
       </c>
-      <c r="AD23" s="2" t="n">
+      <c r="AL23" s="2" t="n">
         <v>119.77</v>
       </c>
-      <c r="AE23" s="3" t="n">
+      <c r="AM23" s="3" t="n">
         <v>19.1</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B24" s="2" t="n">
         <v>4.73750625719472</v>
@@ -26945,7 +27427,7 @@
         <v>93.530000000001</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="J24" s="2" t="n">
         <v>4.74029720513826</v>
@@ -26987,24 +27469,45 @@
         <v>49.3</v>
       </c>
       <c r="Y24" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="Z24" s="2" t="n">
+        <v>4.75524645113817</v>
+      </c>
+      <c r="AA24" s="2" t="n">
+        <v>0.493289803166678</v>
+      </c>
+      <c r="AB24" s="2" t="n">
+        <v>0.0129637986805935</v>
+      </c>
+      <c r="AC24" s="2" t="n">
+        <v>2.0225209242189</v>
+      </c>
+      <c r="AD24" s="2" t="n">
+        <v>759.17</v>
+      </c>
+      <c r="AE24" s="3" t="n">
+        <v>30.2</v>
+      </c>
+      <c r="AG24" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="Z24" s="2" t="n">
+      <c r="AH24" s="2" t="n">
         <v>5.53061476143937</v>
       </c>
-      <c r="AA24" s="2" t="n">
+      <c r="AI24" s="2" t="n">
         <v>0.544067303981715</v>
       </c>
-      <c r="AB24" s="2" t="n">
+      <c r="AJ24" s="2" t="n">
         <v>0.0228259975865514</v>
       </c>
-      <c r="AC24" s="2" t="n">
+      <c r="AK24" s="2" t="n">
         <v>2.02110545965087</v>
       </c>
-      <c r="AD24" s="2" t="n">
+      <c r="AL24" s="2" t="n">
         <v>354.780000000001</v>
       </c>
-      <c r="AE24" s="3" t="n">
+      <c r="AM24" s="3" t="n">
         <v>21</v>
       </c>
     </row>
@@ -27052,7 +27555,7 @@
         <v>192.94</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="R25" s="2" t="n">
         <v>10.7344618261651</v>
@@ -27073,24 +27576,45 @@
         <v>49.4</v>
       </c>
       <c r="Y25" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="Z25" s="2" t="n">
+        <v>4.92081349378116</v>
+      </c>
+      <c r="AA25" s="2" t="n">
+        <v>0.497880942417943</v>
+      </c>
+      <c r="AB25" s="2" t="n">
+        <v>0.0153675399086633</v>
+      </c>
+      <c r="AC25" s="2" t="n">
+        <v>2.02181939345828</v>
+      </c>
+      <c r="AD25" s="2" t="n">
+        <v>788.39</v>
+      </c>
+      <c r="AE25" s="3" t="n">
+        <v>29.2</v>
+      </c>
+      <c r="AG25" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="Z25" s="2" t="n">
+      <c r="AH25" s="2" t="n">
         <v>5.54636459222882</v>
       </c>
-      <c r="AA25" s="2" t="n">
+      <c r="AI25" s="2" t="n">
         <v>0.450301525598511</v>
       </c>
-      <c r="AB25" s="2" t="n">
+      <c r="AJ25" s="2" t="n">
         <v>0.00439832399308458</v>
       </c>
-      <c r="AC25" s="2" t="n">
+      <c r="AK25" s="2" t="n">
         <v>2.02623292995681</v>
       </c>
-      <c r="AD25" s="2" t="n">
+      <c r="AL25" s="2" t="n">
         <v>548.75</v>
       </c>
-      <c r="AE25" s="3" t="n">
+      <c r="AM25" s="3" t="n">
         <v>18.8</v>
       </c>
     </row>
@@ -27138,7 +27662,7 @@
         <v>185.79</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="R26" s="2" t="n">
         <v>11.5474903969739</v>
@@ -27159,24 +27683,45 @@
         <v>51.4</v>
       </c>
       <c r="Y26" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="Z26" s="2" t="n">
+        <v>4.76085733480188</v>
+      </c>
+      <c r="AA26" s="2" t="n">
+        <v>0.493259844879015</v>
+      </c>
+      <c r="AB26" s="2" t="n">
+        <v>0.0132383944115297</v>
+      </c>
+      <c r="AC26" s="2" t="n">
+        <v>2.02239652084699</v>
+      </c>
+      <c r="AD26" s="2" t="n">
+        <v>817.88</v>
+      </c>
+      <c r="AE26" s="3" t="n">
+        <v>29.5</v>
+      </c>
+      <c r="AG26" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="Z26" s="2" t="n">
+      <c r="AH26" s="2" t="n">
         <v>5.68621616072169</v>
       </c>
-      <c r="AA26" s="2" t="n">
+      <c r="AI26" s="2" t="n">
         <v>0.550729116328858</v>
       </c>
-      <c r="AB26" s="2" t="n">
+      <c r="AJ26" s="2" t="n">
         <v>0.0241401540325002</v>
       </c>
-      <c r="AC26" s="2" t="n">
+      <c r="AK26" s="2" t="n">
         <v>2.02111164912474</v>
       </c>
-      <c r="AD26" s="2" t="n">
+      <c r="AL26" s="2" t="n">
         <v>195.99</v>
       </c>
-      <c r="AE26" s="3" t="n">
+      <c r="AM26" s="3" t="n">
         <v>18.8</v>
       </c>
     </row>
@@ -27245,24 +27790,45 @@
         <v>50.5</v>
       </c>
       <c r="Y27" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="Z27" s="2" t="n">
+        <v>4.73515617351864</v>
+      </c>
+      <c r="AA27" s="2" t="n">
+        <v>0.487284831388892</v>
+      </c>
+      <c r="AB27" s="2" t="n">
+        <v>0.0117523328256463</v>
+      </c>
+      <c r="AC27" s="2" t="n">
+        <v>2.02292759078908</v>
+      </c>
+      <c r="AD27" s="2" t="n">
+        <v>847.17</v>
+      </c>
+      <c r="AE27" s="3" t="n">
+        <v>29.3</v>
+      </c>
+      <c r="AG27" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="Z27" s="2" t="n">
+      <c r="AH27" s="2" t="n">
         <v>5.6917015780514</v>
       </c>
-      <c r="AA27" s="2" t="n">
+      <c r="AI27" s="2" t="n">
         <v>0.551282825258859</v>
       </c>
-      <c r="AB27" s="2" t="n">
+      <c r="AJ27" s="2" t="n">
         <v>0.0238474547305066</v>
       </c>
-      <c r="AC27" s="2" t="n">
+      <c r="AK27" s="2" t="n">
         <v>2.02155054029698</v>
       </c>
-      <c r="AD27" s="2" t="n">
+      <c r="AL27" s="2" t="n">
         <v>412.27</v>
       </c>
-      <c r="AE27" s="3" t="n">
+      <c r="AM27" s="3" t="n">
         <v>18.8</v>
       </c>
     </row>
@@ -27331,30 +27897,51 @@
         <v>42.4</v>
       </c>
       <c r="Y28" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="Z28" s="2" t="n">
+        <v>4.98440894751909</v>
+      </c>
+      <c r="AA28" s="2" t="n">
+        <v>0.514156057484994</v>
+      </c>
+      <c r="AB28" s="2" t="n">
+        <v>0.0174806679088208</v>
+      </c>
+      <c r="AC28" s="2" t="n">
+        <v>2.0216683339422</v>
+      </c>
+      <c r="AD28" s="2" t="n">
+        <v>879.54</v>
+      </c>
+      <c r="AE28" s="3" t="n">
+        <v>32.4</v>
+      </c>
+      <c r="AG28" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="Z28" s="2" t="n">
+      <c r="AH28" s="2" t="n">
         <v>5.79493054981968</v>
       </c>
-      <c r="AA28" s="2" t="n">
+      <c r="AI28" s="2" t="n">
         <v>0.552679315673452</v>
       </c>
-      <c r="AB28" s="2" t="n">
+      <c r="AJ28" s="2" t="n">
         <v>0.0257898341104866</v>
       </c>
-      <c r="AC28" s="2" t="n">
+      <c r="AK28" s="2" t="n">
         <v>2.02039586868464</v>
       </c>
-      <c r="AD28" s="2" t="n">
+      <c r="AL28" s="2" t="n">
         <v>449.73</v>
       </c>
-      <c r="AE28" s="3" t="n">
+      <c r="AM28" s="3" t="n">
         <v>18.9</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="B29" s="2" t="n">
         <v>4.74131495839404</v>
@@ -27375,7 +27962,7 @@
         <v>99.35</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="J29" s="2" t="n">
         <v>4.79325080296581</v>
@@ -27417,30 +28004,51 @@
         <v>49.9</v>
       </c>
       <c r="Y29" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="Z29" s="2" t="n">
+        <v>4.90207479313799</v>
+      </c>
+      <c r="AA29" s="2" t="n">
+        <v>0.505927223899367</v>
+      </c>
+      <c r="AB29" s="2" t="n">
+        <v>0.0162108016602863</v>
+      </c>
+      <c r="AC29" s="2" t="n">
+        <v>2.02164991059931</v>
+      </c>
+      <c r="AD29" s="2" t="n">
+        <v>910.83</v>
+      </c>
+      <c r="AE29" s="3" t="n">
+        <v>31.3</v>
+      </c>
+      <c r="AG29" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="Z29" s="2" t="n">
+      <c r="AH29" s="2" t="n">
         <v>5.81314261535196</v>
       </c>
-      <c r="AA29" s="2" t="n">
+      <c r="AI29" s="2" t="n">
         <v>0.552438666640035</v>
       </c>
-      <c r="AB29" s="2" t="n">
+      <c r="AJ29" s="2" t="n">
         <v>0.0260364439741952</v>
       </c>
-      <c r="AC29" s="2" t="n">
+      <c r="AK29" s="2" t="n">
         <v>2.02006521694369</v>
       </c>
-      <c r="AD29" s="2" t="n">
+      <c r="AL29" s="2" t="n">
         <v>314.98</v>
       </c>
-      <c r="AE29" s="3" t="n">
+      <c r="AM29" s="3" t="n">
         <v>18.1</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="B30" s="2" t="n">
         <v>4.74341171169469</v>
@@ -27482,7 +28090,7 @@
         <v>201.1</v>
       </c>
       <c r="Q30" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="R30" s="2" t="n">
         <v>14.5297619190541</v>
@@ -27503,24 +28111,45 @@
         <v>54.5</v>
       </c>
       <c r="Y30" s="1" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="Z30" s="2" t="n">
+        <v>4.82575210138327</v>
+      </c>
+      <c r="AA30" s="2" t="n">
+        <v>0.497221043515114</v>
+      </c>
+      <c r="AB30" s="2" t="n">
+        <v>0.0145796499998766</v>
+      </c>
+      <c r="AC30" s="2" t="n">
+        <v>2.02182628376977</v>
+      </c>
+      <c r="AD30" s="2" t="n">
+        <v>942.62</v>
+      </c>
+      <c r="AE30" s="3" t="n">
+        <v>31.8</v>
+      </c>
+      <c r="AG30" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="AH30" s="2" t="n">
         <v>6.60147190401879</v>
       </c>
-      <c r="AA30" s="2" t="n">
+      <c r="AI30" s="2" t="n">
         <v>0.581859590187604</v>
       </c>
-      <c r="AB30" s="2" t="n">
+      <c r="AJ30" s="2" t="n">
         <v>0.0322061123393598</v>
       </c>
-      <c r="AC30" s="2" t="n">
+      <c r="AK30" s="2" t="n">
         <v>2.01971131920745</v>
       </c>
-      <c r="AD30" s="2" t="n">
+      <c r="AL30" s="2" t="n">
         <v>100.67</v>
       </c>
-      <c r="AE30" s="3" t="n">
+      <c r="AM30" s="3" t="n">
         <v>19.3</v>
       </c>
     </row>
@@ -27589,24 +28218,45 @@
         <v>54.7</v>
       </c>
       <c r="Y31" s="1" t="s">
-        <v>151</v>
+        <v>131</v>
       </c>
       <c r="Z31" s="2" t="n">
+        <v>4.77896907876279</v>
+      </c>
+      <c r="AA31" s="2" t="n">
+        <v>0.474691738545627</v>
+      </c>
+      <c r="AB31" s="2" t="n">
+        <v>0.00929683638159426</v>
+      </c>
+      <c r="AC31" s="2" t="n">
+        <v>2.02351299903581</v>
+      </c>
+      <c r="AD31" s="2" t="n">
+        <v>976.52</v>
+      </c>
+      <c r="AE31" s="3" t="n">
+        <v>33.9</v>
+      </c>
+      <c r="AG31" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="AH31" s="2" t="n">
         <v>6.69584862019204</v>
       </c>
-      <c r="AA31" s="2" t="n">
+      <c r="AI31" s="2" t="n">
         <v>0.573781261508616</v>
       </c>
-      <c r="AB31" s="2" t="n">
+      <c r="AJ31" s="2" t="n">
         <v>0.0333309402681</v>
       </c>
-      <c r="AC31" s="2" t="n">
+      <c r="AK31" s="2" t="n">
         <v>2.01851960457967</v>
       </c>
-      <c r="AD31" s="2" t="n">
+      <c r="AL31" s="2" t="n">
         <v>22.7600000000002</v>
       </c>
-      <c r="AE31" s="3" t="n">
+      <c r="AM31" s="3" t="n">
         <v>22.8</v>
       </c>
     </row>
@@ -27633,7 +28283,7 @@
         <v>99.1700000000001</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="J32" s="2" t="n">
         <v>4.84794027256065</v>
@@ -27675,141 +28325,349 @@
         <v>49.5</v>
       </c>
       <c r="Y32" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="Z32" s="2" t="n">
+        <v>4.78242373061582</v>
+      </c>
+      <c r="AA32" s="2" t="n">
+        <v>0.496450511192072</v>
+      </c>
+      <c r="AB32" s="2" t="n">
+        <v>0.0138941541608426</v>
+      </c>
+      <c r="AC32" s="2" t="n">
+        <v>2.02225552637242</v>
+      </c>
+      <c r="AD32" s="2" t="n">
+        <v>1009.78</v>
+      </c>
+      <c r="AE32" s="3" t="n">
+        <v>33.3</v>
+      </c>
+      <c r="AG32" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="Z32" s="2" t="n">
+      <c r="AH32" s="2" t="n">
         <v>8.71009886078587</v>
       </c>
-      <c r="AA32" s="2" t="n">
+      <c r="AI32" s="2" t="n">
         <v>0.628011529441782</v>
       </c>
-      <c r="AB32" s="2" t="n">
+      <c r="AJ32" s="2" t="n">
         <v>0.0485381822999904</v>
       </c>
-      <c r="AC32" s="2" t="n">
+      <c r="AK32" s="2" t="n">
         <v>2.01471658138896</v>
       </c>
-      <c r="AD32" s="2" t="n">
+      <c r="AL32" s="2" t="n">
         <v>567.440000000001</v>
       </c>
-      <c r="AE32" s="3" t="n">
+      <c r="AM32" s="3" t="n">
         <v>18.7</v>
       </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AM33" s="3"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B34" s="0" t="n">
         <f aca="false">MIN(B3:B32)</f>
         <v>4.73248753274178</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="G34" s="3" t="n">
         <f aca="false">MIN(G3:G32)</f>
         <v>92.51</v>
       </c>
       <c r="I34" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="J34" s="0" t="n">
         <f aca="false">MIN(J3:J32)</f>
         <v>4.73241918756398</v>
       </c>
       <c r="N34" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="O34" s="3" t="n">
         <f aca="false">MIN(O3:O32)</f>
         <v>184.45</v>
       </c>
       <c r="Q34" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="R34" s="0" t="n">
         <f aca="false">MIN(R3:R32)</f>
         <v>4.7331248630718</v>
       </c>
       <c r="V34" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="W34" s="3" t="n">
         <f aca="false">MIN(W3:W32)</f>
         <v>38.3</v>
       </c>
       <c r="Y34" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="Z34" s="0" t="n">
         <f aca="false">MIN(Z3:Z32)</f>
-        <v>4.73365937265043</v>
+        <v>4.73266263880405</v>
       </c>
       <c r="AD34" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="AE34" s="3" t="n">
         <f aca="false">MIN(AE3:AE32)</f>
+        <v>29.2</v>
+      </c>
+      <c r="AG34" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="AH34" s="0" t="n">
+        <f aca="false">MIN(AH3:AH32)</f>
+        <v>4.73365937265043</v>
+      </c>
+      <c r="AL34" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="AM34" s="3" t="n">
+        <f aca="false">MIN(AM3:AM32)</f>
         <v>18.1</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B35" s="0" t="n">
         <f aca="false">AVERAGE(B3:B32)</f>
         <v>4.73756836745389</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="G35" s="3" t="n">
         <f aca="false">AVERAGE(G3:G32)</f>
         <v>98.084</v>
       </c>
       <c r="I35" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="J35" s="0" t="n">
         <f aca="false">AVERAGE(J3:J32)</f>
         <v>4.74954683785947</v>
       </c>
       <c r="N35" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="O35" s="3" t="n">
         <f aca="false">AVERAGE(O3:O32)</f>
         <v>193.975</v>
       </c>
       <c r="Q35" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="R35" s="0" t="n">
         <f aca="false">AVERAGE(R3:R32)</f>
         <v>7.80846874577006</v>
       </c>
       <c r="V35" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="W35" s="3" t="n">
         <f aca="false">AVERAGE(W3:W32)</f>
         <v>47.96</v>
       </c>
       <c r="Y35" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="Z35" s="0" t="n">
         <f aca="false">AVERAGE(Z3:Z32)</f>
-        <v>5.3321773375202</v>
+        <v>5.14742963212637</v>
       </c>
       <c r="AD35" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="AE35" s="3" t="n">
         <f aca="false">AVERAGE(AE3:AE32)</f>
+        <v>33.6633333333333</v>
+      </c>
+      <c r="AG35" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="AH35" s="0" t="n">
+        <f aca="false">AVERAGE(AH3:AH32)</f>
+        <v>5.3321773375202</v>
+      </c>
+      <c r="AL35" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="AM35" s="3" t="n">
+        <f aca="false">AVERAGE(AM3:AM32)</f>
         <v>19.5433333333333</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J47" s="0" t="n">
+        <v>4.86356438852961</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J48" s="0" t="n">
+        <v>7.28021806479377</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J49" s="0" t="n">
+        <v>4.7524336666441</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J50" s="0" t="n">
+        <v>5.48662926647256</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J51" s="0" t="n">
+        <v>5.09305097312991</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J52" s="0" t="n">
+        <v>9.35380705222917</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J53" s="0" t="n">
+        <v>4.74324957927919</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J54" s="0" t="n">
+        <v>4.73266263880405</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J55" s="0" t="n">
+        <v>4.74661936612423</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J56" s="0" t="n">
+        <v>4.73469303823187</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J57" s="0" t="n">
+        <v>4.76529694877274</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J58" s="0" t="n">
+        <v>5.04995954226894</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J59" s="0" t="n">
+        <v>4.86539203629354</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J60" s="0" t="n">
+        <v>5.6660097928394</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J61" s="0" t="n">
+        <v>5.11570901472011</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J62" s="0" t="n">
+        <v>4.99787427727374</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J63" s="0" t="n">
+        <v>5.03890360428101</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J64" s="0" t="n">
+        <v>4.73467225629083</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J65" s="0" t="n">
+        <v>5.02518532294795</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J66" s="0" t="n">
+        <v>4.7884982880119</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J67" s="0" t="n">
+        <v>5.14275774119359</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J68" s="0" t="n">
+        <v>4.75524645113817</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J69" s="0" t="n">
+        <v>4.92081349378116</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J70" s="0" t="n">
+        <v>4.76085733480188</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J71" s="0" t="n">
+        <v>4.73515617351864</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J72" s="0" t="n">
+        <v>4.98440894751909</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J73" s="0" t="n">
+        <v>4.90207479313799</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J74" s="0" t="n">
+        <v>4.82575210138327</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J75" s="0" t="n">
+        <v>4.77896907876279</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J76" s="0" t="n">
+        <v>4.78242373061582</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J78" s="0" t="n">
+        <f aca="false">AVERAGE(J47:J76)</f>
+        <v>5.14742963212637</v>
       </c>
     </row>
   </sheetData>
@@ -27834,7 +28692,7 @@
       <selection pane="topLeft" activeCell="M15" activeCellId="0" sqref="M15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="6.18359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -27876,10 +28734,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="2" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29044,7 +29902,7 @@
       <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="6.71"/>
   </cols>
@@ -29738,7 +30596,7 @@
       <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="7.98"/>
   </cols>

</xml_diff>

<commit_message>
add min and average J + parameters and time for each of 4 algorithms
</commit_message>
<xml_diff>
--- a/results_from_all_algos.xlsx
+++ b/results_from_all_algos.xlsx
@@ -5,14 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="WOA_CONV" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="WOA_RESULTS" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="GA" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="SA" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="CSA" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="WOA_CONV" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="WOA_RESULTS" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="GA" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="SA" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="CSA" sheetId="5" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="162">
   <si>
     <t xml:space="preserve">ITER#</t>
   </si>
@@ -508,6 +508,9 @@
   <si>
     <t xml:space="preserve">Population 400</t>
   </si>
+  <si>
+    <t xml:space="preserve">PARs</t>
+  </si>
 </sst>
 </file>
 
@@ -517,7 +520,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -545,6 +548,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -589,7 +597,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -602,11 +610,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -619,31 +631,128 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:CW132"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="Y2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="Y1" activeCellId="0" sqref="Y1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B102" activeCellId="0" sqref="B102"/>
+      <selection pane="bottomRight" activeCell="B102" activeCellId="1" sqref="B37 B102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.8125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -24994,29 +25103,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AM78"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="N1" activeCellId="0" sqref="N1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T14" activeCellId="0" sqref="T14"/>
+      <selection pane="bottomRight" activeCell="Q34" activeCellId="1" sqref="B37 Q34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="10.42"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="6.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="9.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="8.37"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="15" min="15" style="3" width="6.54"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="23" min="23" style="3" width="6.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="7.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="2" width="7.34"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="31" min="31" style="3" width="6.54"/>
   </cols>
   <sheetData>
@@ -28371,70 +28480,70 @@
       <c r="AM33" s="3"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="A34" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="B34" s="0" t="n">
+      <c r="B34" s="2" t="n">
         <f aca="false">MIN(B3:B32)</f>
         <v>4.73248753274178</v>
       </c>
-      <c r="F34" s="0" t="s">
+      <c r="F34" s="2" t="s">
         <v>157</v>
       </c>
       <c r="G34" s="3" t="n">
         <f aca="false">MIN(G3:G32)</f>
         <v>92.51</v>
       </c>
-      <c r="I34" s="0" t="s">
+      <c r="I34" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="J34" s="0" t="n">
+      <c r="J34" s="2" t="n">
         <f aca="false">MIN(J3:J32)</f>
         <v>4.73241918756398</v>
       </c>
-      <c r="N34" s="0" t="s">
+      <c r="N34" s="2" t="s">
         <v>157</v>
       </c>
       <c r="O34" s="3" t="n">
         <f aca="false">MIN(O3:O32)</f>
         <v>184.45</v>
       </c>
-      <c r="Q34" s="0" t="s">
+      <c r="Q34" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="R34" s="0" t="n">
+      <c r="R34" s="2" t="n">
         <f aca="false">MIN(R3:R32)</f>
         <v>4.7331248630718</v>
       </c>
-      <c r="V34" s="0" t="s">
+      <c r="V34" s="2" t="s">
         <v>157</v>
       </c>
       <c r="W34" s="3" t="n">
         <f aca="false">MIN(W3:W32)</f>
         <v>38.3</v>
       </c>
-      <c r="Y34" s="0" t="s">
+      <c r="Y34" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="Z34" s="0" t="n">
+      <c r="Z34" s="2" t="n">
         <f aca="false">MIN(Z3:Z32)</f>
         <v>4.73266263880405</v>
       </c>
-      <c r="AD34" s="0" t="s">
+      <c r="AD34" s="2" t="s">
         <v>157</v>
       </c>
       <c r="AE34" s="3" t="n">
         <f aca="false">MIN(AE3:AE32)</f>
         <v>29.2</v>
       </c>
-      <c r="AG34" s="0" t="s">
+      <c r="AG34" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="AH34" s="0" t="n">
+      <c r="AH34" s="2" t="n">
         <f aca="false">MIN(AH3:AH32)</f>
         <v>4.73365937265043</v>
       </c>
-      <c r="AL34" s="0" t="s">
+      <c r="AL34" s="2" t="s">
         <v>157</v>
       </c>
       <c r="AM34" s="3" t="n">
@@ -28443,70 +28552,70 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+      <c r="A35" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="B35" s="0" t="n">
+      <c r="B35" s="2" t="n">
         <f aca="false">AVERAGE(B3:B32)</f>
         <v>4.73756836745389</v>
       </c>
-      <c r="F35" s="0" t="s">
+      <c r="F35" s="2" t="s">
         <v>158</v>
       </c>
       <c r="G35" s="3" t="n">
         <f aca="false">AVERAGE(G3:G32)</f>
         <v>98.084</v>
       </c>
-      <c r="I35" s="0" t="s">
+      <c r="I35" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="J35" s="0" t="n">
+      <c r="J35" s="2" t="n">
         <f aca="false">AVERAGE(J3:J32)</f>
         <v>4.74954683785947</v>
       </c>
-      <c r="N35" s="0" t="s">
+      <c r="N35" s="2" t="s">
         <v>158</v>
       </c>
       <c r="O35" s="3" t="n">
         <f aca="false">AVERAGE(O3:O32)</f>
         <v>193.975</v>
       </c>
-      <c r="Q35" s="0" t="s">
+      <c r="Q35" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="R35" s="0" t="n">
+      <c r="R35" s="2" t="n">
         <f aca="false">AVERAGE(R3:R32)</f>
         <v>7.80846874577006</v>
       </c>
-      <c r="V35" s="0" t="s">
+      <c r="V35" s="2" t="s">
         <v>158</v>
       </c>
       <c r="W35" s="3" t="n">
         <f aca="false">AVERAGE(W3:W32)</f>
         <v>47.96</v>
       </c>
-      <c r="Y35" s="0" t="s">
+      <c r="Y35" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="Z35" s="0" t="n">
+      <c r="Z35" s="2" t="n">
         <f aca="false">AVERAGE(Z3:Z32)</f>
         <v>5.14742963212637</v>
       </c>
-      <c r="AD35" s="0" t="s">
+      <c r="AD35" s="2" t="s">
         <v>158</v>
       </c>
       <c r="AE35" s="3" t="n">
         <f aca="false">AVERAGE(AE3:AE32)</f>
         <v>33.6633333333333</v>
       </c>
-      <c r="AG35" s="0" t="s">
+      <c r="AG35" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="AH35" s="0" t="n">
+      <c r="AH35" s="2" t="n">
         <f aca="false">AVERAGE(AH3:AH32)</f>
         <v>5.3321773375202</v>
       </c>
-      <c r="AL35" s="0" t="s">
+      <c r="AL35" s="2" t="s">
         <v>158</v>
       </c>
       <c r="AM35" s="3" t="n">
@@ -28515,157 +28624,157 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J47" s="0" t="n">
+      <c r="J47" s="2" t="n">
         <v>4.86356438852961</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J48" s="0" t="n">
+      <c r="J48" s="2" t="n">
         <v>7.28021806479377</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J49" s="0" t="n">
+      <c r="J49" s="2" t="n">
         <v>4.7524336666441</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J50" s="0" t="n">
+      <c r="J50" s="2" t="n">
         <v>5.48662926647256</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J51" s="0" t="n">
+      <c r="J51" s="2" t="n">
         <v>5.09305097312991</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J52" s="0" t="n">
+      <c r="J52" s="2" t="n">
         <v>9.35380705222917</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J53" s="0" t="n">
+      <c r="J53" s="2" t="n">
         <v>4.74324957927919</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J54" s="0" t="n">
+      <c r="J54" s="2" t="n">
         <v>4.73266263880405</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J55" s="0" t="n">
+      <c r="J55" s="2" t="n">
         <v>4.74661936612423</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J56" s="0" t="n">
+      <c r="J56" s="2" t="n">
         <v>4.73469303823187</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J57" s="0" t="n">
+      <c r="J57" s="2" t="n">
         <v>4.76529694877274</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J58" s="0" t="n">
+      <c r="J58" s="2" t="n">
         <v>5.04995954226894</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J59" s="0" t="n">
+      <c r="J59" s="2" t="n">
         <v>4.86539203629354</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J60" s="0" t="n">
+      <c r="J60" s="2" t="n">
         <v>5.6660097928394</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J61" s="0" t="n">
+      <c r="J61" s="2" t="n">
         <v>5.11570901472011</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J62" s="0" t="n">
+      <c r="J62" s="2" t="n">
         <v>4.99787427727374</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J63" s="0" t="n">
+      <c r="J63" s="2" t="n">
         <v>5.03890360428101</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J64" s="0" t="n">
+      <c r="J64" s="2" t="n">
         <v>4.73467225629083</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J65" s="0" t="n">
+      <c r="J65" s="2" t="n">
         <v>5.02518532294795</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J66" s="0" t="n">
+      <c r="J66" s="2" t="n">
         <v>4.7884982880119</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J67" s="0" t="n">
+      <c r="J67" s="2" t="n">
         <v>5.14275774119359</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J68" s="0" t="n">
+      <c r="J68" s="2" t="n">
         <v>4.75524645113817</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J69" s="0" t="n">
+      <c r="J69" s="2" t="n">
         <v>4.92081349378116</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J70" s="0" t="n">
+      <c r="J70" s="2" t="n">
         <v>4.76085733480188</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J71" s="0" t="n">
+      <c r="J71" s="2" t="n">
         <v>4.73515617351864</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J72" s="0" t="n">
+      <c r="J72" s="2" t="n">
         <v>4.98440894751909</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J73" s="0" t="n">
+      <c r="J73" s="2" t="n">
         <v>4.90207479313799</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J74" s="0" t="n">
+      <c r="J74" s="2" t="n">
         <v>4.82575210138327</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J75" s="0" t="n">
+      <c r="J75" s="2" t="n">
         <v>4.77896907876279</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J76" s="0" t="n">
+      <c r="J76" s="2" t="n">
         <v>4.78242373061582</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J78" s="0" t="n">
+      <c r="J78" s="2" t="n">
         <f aca="false">AVERAGE(J47:J76)</f>
         <v>5.14742963212637</v>
       </c>
@@ -28682,14 +28791,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M32"/>
+  <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M15" activeCellId="0" sqref="M15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I37" activeCellId="1" sqref="B37 I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.18359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -29878,6 +29987,78 @@
       </c>
       <c r="M32" s="2" t="n">
         <v>24</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B34" s="2" t="n">
+        <f aca="false">MIN(B3:B32)</f>
+        <v>4.80704998386385</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="I34" s="2" t="n">
+        <f aca="false">MIN(I3:I32)</f>
+        <v>4.74913733488581</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B35" s="2" t="n">
+        <f aca="false">AVERAGE(B3:B32)</f>
+        <v>7.64842455812787</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="I35" s="2" t="n">
+        <f aca="false">AVERAGE(I3:I32)</f>
+        <v>5.4623896955627</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="B36" s="2" t="n">
+        <v>0.478124883770832</v>
+      </c>
+      <c r="C36" s="2" t="n">
+        <v>0.0106567264144196</v>
+      </c>
+      <c r="D36" s="2" t="n">
+        <v>2.0197863767494</v>
+      </c>
+      <c r="H36" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="I36" s="2" t="n">
+        <v>0.481101494885917</v>
+      </c>
+      <c r="J36" s="2" t="n">
+        <v>0.0109079590873328</v>
+      </c>
+      <c r="K36" s="2" t="n">
+        <v>2.02147199771118</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="B37" s="2" t="n">
+        <v>7.86000000000058</v>
+      </c>
+      <c r="H37" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="I37" s="2" t="n">
+        <v>27.1899999999987</v>
       </c>
     </row>
   </sheetData>
@@ -29892,14 +30073,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AC32"/>
+  <dimension ref="A1:AC37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A23" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B37" activeCellId="0" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -30572,6 +30753,46 @@
       </c>
       <c r="F32" s="2" t="n">
         <v>549.419999999998</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B34" s="2" t="n">
+        <f aca="false">MIN(B3:B32)</f>
+        <v>6.13686366876309</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B35" s="2" t="n">
+        <f aca="false">AVERAGE(B3:B32)</f>
+        <v>7.58154457514752</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B36" s="2" t="n">
+        <v>0.488253836088191</v>
+      </c>
+      <c r="C36" s="2" t="n">
+        <v>0.0189523996697701</v>
+      </c>
+      <c r="D36" s="2" t="n">
+        <v>2.01361917597072</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B37" s="5" t="n">
+        <v>336.56</v>
       </c>
     </row>
   </sheetData>
@@ -30586,19 +30807,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B37" activeCellId="0" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="7.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.33"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31222,6 +31444,46 @@
       </c>
       <c r="F32" s="2" t="n">
         <v>653.669999999998</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B34" s="2" t="n">
+        <f aca="false">MIN(B3:B32)</f>
+        <v>4.63995154977365</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B35" s="2" t="n">
+        <f aca="false">AVERAGE(B3:B32)</f>
+        <v>4.63995154991595</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B36" s="2" t="n">
+        <v>0.483924848808133</v>
+      </c>
+      <c r="C36" s="2" t="n">
+        <v>0.0112093156744636</v>
+      </c>
+      <c r="D36" s="2" t="n">
+        <v>2.02473089959601</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B37" s="2" t="n">
+        <v>204.52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add the sheet with the compare table
</commit_message>
<xml_diff>
--- a/results_from_all_algos.xlsx
+++ b/results_from_all_algos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="WOA_CONV" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,6 +14,7 @@
     <sheet name="SA" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="CSA" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="ICrA" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="compare GA, SA, CSA, WOA" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="175">
   <si>
     <t xml:space="preserve">ITER#</t>
   </si>
@@ -536,6 +537,21 @@
   <si>
     <t xml:space="preserve">ν-table</t>
   </si>
+  <si>
+    <t xml:space="preserve">J avg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J best</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Par 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Par 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Par 3</t>
+  </si>
 </sst>
 </file>
 
@@ -550,6 +566,7 @@
       <sz val="10"/>
       <name val="Noto Sans JP"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -571,6 +588,7 @@
       <sz val="10"/>
       <name val="Noto Sans JP"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -628,7 +646,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -641,7 +659,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -658,6 +676,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -685,10 +711,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="Y1" activeCellId="0" sqref="Y1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B102" activeCellId="0" sqref="B102"/>
+      <selection pane="bottomRight" activeCell="B102" activeCellId="1" sqref="A1:F5 B102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.28125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="7.28515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.25"/>
   </cols>
@@ -25047,14 +25073,14 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="N1" activeCellId="0" sqref="N1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q34" activeCellId="0" sqref="Q34"/>
+      <selection pane="bottomRight" activeCell="Q34" activeCellId="1" sqref="A1:F5 Q34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="11.16"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="4" width="7.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="10.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="10.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="3" width="8.96"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="15" min="15" style="4" width="7.01"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="23" min="23" style="4" width="7.01"/>
@@ -28731,10 +28757,10 @@
   <dimension ref="A1:M37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I37" activeCellId="0" sqref="I37"/>
+      <selection pane="topLeft" activeCell="I37" activeCellId="1" sqref="A1:F5 I37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="6.6171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -30013,10 +30039,10 @@
   <dimension ref="A1:AC37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A23" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B37" activeCellId="0" sqref="B37"/>
+      <selection pane="topLeft" activeCell="B37" activeCellId="1" sqref="A1:F5 B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.40625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.40234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="7.19"/>
   </cols>
@@ -30747,10 +30773,10 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B37" activeCellId="0" sqref="B37"/>
+      <selection pane="topLeft" activeCell="B37" activeCellId="1" sqref="A1:F5 B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.40625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.40234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="8.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="6" width="17.49"/>
@@ -31437,11 +31463,11 @@
   </sheetPr>
   <dimension ref="A1:W45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H38" activeCellId="0" sqref="H38"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H38" activeCellId="1" sqref="A1:F5 H38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.3125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.31640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
@@ -34030,6 +34056,127 @@
       </c>
       <c r="W45" s="0" t="n">
         <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.08203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>7.64842455812787</v>
+      </c>
+      <c r="C2" s="9" t="n">
+        <v>4.80704998386385</v>
+      </c>
+      <c r="D2" s="9" t="n">
+        <v>0.478124883770832</v>
+      </c>
+      <c r="E2" s="9" t="n">
+        <v>0.0106567264144196</v>
+      </c>
+      <c r="F2" s="9" t="n">
+        <v>2.0197863767494</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>7.58154457514752</v>
+      </c>
+      <c r="C3" s="9" t="n">
+        <v>6.13686366876309</v>
+      </c>
+      <c r="D3" s="9" t="n">
+        <v>0.488253836088191</v>
+      </c>
+      <c r="E3" s="9" t="n">
+        <v>0.0189523996697701</v>
+      </c>
+      <c r="F3" s="9" t="n">
+        <v>2.01361917597072</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>4.63995154991595</v>
+      </c>
+      <c r="C4" s="9" t="n">
+        <v>4.63995154977365</v>
+      </c>
+      <c r="D4" s="9" t="n">
+        <v>0.483924848808133</v>
+      </c>
+      <c r="E4" s="9" t="n">
+        <v>0.0112093156744636</v>
+      </c>
+      <c r="F4" s="9" t="n">
+        <v>2.02473089959601</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>5.14742963212637</v>
+      </c>
+      <c r="C5" s="9" t="n">
+        <v>4.73266263880405</v>
+      </c>
+      <c r="D5" s="9" t="n">
+        <v>0.484997268353348</v>
+      </c>
+      <c r="E5" s="9" t="n">
+        <v>0.0114389330008822</v>
+      </c>
+      <c r="F5" s="9" t="n">
+        <v>2.02287735189339</v>
       </c>
     </row>
   </sheetData>

</xml_diff>